<commit_message>
data entry for 1/12/16 general details batch 2
</commit_message>
<xml_diff>
--- a/data/ldeli_integrate.xlsx
+++ b/data/ldeli_integrate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="137">
   <si>
     <t>date</t>
   </si>
@@ -437,10 +437,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ am/pm"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -527,11 +526,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="128">
+  <cellStyleXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -683,7 +696,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -714,14 +727,14 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="128">
+  <cellStyles count="142">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -787,6 +800,13 @@
     <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -849,6 +869,13 @@
     <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1178,11 +1205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB212"/>
+  <dimension ref="A1:AB254"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P200" sqref="P200:P212"/>
+      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N215" sqref="N215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -7778,7 +7805,7 @@
         <v>0.39930555555555558</v>
       </c>
       <c r="P129" s="2">
-        <f t="shared" ref="P128:P169" si="2">O129*1440-N129*1440</f>
+        <f t="shared" ref="P129:P163" si="2">O129*1440-N129*1440</f>
         <v>89.999999999999943</v>
       </c>
     </row>
@@ -9563,7 +9590,7 @@
         <v>0.55763888888888891</v>
       </c>
       <c r="P164" s="2">
-        <f>O165*1440-N164*1440</f>
+        <f t="shared" ref="P164:P169" si="3">O165*1440-N164*1440</f>
         <v>92</v>
       </c>
     </row>
@@ -9614,7 +9641,7 @@
         <v>0.55902777777777779</v>
       </c>
       <c r="P165" s="2">
-        <f>O166*1440-N165*1440</f>
+        <f t="shared" si="3"/>
         <v>92.000000000000114</v>
       </c>
     </row>
@@ -9665,7 +9692,7 @@
         <v>0.56041666666666667</v>
       </c>
       <c r="P166" s="2">
-        <f>O167*1440-N166*1440</f>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
     </row>
@@ -9716,7 +9743,7 @@
         <v>0.56111111111111112</v>
       </c>
       <c r="P167" s="2">
-        <f>O168*1440-N167*1440</f>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
     </row>
@@ -9767,7 +9794,7 @@
         <v>0.56180555555555556</v>
       </c>
       <c r="P168" s="2">
-        <f>O169*1440-N168*1440</f>
+        <f t="shared" si="3"/>
         <v>93.000000000000114</v>
       </c>
     </row>
@@ -9818,7 +9845,7 @@
         <v>0.56388888888888888</v>
       </c>
       <c r="P169" s="2">
-        <f>O170*1440-N169*1440</f>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
     </row>
@@ -9971,7 +9998,7 @@
         <v>0.41180555555555554</v>
       </c>
       <c r="P172" s="2">
-        <f t="shared" ref="P172:P212" si="3">O172*1440-N172*1440</f>
+        <f t="shared" ref="P172:P212" si="4">O172*1440-N172*1440</f>
         <v>90.999999999999943</v>
       </c>
     </row>
@@ -10022,7 +10049,7 @@
         <v>0.41250000000000003</v>
       </c>
       <c r="P173" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89.999999999999943</v>
       </c>
     </row>
@@ -10073,7 +10100,7 @@
         <v>0.41388888888888892</v>
       </c>
       <c r="P174" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89.999999999999943</v>
       </c>
     </row>
@@ -10124,7 +10151,7 @@
         <v>0.4152777777777778</v>
       </c>
       <c r="P175" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.000000000000057</v>
       </c>
     </row>
@@ -10175,7 +10202,7 @@
         <v>0.41597222222222219</v>
       </c>
       <c r="P176" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.000000000000057</v>
       </c>
     </row>
@@ -10226,7 +10253,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="P177" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10277,7 +10304,7 @@
         <v>0.41875000000000001</v>
       </c>
       <c r="P178" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
     </row>
@@ -10328,7 +10355,7 @@
         <v>0.4201388888888889</v>
       </c>
       <c r="P179" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
     </row>
@@ -10379,7 +10406,7 @@
         <v>0.42152777777777778</v>
       </c>
       <c r="P180" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
     </row>
@@ -10430,7 +10457,7 @@
         <v>0.45208333333333334</v>
       </c>
       <c r="P181" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10481,7 +10508,7 @@
         <v>0.45347222222222222</v>
       </c>
       <c r="P182" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10532,7 +10559,7 @@
         <v>0.45416666666666666</v>
       </c>
       <c r="P183" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10583,7 +10610,7 @@
         <v>0.45555555555555555</v>
       </c>
       <c r="P184" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10634,7 +10661,7 @@
         <v>0.45624999999999999</v>
       </c>
       <c r="P185" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
     </row>
@@ -10685,7 +10712,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="P186" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -10736,7 +10763,7 @@
         <v>0.45902777777777781</v>
       </c>
       <c r="P187" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10787,7 +10814,7 @@
         <v>0.4604166666666667</v>
       </c>
       <c r="P188" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -10838,7 +10865,7 @@
         <v>0.46111111111111108</v>
       </c>
       <c r="P189" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10889,7 +10916,7 @@
         <v>0.46249999999999997</v>
       </c>
       <c r="P190" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -10940,7 +10967,7 @@
         <v>0.46388888888888885</v>
       </c>
       <c r="P191" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -10991,7 +11018,7 @@
         <v>0.52847222222222223</v>
       </c>
       <c r="P192" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -11042,7 +11069,7 @@
         <v>0.52986111111111112</v>
       </c>
       <c r="P193" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.000000000000114</v>
       </c>
     </row>
@@ -11093,7 +11120,7 @@
         <v>0.53055555555555556</v>
       </c>
       <c r="P194" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.000000000000114</v>
       </c>
     </row>
@@ -11144,7 +11171,7 @@
         <v>0.53194444444444444</v>
       </c>
       <c r="P195" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -11195,7 +11222,7 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="P196" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -11246,7 +11273,7 @@
         <v>0.53402777777777777</v>
       </c>
       <c r="P197" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.999999999999886</v>
       </c>
     </row>
@@ -11297,7 +11324,7 @@
         <v>0.53541666666666665</v>
       </c>
       <c r="P198" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.999999999999886</v>
       </c>
     </row>
@@ -11348,7 +11375,7 @@
         <v>0.53611111111111109</v>
       </c>
       <c r="P199" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -11399,7 +11426,7 @@
         <v>0.53749999999999998</v>
       </c>
       <c r="P200" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -11450,7 +11477,7 @@
         <v>0.53888888888888886</v>
       </c>
       <c r="P201" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
     </row>
@@ -11501,7 +11528,7 @@
         <v>0.57152777777777775</v>
       </c>
       <c r="P202" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
@@ -11552,7 +11579,7 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="P203" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
     </row>
@@ -11603,7 +11630,7 @@
         <v>0.57430555555555551</v>
       </c>
       <c r="P204" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.999999999999773</v>
       </c>
     </row>
@@ -11654,7 +11681,7 @@
         <v>0.57500000000000007</v>
       </c>
       <c r="P205" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.000000000000227</v>
       </c>
     </row>
@@ -11705,7 +11732,7 @@
         <v>0.57638888888888895</v>
       </c>
       <c r="P206" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.000000000000227</v>
       </c>
     </row>
@@ -11756,7 +11783,7 @@
         <v>0.57708333333333328</v>
       </c>
       <c r="P207" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.999999999999773</v>
       </c>
     </row>
@@ -11807,7 +11834,7 @@
         <v>0.57847222222222217</v>
       </c>
       <c r="P208" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.999999999999773</v>
       </c>
     </row>
@@ -11858,7 +11885,7 @@
         <v>0.57986111111111105</v>
       </c>
       <c r="P209" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.999999999999773</v>
       </c>
     </row>
@@ -11909,7 +11936,7 @@
         <v>0.58124999999999993</v>
       </c>
       <c r="P210" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
     </row>
@@ -11960,7 +11987,7 @@
         <v>0.58194444444444449</v>
       </c>
       <c r="P211" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.000000000000227</v>
       </c>
     </row>
@@ -12011,8 +12038,1736 @@
         <v>0.58263888888888882</v>
       </c>
       <c r="P212" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.999999999999773</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" ht="16" customHeight="1">
+      <c r="A213" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B213" s="1">
+        <v>1</v>
+      </c>
+      <c r="C213" s="1">
+        <v>2</v>
+      </c>
+      <c r="D213" s="1">
+        <v>1</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G213" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H213" s="1">
+        <v>24</v>
+      </c>
+      <c r="I213" s="20">
+        <v>18.042000000000002</v>
+      </c>
+      <c r="J213" s="20">
+        <v>19.326000000000001</v>
+      </c>
+      <c r="K213">
+        <v>1</v>
+      </c>
+      <c r="L213" s="1">
+        <v>1</v>
+      </c>
+      <c r="M213" s="1">
+        <v>32</v>
+      </c>
+      <c r="N213" s="8">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" ht="16" customHeight="1">
+      <c r="A214" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B214" s="1">
+        <v>1</v>
+      </c>
+      <c r="C214" s="1">
+        <v>2</v>
+      </c>
+      <c r="D214" s="1">
+        <v>2</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H214" s="1">
+        <v>25</v>
+      </c>
+      <c r="I214" s="20">
+        <v>17.376999999999999</v>
+      </c>
+      <c r="J214" s="20">
+        <v>18.704000000000001</v>
+      </c>
+      <c r="K214">
+        <v>1</v>
+      </c>
+      <c r="L214" s="1">
+        <v>1</v>
+      </c>
+      <c r="M214" s="1">
+        <v>32</v>
+      </c>
+      <c r="N214" s="8">
+        <v>0.35555555555555557</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" ht="16" customHeight="1">
+      <c r="A215" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B215" s="1">
+        <v>1</v>
+      </c>
+      <c r="C215" s="1">
+        <v>2</v>
+      </c>
+      <c r="D215" s="1">
+        <v>3</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G215" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H215" s="1">
+        <v>26</v>
+      </c>
+      <c r="I215" s="20">
+        <v>17.722999999999999</v>
+      </c>
+      <c r="J215" s="20">
+        <v>18.847000000000001</v>
+      </c>
+      <c r="K215">
+        <v>1</v>
+      </c>
+      <c r="L215" s="1">
+        <v>1</v>
+      </c>
+      <c r="M215" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" ht="16" customHeight="1">
+      <c r="A216" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B216" s="1">
+        <v>1</v>
+      </c>
+      <c r="C216" s="1">
+        <v>2</v>
+      </c>
+      <c r="D216" s="1">
+        <v>4</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G216" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H216" s="1">
+        <v>24</v>
+      </c>
+      <c r="I216" s="20">
+        <v>17.268000000000001</v>
+      </c>
+      <c r="J216" s="20">
+        <v>18.637</v>
+      </c>
+      <c r="K216">
+        <v>1</v>
+      </c>
+      <c r="L216" s="1">
+        <v>1</v>
+      </c>
+      <c r="M216" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" ht="16" customHeight="1">
+      <c r="A217" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B217" s="1">
+        <v>1</v>
+      </c>
+      <c r="C217" s="1">
+        <v>2</v>
+      </c>
+      <c r="D217" s="1">
+        <v>5</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G217" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H217" s="1">
+        <v>27</v>
+      </c>
+      <c r="I217" s="20">
+        <v>17.606000000000002</v>
+      </c>
+      <c r="J217" s="20">
+        <v>18.800999999999998</v>
+      </c>
+      <c r="K217">
+        <v>1</v>
+      </c>
+      <c r="L217" s="1">
+        <v>1</v>
+      </c>
+      <c r="M217" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" ht="16" customHeight="1">
+      <c r="A218" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B218" s="1">
+        <v>1</v>
+      </c>
+      <c r="C218" s="1">
+        <v>2</v>
+      </c>
+      <c r="D218" s="1">
+        <v>6</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G218" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H218" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I218" s="20">
+        <v>17.651</v>
+      </c>
+      <c r="J218" s="20">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="K218">
+        <v>1</v>
+      </c>
+      <c r="L218" s="1">
+        <v>1</v>
+      </c>
+      <c r="M218" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" ht="16" customHeight="1">
+      <c r="A219" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B219" s="1">
+        <v>1</v>
+      </c>
+      <c r="C219" s="1">
+        <v>2</v>
+      </c>
+      <c r="D219" s="1">
+        <v>7</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G219" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H219" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I219" s="20">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="J219" s="20">
+        <v>18.678000000000001</v>
+      </c>
+      <c r="K219">
+        <v>1</v>
+      </c>
+      <c r="L219" s="1">
+        <v>1</v>
+      </c>
+      <c r="M219" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" ht="16" customHeight="1">
+      <c r="A220" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B220" s="1">
+        <v>1</v>
+      </c>
+      <c r="C220" s="1">
+        <v>2</v>
+      </c>
+      <c r="D220" s="1">
+        <v>8</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G220" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H220" s="1">
+        <v>26</v>
+      </c>
+      <c r="I220" s="20">
+        <v>17.606000000000002</v>
+      </c>
+      <c r="J220" s="20">
+        <v>18.702999999999999</v>
+      </c>
+      <c r="K220">
+        <v>1</v>
+      </c>
+      <c r="L220" s="1">
+        <v>1</v>
+      </c>
+      <c r="M220" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" ht="16" customHeight="1">
+      <c r="A221" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B221" s="1">
+        <v>1</v>
+      </c>
+      <c r="C221" s="1">
+        <v>2</v>
+      </c>
+      <c r="D221" s="1">
+        <v>9</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G221" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H221" s="1">
+        <v>25</v>
+      </c>
+      <c r="I221" s="20">
+        <v>17.673999999999999</v>
+      </c>
+      <c r="J221" s="20">
+        <v>18.905000000000001</v>
+      </c>
+      <c r="K221">
+        <v>1</v>
+      </c>
+      <c r="L221" s="1">
+        <v>1</v>
+      </c>
+      <c r="M221" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" ht="16" customHeight="1">
+      <c r="A222" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B222" s="1">
+        <v>1</v>
+      </c>
+      <c r="C222" s="1">
+        <v>2</v>
+      </c>
+      <c r="D222" s="1">
+        <v>10</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H222" s="1">
+        <v>25</v>
+      </c>
+      <c r="I222" s="20">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="J222" s="20">
+        <v>19.099</v>
+      </c>
+      <c r="K222">
+        <v>1</v>
+      </c>
+      <c r="L222" s="1">
+        <v>1</v>
+      </c>
+      <c r="M222" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" ht="16" customHeight="1">
+      <c r="A223" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B223" s="1">
+        <v>1</v>
+      </c>
+      <c r="C223" s="1">
+        <v>2</v>
+      </c>
+      <c r="D223" s="1">
+        <v>11</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G223" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H223" s="1">
+        <v>27</v>
+      </c>
+      <c r="I223" s="20">
+        <v>17.344000000000001</v>
+      </c>
+      <c r="J223" s="20">
+        <v>18.751999999999999</v>
+      </c>
+      <c r="K223">
+        <v>2</v>
+      </c>
+      <c r="L223" s="1">
+        <v>1</v>
+      </c>
+      <c r="M223" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" ht="16" customHeight="1">
+      <c r="A224" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B224" s="1">
+        <v>1</v>
+      </c>
+      <c r="C224" s="1">
+        <v>2</v>
+      </c>
+      <c r="D224" s="1">
+        <v>12</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G224" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H224" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I224" s="20">
+        <v>17.614000000000001</v>
+      </c>
+      <c r="J224" s="20">
+        <v>18.695</v>
+      </c>
+      <c r="K224">
+        <v>2</v>
+      </c>
+      <c r="L224" s="1">
+        <v>1</v>
+      </c>
+      <c r="M224" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" ht="16" customHeight="1">
+      <c r="A225" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B225" s="1">
+        <v>1</v>
+      </c>
+      <c r="C225" s="1">
+        <v>2</v>
+      </c>
+      <c r="D225" s="1">
+        <v>13</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G225" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H225" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="I225" s="20">
+        <v>17.628</v>
+      </c>
+      <c r="J225" s="20">
+        <v>18.600999999999999</v>
+      </c>
+      <c r="K225">
+        <v>2</v>
+      </c>
+      <c r="L225" s="1">
+        <v>1</v>
+      </c>
+      <c r="M225" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" ht="16" customHeight="1">
+      <c r="A226" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B226" s="1">
+        <v>1</v>
+      </c>
+      <c r="C226" s="1">
+        <v>2</v>
+      </c>
+      <c r="D226" s="1">
+        <v>14</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G226" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H226" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="I226" s="20">
+        <v>17.934000000000001</v>
+      </c>
+      <c r="J226" s="20">
+        <v>19.036999999999999</v>
+      </c>
+      <c r="K226">
+        <v>2</v>
+      </c>
+      <c r="L226" s="1">
+        <v>1</v>
+      </c>
+      <c r="M226" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" ht="16" customHeight="1">
+      <c r="A227" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B227" s="1">
+        <v>1</v>
+      </c>
+      <c r="C227" s="1">
+        <v>2</v>
+      </c>
+      <c r="D227" s="1">
+        <v>15</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G227" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H227" s="1">
+        <v>25</v>
+      </c>
+      <c r="I227" s="20">
+        <v>17.792999999999999</v>
+      </c>
+      <c r="J227" s="20">
+        <v>19.093</v>
+      </c>
+      <c r="K227">
+        <v>2</v>
+      </c>
+      <c r="L227" s="1">
+        <v>1</v>
+      </c>
+      <c r="M227" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" ht="16" customHeight="1">
+      <c r="A228" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B228" s="1">
+        <v>1</v>
+      </c>
+      <c r="C228" s="1">
+        <v>2</v>
+      </c>
+      <c r="D228" s="1">
+        <v>16</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G228" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H228" s="1">
+        <v>24</v>
+      </c>
+      <c r="I228" s="20">
+        <v>17.776</v>
+      </c>
+      <c r="J228" s="20">
+        <v>19.172000000000001</v>
+      </c>
+      <c r="K228">
+        <v>2</v>
+      </c>
+      <c r="L228" s="1">
+        <v>1</v>
+      </c>
+      <c r="M228" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" ht="16" customHeight="1">
+      <c r="A229" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B229" s="1">
+        <v>1</v>
+      </c>
+      <c r="C229" s="1">
+        <v>2</v>
+      </c>
+      <c r="D229" s="1">
+        <v>17</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G229" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H229" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I229" s="20">
+        <v>17.463999999999999</v>
+      </c>
+      <c r="J229" s="20">
+        <v>18.841999999999999</v>
+      </c>
+      <c r="K229">
+        <v>2</v>
+      </c>
+      <c r="L229" s="1">
+        <v>1</v>
+      </c>
+      <c r="M229" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" ht="16" customHeight="1">
+      <c r="A230" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B230" s="1">
+        <v>1</v>
+      </c>
+      <c r="C230" s="1">
+        <v>2</v>
+      </c>
+      <c r="D230" s="1">
+        <v>18</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G230" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H230" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I230" s="20">
+        <v>17.652000000000001</v>
+      </c>
+      <c r="J230" s="20">
+        <v>18.739000000000001</v>
+      </c>
+      <c r="K230">
+        <v>2</v>
+      </c>
+      <c r="L230" s="1">
+        <v>1</v>
+      </c>
+      <c r="M230" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" ht="16" customHeight="1">
+      <c r="A231" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B231" s="1">
+        <v>1</v>
+      </c>
+      <c r="C231" s="1">
+        <v>2</v>
+      </c>
+      <c r="D231" s="1">
+        <v>19</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G231" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H231" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I231" s="20">
+        <v>17.291</v>
+      </c>
+      <c r="J231" s="20">
+        <v>18.18</v>
+      </c>
+      <c r="K231">
+        <v>2</v>
+      </c>
+      <c r="L231" s="1">
+        <v>1</v>
+      </c>
+      <c r="M231" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" ht="16" customHeight="1">
+      <c r="A232" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B232" s="1">
+        <v>1</v>
+      </c>
+      <c r="C232" s="1">
+        <v>2</v>
+      </c>
+      <c r="D232" s="1">
+        <v>20</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G232" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H232" s="1">
+        <v>26</v>
+      </c>
+      <c r="I232" s="20">
+        <v>17.533000000000001</v>
+      </c>
+      <c r="J232" s="20">
+        <v>18.739000000000001</v>
+      </c>
+      <c r="K232">
+        <v>2</v>
+      </c>
+      <c r="L232" s="1">
+        <v>1</v>
+      </c>
+      <c r="M232" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" ht="16" customHeight="1">
+      <c r="A233" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B233" s="1">
+        <v>1</v>
+      </c>
+      <c r="C233" s="1">
+        <v>2</v>
+      </c>
+      <c r="D233" s="1">
+        <v>21</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G233" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H233" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I233" s="20">
+        <v>17.449000000000002</v>
+      </c>
+      <c r="J233" s="20">
+        <v>18.835999999999999</v>
+      </c>
+      <c r="K233">
+        <v>2</v>
+      </c>
+      <c r="L233" s="1">
+        <v>1</v>
+      </c>
+      <c r="M233" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" ht="16" customHeight="1">
+      <c r="A234" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B234" s="1">
+        <v>1</v>
+      </c>
+      <c r="C234" s="1">
+        <v>2</v>
+      </c>
+      <c r="D234" s="1">
+        <v>1</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G234" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H234" s="1">
+        <v>24</v>
+      </c>
+      <c r="I234" s="20">
+        <v>18.042000000000002</v>
+      </c>
+      <c r="J234" s="20">
+        <v>19.326000000000001</v>
+      </c>
+      <c r="K234">
+        <v>1</v>
+      </c>
+      <c r="L234" s="1">
+        <v>2</v>
+      </c>
+      <c r="M234" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" ht="16" customHeight="1">
+      <c r="A235" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B235" s="1">
+        <v>1</v>
+      </c>
+      <c r="C235" s="1">
+        <v>2</v>
+      </c>
+      <c r="D235" s="1">
+        <v>2</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G235" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H235" s="1">
+        <v>25</v>
+      </c>
+      <c r="I235" s="20">
+        <v>17.376999999999999</v>
+      </c>
+      <c r="J235" s="20">
+        <v>18.704000000000001</v>
+      </c>
+      <c r="K235">
+        <v>1</v>
+      </c>
+      <c r="L235" s="1">
+        <v>2</v>
+      </c>
+      <c r="M235" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" ht="16" customHeight="1">
+      <c r="A236" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B236" s="1">
+        <v>1</v>
+      </c>
+      <c r="C236" s="1">
+        <v>2</v>
+      </c>
+      <c r="D236" s="1">
+        <v>3</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G236" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H236" s="1">
+        <v>26</v>
+      </c>
+      <c r="I236" s="20">
+        <v>17.722999999999999</v>
+      </c>
+      <c r="J236" s="20">
+        <v>18.847000000000001</v>
+      </c>
+      <c r="K236">
+        <v>1</v>
+      </c>
+      <c r="L236" s="1">
+        <v>2</v>
+      </c>
+      <c r="M236" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" ht="16" customHeight="1">
+      <c r="A237" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B237" s="1">
+        <v>1</v>
+      </c>
+      <c r="C237" s="1">
+        <v>2</v>
+      </c>
+      <c r="D237" s="1">
+        <v>4</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G237" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H237" s="1">
+        <v>24</v>
+      </c>
+      <c r="I237" s="20">
+        <v>17.268000000000001</v>
+      </c>
+      <c r="J237" s="20">
+        <v>18.637</v>
+      </c>
+      <c r="K237">
+        <v>1</v>
+      </c>
+      <c r="L237" s="1">
+        <v>2</v>
+      </c>
+      <c r="M237" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" ht="16" customHeight="1">
+      <c r="A238" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B238" s="1">
+        <v>1</v>
+      </c>
+      <c r="C238" s="1">
+        <v>2</v>
+      </c>
+      <c r="D238" s="1">
+        <v>5</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G238" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H238" s="1">
+        <v>27</v>
+      </c>
+      <c r="I238" s="20">
+        <v>17.606000000000002</v>
+      </c>
+      <c r="J238" s="20">
+        <v>18.800999999999998</v>
+      </c>
+      <c r="K238">
+        <v>1</v>
+      </c>
+      <c r="L238" s="1">
+        <v>2</v>
+      </c>
+      <c r="M238" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" ht="16" customHeight="1">
+      <c r="A239" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B239" s="1">
+        <v>1</v>
+      </c>
+      <c r="C239" s="1">
+        <v>2</v>
+      </c>
+      <c r="D239" s="1">
+        <v>6</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G239" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H239" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I239" s="20">
+        <v>17.651</v>
+      </c>
+      <c r="J239" s="20">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="K239">
+        <v>1</v>
+      </c>
+      <c r="L239" s="1">
+        <v>2</v>
+      </c>
+      <c r="M239" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" ht="16" customHeight="1">
+      <c r="A240" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B240" s="1">
+        <v>1</v>
+      </c>
+      <c r="C240" s="1">
+        <v>2</v>
+      </c>
+      <c r="D240" s="1">
+        <v>7</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G240" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H240" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I240" s="20">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="J240" s="20">
+        <v>18.678000000000001</v>
+      </c>
+      <c r="K240">
+        <v>1</v>
+      </c>
+      <c r="L240" s="1">
+        <v>2</v>
+      </c>
+      <c r="M240" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" ht="16" customHeight="1">
+      <c r="A241" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B241" s="1">
+        <v>1</v>
+      </c>
+      <c r="C241" s="1">
+        <v>2</v>
+      </c>
+      <c r="D241" s="1">
+        <v>8</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G241" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H241" s="1">
+        <v>26</v>
+      </c>
+      <c r="I241" s="20">
+        <v>17.606000000000002</v>
+      </c>
+      <c r="J241" s="20">
+        <v>18.702999999999999</v>
+      </c>
+      <c r="K241">
+        <v>1</v>
+      </c>
+      <c r="L241" s="1">
+        <v>2</v>
+      </c>
+      <c r="M241" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" ht="16" customHeight="1">
+      <c r="A242" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B242" s="1">
+        <v>1</v>
+      </c>
+      <c r="C242" s="1">
+        <v>2</v>
+      </c>
+      <c r="D242" s="1">
+        <v>9</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G242" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H242" s="1">
+        <v>25</v>
+      </c>
+      <c r="I242" s="20">
+        <v>17.673999999999999</v>
+      </c>
+      <c r="J242" s="20">
+        <v>18.905000000000001</v>
+      </c>
+      <c r="K242">
+        <v>1</v>
+      </c>
+      <c r="L242" s="1">
+        <v>2</v>
+      </c>
+      <c r="M242" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" ht="16" customHeight="1">
+      <c r="A243" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B243" s="1">
+        <v>1</v>
+      </c>
+      <c r="C243" s="1">
+        <v>2</v>
+      </c>
+      <c r="D243" s="1">
+        <v>10</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G243" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H243" s="1">
+        <v>25</v>
+      </c>
+      <c r="I243" s="20">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="J243" s="20">
+        <v>19.099</v>
+      </c>
+      <c r="K243">
+        <v>1</v>
+      </c>
+      <c r="L243" s="1">
+        <v>2</v>
+      </c>
+      <c r="M243" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" ht="16" customHeight="1">
+      <c r="A244" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B244" s="1">
+        <v>1</v>
+      </c>
+      <c r="C244" s="1">
+        <v>2</v>
+      </c>
+      <c r="D244" s="1">
+        <v>11</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G244" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H244" s="1">
+        <v>27</v>
+      </c>
+      <c r="I244" s="20">
+        <v>17.344000000000001</v>
+      </c>
+      <c r="J244" s="20">
+        <v>18.751999999999999</v>
+      </c>
+      <c r="K244">
+        <v>2</v>
+      </c>
+      <c r="L244" s="1">
+        <v>2</v>
+      </c>
+      <c r="M244" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" ht="16" customHeight="1">
+      <c r="A245" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B245" s="1">
+        <v>1</v>
+      </c>
+      <c r="C245" s="1">
+        <v>2</v>
+      </c>
+      <c r="D245" s="1">
+        <v>12</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G245" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H245" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I245" s="20">
+        <v>17.614000000000001</v>
+      </c>
+      <c r="J245" s="20">
+        <v>18.695</v>
+      </c>
+      <c r="K245">
+        <v>2</v>
+      </c>
+      <c r="L245" s="1">
+        <v>2</v>
+      </c>
+      <c r="M245" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" ht="16" customHeight="1">
+      <c r="A246" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B246" s="1">
+        <v>1</v>
+      </c>
+      <c r="C246" s="1">
+        <v>2</v>
+      </c>
+      <c r="D246" s="1">
+        <v>13</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G246" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H246" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="I246" s="20">
+        <v>17.628</v>
+      </c>
+      <c r="J246" s="20">
+        <v>18.600999999999999</v>
+      </c>
+      <c r="K246">
+        <v>2</v>
+      </c>
+      <c r="L246" s="1">
+        <v>2</v>
+      </c>
+      <c r="M246" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" ht="16" customHeight="1">
+      <c r="A247" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B247" s="1">
+        <v>1</v>
+      </c>
+      <c r="C247" s="1">
+        <v>2</v>
+      </c>
+      <c r="D247" s="1">
+        <v>14</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G247" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H247" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="I247" s="20">
+        <v>17.934000000000001</v>
+      </c>
+      <c r="J247" s="20">
+        <v>19.036999999999999</v>
+      </c>
+      <c r="K247">
+        <v>2</v>
+      </c>
+      <c r="L247" s="1">
+        <v>2</v>
+      </c>
+      <c r="M247" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" ht="16" customHeight="1">
+      <c r="A248" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B248" s="1">
+        <v>1</v>
+      </c>
+      <c r="C248" s="1">
+        <v>2</v>
+      </c>
+      <c r="D248" s="1">
+        <v>15</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H248" s="1">
+        <v>25</v>
+      </c>
+      <c r="I248" s="20">
+        <v>17.792999999999999</v>
+      </c>
+      <c r="J248" s="20">
+        <v>19.093</v>
+      </c>
+      <c r="K248">
+        <v>2</v>
+      </c>
+      <c r="L248" s="1">
+        <v>2</v>
+      </c>
+      <c r="M248" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" ht="16" customHeight="1">
+      <c r="A249" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B249" s="1">
+        <v>1</v>
+      </c>
+      <c r="C249" s="1">
+        <v>2</v>
+      </c>
+      <c r="D249" s="1">
+        <v>16</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G249" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H249" s="1">
+        <v>24</v>
+      </c>
+      <c r="I249" s="20">
+        <v>17.776</v>
+      </c>
+      <c r="J249" s="20">
+        <v>19.172000000000001</v>
+      </c>
+      <c r="K249">
+        <v>2</v>
+      </c>
+      <c r="L249" s="1">
+        <v>2</v>
+      </c>
+      <c r="M249" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" ht="16" customHeight="1">
+      <c r="A250" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B250" s="1">
+        <v>1</v>
+      </c>
+      <c r="C250" s="1">
+        <v>2</v>
+      </c>
+      <c r="D250" s="1">
+        <v>17</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G250" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H250" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I250" s="20">
+        <v>17.463999999999999</v>
+      </c>
+      <c r="J250" s="20">
+        <v>18.841999999999999</v>
+      </c>
+      <c r="K250">
+        <v>2</v>
+      </c>
+      <c r="L250" s="1">
+        <v>2</v>
+      </c>
+      <c r="M250" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" ht="16" customHeight="1">
+      <c r="A251" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B251" s="1">
+        <v>1</v>
+      </c>
+      <c r="C251" s="1">
+        <v>2</v>
+      </c>
+      <c r="D251" s="1">
+        <v>18</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G251" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H251" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I251" s="20">
+        <v>17.652000000000001</v>
+      </c>
+      <c r="J251" s="20">
+        <v>18.739000000000001</v>
+      </c>
+      <c r="K251">
+        <v>2</v>
+      </c>
+      <c r="L251" s="1">
+        <v>2</v>
+      </c>
+      <c r="M251" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" ht="16" customHeight="1">
+      <c r="A252" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B252" s="1">
+        <v>1</v>
+      </c>
+      <c r="C252" s="1">
+        <v>2</v>
+      </c>
+      <c r="D252" s="1">
+        <v>19</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G252" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H252" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I252" s="20">
+        <v>17.291</v>
+      </c>
+      <c r="J252" s="20">
+        <v>18.18</v>
+      </c>
+      <c r="K252">
+        <v>2</v>
+      </c>
+      <c r="L252" s="1">
+        <v>2</v>
+      </c>
+      <c r="M252" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" ht="16" customHeight="1">
+      <c r="A253" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B253" s="1">
+        <v>1</v>
+      </c>
+      <c r="C253" s="1">
+        <v>2</v>
+      </c>
+      <c r="D253" s="1">
+        <v>20</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G253" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H253" s="1">
+        <v>26</v>
+      </c>
+      <c r="I253" s="20">
+        <v>17.533000000000001</v>
+      </c>
+      <c r="J253" s="20">
+        <v>18.739000000000001</v>
+      </c>
+      <c r="K253">
+        <v>2</v>
+      </c>
+      <c r="L253" s="1">
+        <v>2</v>
+      </c>
+      <c r="M253" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" ht="16" customHeight="1">
+      <c r="A254" s="3">
+        <v>42705</v>
+      </c>
+      <c r="B254" s="1">
+        <v>1</v>
+      </c>
+      <c r="C254" s="1">
+        <v>2</v>
+      </c>
+      <c r="D254" s="1">
+        <v>21</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G254" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H254" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I254" s="20">
+        <v>17.449000000000002</v>
+      </c>
+      <c r="J254" s="20">
+        <v>18.835999999999999</v>
+      </c>
+      <c r="K254">
+        <v>2</v>
+      </c>
+      <c r="L254" s="1">
+        <v>2</v>
+      </c>
+      <c r="M254" s="1">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entered temp and mass data for 16/1/17
</commit_message>
<xml_diff>
--- a/data/ldeli_integrate.xlsx
+++ b/data/ldeli_integrate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="3440" windowWidth="16040" windowHeight="11140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5417" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5432" uniqueCount="171">
   <si>
     <t>date</t>
   </si>
@@ -531,6 +531,9 @@
   <si>
     <t>MultiPO2BL</t>
   </si>
+  <si>
+    <t>DoublePO2BL</t>
+  </si>
 </sst>
 </file>
 
@@ -626,11 +629,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="538">
+  <cellStyleXfs count="574">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1251,7 +1290,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="538">
+  <cellStyles count="574">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1522,6 +1561,24 @@
     <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -1789,6 +1846,24 @@
     <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2118,11 +2193,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD1779"/>
+  <dimension ref="A1:AG1779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T43" sqref="T43"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1302" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1314" sqref="G1314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -4867,6 +4942,15 @@
       <c r="Q44" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="R44" s="28">
+        <v>2.101E-3</v>
+      </c>
+      <c r="S44" s="1">
+        <v>1.2664699999999999E-2</v>
+      </c>
+      <c r="T44" s="1">
+        <v>1.34059E-2</v>
+      </c>
     </row>
     <row r="45" spans="1:29" ht="16" customHeight="1">
       <c r="A45" s="3">
@@ -4918,6 +5002,15 @@
       <c r="Q45" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="R45" s="28">
+        <v>1.191E-3</v>
+      </c>
+      <c r="S45" s="1">
+        <v>1.05781E-2</v>
+      </c>
+      <c r="T45" s="1">
+        <v>8.7690000000000008E-3</v>
+      </c>
     </row>
     <row r="46" spans="1:29" ht="16" customHeight="1">
       <c r="A46" s="3">
@@ -4969,6 +5062,15 @@
       <c r="Q46" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="R46" s="28">
+        <v>1.1100000000000001E-3</v>
+      </c>
+      <c r="S46" s="1">
+        <v>7.9112999999999996E-3</v>
+      </c>
+      <c r="T46" s="28">
+        <v>7.1289999999999999E-3</v>
+      </c>
     </row>
     <row r="47" spans="1:29" ht="16" customHeight="1">
       <c r="A47" s="3">
@@ -5020,6 +5122,15 @@
       <c r="Q47" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="R47" s="28">
+        <v>3.9970000000000001E-4</v>
+      </c>
+      <c r="S47" s="1">
+        <v>8.9168000000000008E-3</v>
+      </c>
+      <c r="T47" s="28">
+        <v>7.6889999999999997E-3</v>
+      </c>
     </row>
     <row r="48" spans="1:29" ht="16" customHeight="1">
       <c r="A48" s="3">
@@ -5071,8 +5182,17 @@
       <c r="Q48" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" ht="16" customHeight="1">
+      <c r="R48" s="28">
+        <v>1.224E-3</v>
+      </c>
+      <c r="S48" s="1">
+        <v>8.8973000000000003E-3</v>
+      </c>
+      <c r="T48" s="1">
+        <v>8.7150999999999999E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" ht="16" customHeight="1">
       <c r="A49" s="3">
         <v>42731</v>
       </c>
@@ -5122,8 +5242,17 @@
       <c r="Q49" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" ht="16" customHeight="1">
+      <c r="R49" s="28">
+        <v>1.547E-3</v>
+      </c>
+      <c r="S49" s="1">
+        <v>1.00786E-2</v>
+      </c>
+      <c r="T49" s="1">
+        <v>9.6693000000000005E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" ht="16" customHeight="1">
       <c r="A50" s="3">
         <v>42731</v>
       </c>
@@ -5173,8 +5302,17 @@
       <c r="Q50" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" ht="16" customHeight="1">
+      <c r="R50" s="28">
+        <v>7.9060000000000003E-4</v>
+      </c>
+      <c r="S50" s="1">
+        <v>8.1457999999999999E-3</v>
+      </c>
+      <c r="T50" s="1">
+        <v>9.5759999999999994E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" ht="16" customHeight="1">
       <c r="A51" s="3">
         <v>42731</v>
       </c>
@@ -5224,8 +5362,20 @@
       <c r="Q51" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" ht="16" customHeight="1">
+      <c r="R51" s="28">
+        <v>1.1130000000000001E-3</v>
+      </c>
+      <c r="S51" s="1">
+        <v>1.60006E-2</v>
+      </c>
+      <c r="T51" s="1">
+        <v>1.5185499999999999E-2</v>
+      </c>
+      <c r="AC51" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" ht="16" customHeight="1">
       <c r="A52" s="3">
         <v>42731</v>
       </c>
@@ -5275,8 +5425,17 @@
       <c r="Q52" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" ht="16" customHeight="1">
+      <c r="R52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S52" s="28">
+        <v>5.5620000000000001E-3</v>
+      </c>
+      <c r="T52" s="28">
+        <v>3.2469999999999999E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" ht="16" customHeight="1">
       <c r="A53" s="3">
         <v>42731</v>
       </c>
@@ -5326,8 +5485,18 @@
       <c r="Q53" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" ht="16" customHeight="1">
+      <c r="R53" s="28">
+        <v>4.1950000000000001E-4</v>
+      </c>
+      <c r="S53" s="1">
+        <v>9.2853999999999992E-3</v>
+      </c>
+      <c r="T53" s="1">
+        <v>8.3931000000000006E-3</v>
+      </c>
+      <c r="AA53" s="28"/>
+    </row>
+    <row r="54" spans="1:29" ht="16" customHeight="1">
       <c r="A54" s="3">
         <v>42731</v>
       </c>
@@ -5377,8 +5546,20 @@
       <c r="Q54" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" ht="16" customHeight="1">
+      <c r="R54" s="28">
+        <v>5.4120000000000004E-4</v>
+      </c>
+      <c r="S54" s="28">
+        <v>4.6039999999999996E-3</v>
+      </c>
+      <c r="T54" s="28">
+        <v>6.8279999999999999E-3</v>
+      </c>
+      <c r="AA54" s="28"/>
+      <c r="AB54" s="28"/>
+      <c r="AC54" s="28"/>
+    </row>
+    <row r="55" spans="1:29" ht="16" customHeight="1">
       <c r="A55" s="3">
         <v>42731</v>
       </c>
@@ -5428,8 +5609,17 @@
       <c r="Q55" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" ht="16" customHeight="1">
+      <c r="R55" s="28">
+        <v>3.4880000000000002E-4</v>
+      </c>
+      <c r="S55" s="28">
+        <v>4.6389999999999999E-3</v>
+      </c>
+      <c r="T55" s="28">
+        <v>5.9579999999999998E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" ht="16" customHeight="1">
       <c r="A56" s="3">
         <v>42731</v>
       </c>
@@ -5479,8 +5669,17 @@
       <c r="Q56" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" ht="16" customHeight="1">
+      <c r="R56" s="28">
+        <v>6.2929999999999995E-4</v>
+      </c>
+      <c r="S56" s="28">
+        <v>6.4200000000000004E-3</v>
+      </c>
+      <c r="T56" s="28">
+        <v>7.561E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" ht="16" customHeight="1">
       <c r="A57" s="3">
         <v>42731</v>
       </c>
@@ -5530,8 +5729,17 @@
       <c r="Q57" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" ht="16" customHeight="1">
+      <c r="R57" s="28">
+        <v>3.5560000000000002E-4</v>
+      </c>
+      <c r="S57" s="28">
+        <v>4.1180000000000001E-3</v>
+      </c>
+      <c r="T57" s="28">
+        <v>4.3400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" ht="16" customHeight="1">
       <c r="A58" s="3">
         <v>42731</v>
       </c>
@@ -5581,8 +5789,17 @@
       <c r="Q58" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" ht="16" customHeight="1">
+      <c r="R58" s="28">
+        <v>3.3639999999999999E-4</v>
+      </c>
+      <c r="S58" s="28">
+        <v>5.5859999999999998E-3</v>
+      </c>
+      <c r="T58" s="28">
+        <v>5.5259999999999997E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" ht="16" customHeight="1">
       <c r="A59" s="3">
         <v>42731</v>
       </c>
@@ -5632,8 +5849,17 @@
       <c r="Q59" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" ht="16" customHeight="1">
+      <c r="R59" s="28">
+        <v>1.379E-3</v>
+      </c>
+      <c r="S59" s="1">
+        <v>1.2882599999999999E-2</v>
+      </c>
+      <c r="T59" s="1">
+        <v>1.12832E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" ht="16" customHeight="1">
       <c r="A60" s="3">
         <v>42731</v>
       </c>
@@ -5683,8 +5909,17 @@
       <c r="Q60" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" ht="16" customHeight="1">
+      <c r="R60" s="28">
+        <v>3.3819999999999998E-4</v>
+      </c>
+      <c r="S60" s="28">
+        <v>4.7479999999999996E-3</v>
+      </c>
+      <c r="T60" s="28">
+        <v>6.1050000000000002E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" ht="16" customHeight="1">
       <c r="A61" s="3">
         <v>42731</v>
       </c>
@@ -5734,8 +5969,17 @@
       <c r="Q61" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" ht="16" customHeight="1">
+      <c r="R61" s="28">
+        <v>9.2639999999999997E-4</v>
+      </c>
+      <c r="S61" s="28">
+        <v>6.4400000000000004E-3</v>
+      </c>
+      <c r="T61" s="28">
+        <v>9.4839999999999996E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" ht="16" customHeight="1">
       <c r="A62" s="3">
         <v>42731</v>
       </c>
@@ -5785,8 +6029,20 @@
       <c r="Q62" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" ht="16" customHeight="1">
+      <c r="R62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S62" s="1">
+        <v>8.5682999999999992E-3</v>
+      </c>
+      <c r="T62" s="28">
+        <v>4.6430000000000004E-3</v>
+      </c>
+      <c r="AC62" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" ht="16" customHeight="1">
       <c r="A63" s="3">
         <v>42731</v>
       </c>
@@ -5836,8 +6092,17 @@
       <c r="Q63" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" ht="16" customHeight="1">
+      <c r="R63" s="28">
+        <v>2.349E-3</v>
+      </c>
+      <c r="S63" s="1">
+        <v>1.1680299999999999E-2</v>
+      </c>
+      <c r="T63" s="28">
+        <v>5.2480000000000001E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" ht="16" customHeight="1">
       <c r="A64" s="3">
         <v>42731</v>
       </c>
@@ -5887,8 +6152,17 @@
       <c r="Q64" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" ht="16" customHeight="1">
+      <c r="R64" s="28">
+        <v>7.672E-4</v>
+      </c>
+      <c r="S64" s="1">
+        <v>8.2289000000000008E-3</v>
+      </c>
+      <c r="T64" s="28">
+        <v>6.339E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:33" ht="16" customHeight="1">
       <c r="A65" s="3">
         <v>42731</v>
       </c>
@@ -5938,8 +6212,20 @@
       <c r="Q65" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" ht="16" customHeight="1">
+      <c r="R65" s="28">
+        <v>1.6130000000000001E-3</v>
+      </c>
+      <c r="S65" s="28">
+        <v>6.1700000000000001E-3</v>
+      </c>
+      <c r="T65" s="28">
+        <v>5.5950000000000001E-3</v>
+      </c>
+      <c r="AE65" s="28"/>
+      <c r="AF65" s="28"/>
+      <c r="AG65" s="28"/>
+    </row>
+    <row r="66" spans="1:33" ht="16" customHeight="1">
       <c r="A66" s="3">
         <v>42731</v>
       </c>
@@ -5989,8 +6275,20 @@
       <c r="Q66" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" ht="16" customHeight="1">
+      <c r="R66" s="28">
+        <v>9.3479999999999995E-4</v>
+      </c>
+      <c r="S66" s="28">
+        <v>7.6740000000000003E-3</v>
+      </c>
+      <c r="T66" s="28">
+        <v>7.2550000000000002E-3</v>
+      </c>
+      <c r="AE66" s="28"/>
+      <c r="AF66" s="28"/>
+      <c r="AG66" s="28"/>
+    </row>
+    <row r="67" spans="1:33" ht="16" customHeight="1">
       <c r="A67" s="3">
         <v>42731</v>
       </c>
@@ -6040,8 +6338,20 @@
       <c r="Q67" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" ht="16" customHeight="1">
+      <c r="R67" s="28">
+        <v>7.8810000000000002E-4</v>
+      </c>
+      <c r="S67" s="28">
+        <v>3.369E-3</v>
+      </c>
+      <c r="T67" s="28">
+        <v>3.0100000000000001E-3</v>
+      </c>
+      <c r="AE67" s="28"/>
+      <c r="AF67" s="28"/>
+      <c r="AG67" s="28"/>
+    </row>
+    <row r="68" spans="1:33" ht="16" customHeight="1">
       <c r="A68" s="3">
         <v>42731</v>
       </c>
@@ -6091,8 +6401,20 @@
       <c r="Q68" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" ht="16" customHeight="1">
+      <c r="R68" s="28">
+        <v>4.8970000000000003E-4</v>
+      </c>
+      <c r="S68" s="28">
+        <v>3.6949999999999999E-3</v>
+      </c>
+      <c r="T68" s="28">
+        <v>3.6059999999999998E-3</v>
+      </c>
+      <c r="AE68" s="28"/>
+      <c r="AF68" s="28"/>
+      <c r="AG68" s="28"/>
+    </row>
+    <row r="69" spans="1:33" ht="16" customHeight="1">
       <c r="A69" s="3">
         <v>42731</v>
       </c>
@@ -6142,8 +6464,20 @@
       <c r="Q69" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" ht="16" customHeight="1">
+      <c r="R69" s="28">
+        <v>9.6389999999999996E-4</v>
+      </c>
+      <c r="S69" s="28">
+        <v>4.0359999999999997E-3</v>
+      </c>
+      <c r="T69" s="28">
+        <v>2.4910000000000002E-3</v>
+      </c>
+      <c r="AE69" s="28"/>
+      <c r="AF69" s="28"/>
+      <c r="AG69" s="28"/>
+    </row>
+    <row r="70" spans="1:33" ht="16" customHeight="1">
       <c r="A70" s="3">
         <v>42731</v>
       </c>
@@ -6193,8 +6527,20 @@
       <c r="Q70" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" ht="16" customHeight="1">
+      <c r="R70" s="28">
+        <v>9.4839999999999996E-4</v>
+      </c>
+      <c r="S70" s="28">
+        <v>4.339E-3</v>
+      </c>
+      <c r="T70" s="28">
+        <v>4.3819999999999996E-3</v>
+      </c>
+      <c r="AE70" s="28"/>
+      <c r="AF70" s="28"/>
+      <c r="AG70" s="28"/>
+    </row>
+    <row r="71" spans="1:33" ht="16" customHeight="1">
       <c r="A71" s="3">
         <v>42731</v>
       </c>
@@ -6244,8 +6590,20 @@
       <c r="Q71" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" ht="16" customHeight="1">
+      <c r="R71" s="28">
+        <v>6.7770000000000005E-4</v>
+      </c>
+      <c r="S71" s="28">
+        <v>3.761E-3</v>
+      </c>
+      <c r="T71" s="28">
+        <v>3.529E-3</v>
+      </c>
+      <c r="AE71" s="28"/>
+      <c r="AF71" s="28"/>
+      <c r="AG71" s="28"/>
+    </row>
+    <row r="72" spans="1:33" ht="16" customHeight="1">
       <c r="A72" s="3">
         <v>42731</v>
       </c>
@@ -6295,8 +6653,18 @@
       <c r="Q72" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" ht="16" customHeight="1">
+      <c r="R72" s="28">
+        <v>4.8529999999999998E-4</v>
+      </c>
+      <c r="S72" s="1">
+        <v>1.2591700000000001E-2</v>
+      </c>
+      <c r="T72" s="1">
+        <v>1.29084E-2</v>
+      </c>
+      <c r="AE72" s="28"/>
+    </row>
+    <row r="73" spans="1:33" ht="16" customHeight="1">
       <c r="A73" s="3">
         <v>42731</v>
       </c>
@@ -6346,8 +6714,23 @@
       <c r="Q73" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" ht="16" customHeight="1">
+      <c r="R73" s="28">
+        <v>1.6119999999999999E-3</v>
+      </c>
+      <c r="S73" s="28">
+        <v>2.4710000000000001E-3</v>
+      </c>
+      <c r="T73" s="28">
+        <v>2.0860000000000002E-3</v>
+      </c>
+      <c r="AC73" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE73" s="28"/>
+      <c r="AF73" s="28"/>
+      <c r="AG73" s="28"/>
+    </row>
+    <row r="74" spans="1:33" ht="16" customHeight="1">
       <c r="A74" s="3">
         <v>42731</v>
       </c>
@@ -6397,8 +6780,20 @@
       <c r="Q74" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" ht="16" customHeight="1">
+      <c r="R74" s="28">
+        <v>5.2979999999999998E-4</v>
+      </c>
+      <c r="S74" s="28">
+        <v>4.0759999999999998E-3</v>
+      </c>
+      <c r="T74" s="28">
+        <v>3.8660000000000001E-3</v>
+      </c>
+      <c r="AE74" s="28"/>
+      <c r="AF74" s="28"/>
+      <c r="AG74" s="28"/>
+    </row>
+    <row r="75" spans="1:33" ht="16" customHeight="1">
       <c r="A75" s="3">
         <v>42731</v>
       </c>
@@ -6448,8 +6843,20 @@
       <c r="Q75" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" ht="16" customHeight="1">
+      <c r="R75" s="28">
+        <v>1.067E-3</v>
+      </c>
+      <c r="S75" s="28">
+        <v>7.077E-3</v>
+      </c>
+      <c r="T75" s="28">
+        <v>6.4050000000000001E-3</v>
+      </c>
+      <c r="AE75" s="28"/>
+      <c r="AF75" s="28"/>
+      <c r="AG75" s="28"/>
+    </row>
+    <row r="76" spans="1:33" ht="16" customHeight="1">
       <c r="A76" s="3">
         <v>42731</v>
       </c>
@@ -6499,8 +6906,20 @@
       <c r="Q76" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" ht="16" customHeight="1">
+      <c r="R76" s="28">
+        <v>1.1739999999999999E-3</v>
+      </c>
+      <c r="S76" s="28">
+        <v>5.8580000000000004E-3</v>
+      </c>
+      <c r="T76" s="28">
+        <v>6.3010000000000002E-3</v>
+      </c>
+      <c r="AE76" s="28"/>
+      <c r="AF76" s="28"/>
+      <c r="AG76" s="28"/>
+    </row>
+    <row r="77" spans="1:33" ht="16" customHeight="1">
       <c r="A77" s="3">
         <v>42731</v>
       </c>
@@ -6550,8 +6969,23 @@
       <c r="Q77" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" ht="16" customHeight="1">
+      <c r="R77" s="28">
+        <v>5.0109999999999998E-4</v>
+      </c>
+      <c r="S77" s="28">
+        <v>4.0099999999999997E-3</v>
+      </c>
+      <c r="T77" s="28">
+        <v>3.4550000000000002E-3</v>
+      </c>
+      <c r="AC77" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE77" s="28"/>
+      <c r="AF77" s="28"/>
+      <c r="AG77" s="28"/>
+    </row>
+    <row r="78" spans="1:33" ht="16" customHeight="1">
       <c r="A78" s="3">
         <v>42731</v>
       </c>
@@ -6601,8 +7035,20 @@
       <c r="Q78" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" ht="16" customHeight="1">
+      <c r="R78" s="28">
+        <v>7.6460000000000005E-4</v>
+      </c>
+      <c r="S78" s="28">
+        <v>2.928E-3</v>
+      </c>
+      <c r="T78" s="28">
+        <v>3.2569999999999999E-3</v>
+      </c>
+      <c r="AE78" s="28"/>
+      <c r="AF78" s="28"/>
+      <c r="AG78" s="28"/>
+    </row>
+    <row r="79" spans="1:33" ht="16" customHeight="1">
       <c r="A79" s="3">
         <v>42731</v>
       </c>
@@ -6652,8 +7098,20 @@
       <c r="Q79" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" ht="16" customHeight="1">
+      <c r="R79" s="28">
+        <v>1.2870000000000001E-4</v>
+      </c>
+      <c r="S79" s="28">
+        <v>5.0169999999999998E-3</v>
+      </c>
+      <c r="T79" s="28">
+        <v>5.032E-3</v>
+      </c>
+      <c r="AE79" s="28"/>
+      <c r="AF79" s="28"/>
+      <c r="AG79" s="28"/>
+    </row>
+    <row r="80" spans="1:33" ht="16" customHeight="1">
       <c r="A80" s="3">
         <v>42731</v>
       </c>
@@ -6703,8 +7161,20 @@
       <c r="Q80" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="81" spans="1:23" ht="16" customHeight="1">
+      <c r="R80" s="28">
+        <v>1.2819999999999999E-3</v>
+      </c>
+      <c r="S80" s="28">
+        <v>6.9100000000000003E-3</v>
+      </c>
+      <c r="T80" s="28">
+        <v>7.0889999999999998E-3</v>
+      </c>
+      <c r="AE80" s="28"/>
+      <c r="AF80" s="28"/>
+      <c r="AG80" s="28"/>
+    </row>
+    <row r="81" spans="1:33" ht="16" customHeight="1">
       <c r="A81" s="3">
         <v>42731</v>
       </c>
@@ -6754,8 +7224,22 @@
       <c r="Q81" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="82" spans="1:23" ht="16" customHeight="1">
+      <c r="R81" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S81" s="28">
+        <v>3.7720000000000002E-3</v>
+      </c>
+      <c r="T81" s="28">
+        <v>3.2239999999999999E-3</v>
+      </c>
+      <c r="AC81" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF81" s="28"/>
+      <c r="AG81" s="28"/>
+    </row>
+    <row r="82" spans="1:33" ht="16" customHeight="1">
       <c r="A82" s="3">
         <v>42731</v>
       </c>
@@ -6805,8 +7289,23 @@
       <c r="Q82" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="83" spans="1:23" ht="16" customHeight="1">
+      <c r="R82" s="28">
+        <v>1.0939999999999999E-3</v>
+      </c>
+      <c r="S82" s="28">
+        <v>7.4299999999999995E-4</v>
+      </c>
+      <c r="T82" s="28">
+        <v>6.6680000000000003E-3</v>
+      </c>
+      <c r="AC82" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE82" s="28"/>
+      <c r="AF82" s="28"/>
+      <c r="AG82" s="28"/>
+    </row>
+    <row r="83" spans="1:33" ht="16" customHeight="1">
       <c r="A83" s="3">
         <v>42731</v>
       </c>
@@ -6856,8 +7355,20 @@
       <c r="Q83" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:23" ht="16" customHeight="1">
+      <c r="R83" s="28">
+        <v>5.0350000000000004E-4</v>
+      </c>
+      <c r="S83" s="28">
+        <v>4.7010000000000003E-3</v>
+      </c>
+      <c r="T83" s="28">
+        <v>5.8929999999999998E-3</v>
+      </c>
+      <c r="AE83" s="28"/>
+      <c r="AF83" s="28"/>
+      <c r="AG83" s="28"/>
+    </row>
+    <row r="84" spans="1:33" ht="16" customHeight="1">
       <c r="A84" s="3">
         <v>42731</v>
       </c>
@@ -6907,8 +7418,20 @@
       <c r="Q84" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:23" ht="16" customHeight="1">
+      <c r="R84" s="28">
+        <v>5.9029999999999998E-4</v>
+      </c>
+      <c r="S84" s="28">
+        <v>1.0690000000000001E-3</v>
+      </c>
+      <c r="T84" s="28">
+        <v>4.7569999999999999E-3</v>
+      </c>
+      <c r="AE84" s="28"/>
+      <c r="AF84" s="28"/>
+      <c r="AG84" s="28"/>
+    </row>
+    <row r="85" spans="1:33" ht="16" customHeight="1">
       <c r="A85" s="3">
         <v>42731</v>
       </c>
@@ -6958,8 +7481,23 @@
       <c r="Q85" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:23" ht="16" customHeight="1">
+      <c r="R85" s="28">
+        <v>7.7890000000000001E-4</v>
+      </c>
+      <c r="S85" s="28">
+        <v>5.4180000000000001E-3</v>
+      </c>
+      <c r="T85" s="28">
+        <v>4.9800000000000001E-3</v>
+      </c>
+      <c r="AC85" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE85" s="28"/>
+      <c r="AF85" s="28"/>
+      <c r="AG85" s="28"/>
+    </row>
+    <row r="86" spans="1:33" ht="16" customHeight="1">
       <c r="A86" s="3">
         <v>42732</v>
       </c>
@@ -7009,8 +7547,17 @@
       <c r="Q86" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="87" spans="1:23" ht="16" customHeight="1">
+      <c r="R86" s="28">
+        <v>1.0139999999999999E-3</v>
+      </c>
+      <c r="S86" s="28">
+        <v>5.4489999999999999E-3</v>
+      </c>
+      <c r="T86" s="28">
+        <v>5.8279999999999998E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:33" ht="16" customHeight="1">
       <c r="A87" s="3">
         <v>42732</v>
       </c>
@@ -7060,11 +7607,20 @@
       <c r="Q87" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="R87" s="28">
+        <v>5.1730000000000005E-4</v>
+      </c>
+      <c r="S87" s="28">
+        <v>3.2989999999999998E-3</v>
+      </c>
+      <c r="T87" s="28">
+        <v>4.6860000000000001E-3</v>
+      </c>
       <c r="U87" s="20"/>
       <c r="V87" s="20"/>
       <c r="W87" s="13"/>
     </row>
-    <row r="88" spans="1:23" ht="16" customHeight="1">
+    <row r="88" spans="1:33" ht="16" customHeight="1">
       <c r="A88" s="3">
         <v>42732</v>
       </c>
@@ -7114,8 +7670,17 @@
       <c r="Q88" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="89" spans="1:23" ht="16" customHeight="1">
+      <c r="R88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S88" s="28">
+        <v>2.5300000000000001E-3</v>
+      </c>
+      <c r="T88" s="28">
+        <v>2.6259999999999999E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:33" ht="16" customHeight="1">
       <c r="A89" s="3">
         <v>42732</v>
       </c>
@@ -7165,8 +7730,17 @@
       <c r="Q89" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="90" spans="1:23" ht="16" customHeight="1">
+      <c r="R89" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S89" s="28">
+        <v>2.5119999999999999E-3</v>
+      </c>
+      <c r="T89" s="28">
+        <v>2.6389999999999999E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:33" ht="16" customHeight="1">
       <c r="A90" s="3">
         <v>42732</v>
       </c>
@@ -7216,8 +7790,17 @@
       <c r="Q90" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="91" spans="1:23" ht="16" customHeight="1">
+      <c r="R90" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S90" s="28">
+        <v>3.2399999999999998E-3</v>
+      </c>
+      <c r="T90" s="28">
+        <v>2.3939999999999999E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:33" ht="16" customHeight="1">
       <c r="A91" s="3">
         <v>42732</v>
       </c>
@@ -7267,8 +7850,17 @@
       <c r="Q91" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="92" spans="1:23" ht="16" customHeight="1">
+      <c r="R91" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S91" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T91" s="28">
+        <v>2.4220000000000001E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:33" ht="16" customHeight="1">
       <c r="A92" s="3">
         <v>42732</v>
       </c>
@@ -7319,7 +7911,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="16" customHeight="1">
+    <row r="93" spans="1:33" ht="16" customHeight="1">
       <c r="A93" s="3">
         <v>42732</v>
       </c>
@@ -7370,7 +7962,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="16" customHeight="1">
+    <row r="94" spans="1:33" ht="16" customHeight="1">
       <c r="A94" s="3">
         <v>42732</v>
       </c>
@@ -7421,7 +8013,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="16" customHeight="1">
+    <row r="95" spans="1:33" ht="16" customHeight="1">
       <c r="A95" s="3">
         <v>42732</v>
       </c>
@@ -7472,7 +8064,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="16" customHeight="1">
+    <row r="96" spans="1:33" ht="16" customHeight="1">
       <c r="A96" s="3">
         <v>42732</v>
       </c>
@@ -67044,11 +67636,23 @@
       <c r="F1272" t="s">
         <v>56</v>
       </c>
+      <c r="G1272" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1272" s="16">
+        <v>18.529</v>
+      </c>
+      <c r="I1272" s="16">
+        <v>19.53</v>
+      </c>
       <c r="J1272">
         <v>1</v>
       </c>
       <c r="K1272" s="1">
         <v>1</v>
+      </c>
+      <c r="L1272" s="1">
+        <v>24</v>
       </c>
       <c r="Q1272" s="7" t="s">
         <v>66</v>
@@ -67073,11 +67677,23 @@
       <c r="F1273" t="s">
         <v>58</v>
       </c>
+      <c r="G1273" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1273" s="16">
+        <v>17.837</v>
+      </c>
+      <c r="I1273" s="16">
+        <v>18.207999999999998</v>
+      </c>
       <c r="J1273">
         <v>1</v>
       </c>
       <c r="K1273" s="1">
         <v>1</v>
+      </c>
+      <c r="L1273" s="1">
+        <v>24</v>
       </c>
       <c r="Q1273" s="7" t="s">
         <v>67</v>
@@ -67102,11 +67718,23 @@
       <c r="F1274" t="s">
         <v>28</v>
       </c>
+      <c r="G1274" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1274" s="16">
+        <v>17.681999999999999</v>
+      </c>
+      <c r="I1274" s="16">
+        <v>18.844999999999999</v>
+      </c>
       <c r="J1274">
         <v>1</v>
       </c>
       <c r="K1274" s="1">
         <v>1</v>
+      </c>
+      <c r="L1274" s="1">
+        <v>24</v>
       </c>
       <c r="Q1274" s="7" t="s">
         <v>68</v>
@@ -67131,11 +67759,23 @@
       <c r="F1275" t="s">
         <v>30</v>
       </c>
+      <c r="G1275" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1275" s="16">
+        <v>17.847000000000001</v>
+      </c>
+      <c r="I1275" s="16">
+        <v>18.998999999999999</v>
+      </c>
       <c r="J1275">
         <v>1</v>
       </c>
       <c r="K1275" s="1">
         <v>1</v>
+      </c>
+      <c r="L1275" s="1">
+        <v>24</v>
       </c>
       <c r="Q1275" s="7" t="s">
         <v>69</v>
@@ -67160,11 +67800,23 @@
       <c r="F1276" t="s">
         <v>46</v>
       </c>
+      <c r="G1276" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1276" s="16">
+        <v>18.119</v>
+      </c>
+      <c r="I1276" s="16">
+        <v>19.367999999999999</v>
+      </c>
       <c r="J1276">
         <v>1</v>
       </c>
       <c r="K1276" s="1">
         <v>1</v>
+      </c>
+      <c r="L1276" s="1">
+        <v>24</v>
       </c>
       <c r="Q1276" s="7" t="s">
         <v>70</v>
@@ -67189,11 +67841,23 @@
       <c r="F1277" t="s">
         <v>54</v>
       </c>
+      <c r="G1277" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1277" s="16">
+        <v>18.164000000000001</v>
+      </c>
+      <c r="I1277" s="16">
+        <v>19.408000000000001</v>
+      </c>
       <c r="J1277">
         <v>1</v>
       </c>
       <c r="K1277" s="1">
         <v>1</v>
+      </c>
+      <c r="L1277" s="1">
+        <v>24</v>
       </c>
       <c r="Q1277" s="7" t="s">
         <v>71</v>
@@ -67218,11 +67882,23 @@
       <c r="F1278" t="s">
         <v>36</v>
       </c>
+      <c r="G1278" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1278" s="16">
+        <v>17.841000000000001</v>
+      </c>
+      <c r="I1278" s="16">
+        <v>19.058</v>
+      </c>
       <c r="J1278">
         <v>1</v>
       </c>
       <c r="K1278" s="1">
         <v>1</v>
+      </c>
+      <c r="L1278" s="1">
+        <v>24</v>
       </c>
       <c r="Q1278" s="7" t="s">
         <v>72</v>
@@ -67247,11 +67923,23 @@
       <c r="F1279" t="s">
         <v>52</v>
       </c>
+      <c r="G1279" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="H1279" s="16">
+        <v>18.123000000000001</v>
+      </c>
+      <c r="I1279" s="16">
+        <v>19.391999999999999</v>
+      </c>
       <c r="J1279">
         <v>1</v>
       </c>
       <c r="K1279" s="1">
         <v>1</v>
+      </c>
+      <c r="L1279" s="1">
+        <v>24</v>
       </c>
       <c r="Q1279" s="7" t="s">
         <v>73</v>
@@ -67276,11 +67964,23 @@
       <c r="F1280" t="s">
         <v>40</v>
       </c>
+      <c r="G1280" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1280" s="16">
+        <v>18.323</v>
+      </c>
+      <c r="I1280" s="16">
+        <v>19.7</v>
+      </c>
       <c r="J1280">
         <v>1</v>
       </c>
       <c r="K1280" s="1">
         <v>1</v>
+      </c>
+      <c r="L1280" s="1">
+        <v>24</v>
       </c>
       <c r="Q1280" s="7" t="s">
         <v>74</v>
@@ -67305,11 +68005,23 @@
       <c r="F1281" t="s">
         <v>26</v>
       </c>
+      <c r="G1281" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1281" s="16">
+        <v>18.102</v>
+      </c>
+      <c r="I1281" s="16">
+        <v>19.463000000000001</v>
+      </c>
       <c r="J1281">
         <v>1</v>
       </c>
       <c r="K1281" s="1">
         <v>1</v>
+      </c>
+      <c r="L1281" s="1">
+        <v>24</v>
       </c>
       <c r="Q1281" s="7" t="s">
         <v>75</v>
@@ -67334,11 +68046,23 @@
       <c r="F1282" t="s">
         <v>24</v>
       </c>
+      <c r="G1282" s="1">
+        <v>28</v>
+      </c>
+      <c r="H1282" s="16">
+        <v>17.713999999999999</v>
+      </c>
+      <c r="I1282" s="16">
+        <v>18.983000000000001</v>
+      </c>
       <c r="J1282">
         <v>2</v>
       </c>
       <c r="K1282" s="1">
         <v>1</v>
+      </c>
+      <c r="L1282" s="1">
+        <v>32</v>
       </c>
       <c r="Q1282" s="7" t="s">
         <v>76</v>
@@ -67363,11 +68087,23 @@
       <c r="F1283" t="s">
         <v>62</v>
       </c>
+      <c r="G1283" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1283" s="16">
+        <v>17.984000000000002</v>
+      </c>
+      <c r="I1283" s="16">
+        <v>19.100999999999999</v>
+      </c>
       <c r="J1283">
         <v>2</v>
       </c>
       <c r="K1283" s="1">
         <v>1</v>
+      </c>
+      <c r="L1283" s="1">
+        <v>32</v>
       </c>
       <c r="Q1283" s="7" t="s">
         <v>77</v>
@@ -67392,11 +68128,23 @@
       <c r="F1284" t="s">
         <v>44</v>
       </c>
+      <c r="G1284" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1284" s="16">
+        <v>18.201000000000001</v>
+      </c>
+      <c r="I1284" s="16">
+        <v>19.332999999999998</v>
+      </c>
       <c r="J1284">
         <v>2</v>
       </c>
       <c r="K1284" s="1">
         <v>1</v>
+      </c>
+      <c r="L1284" s="1">
+        <v>32</v>
       </c>
       <c r="Q1284" s="7" t="s">
         <v>78</v>
@@ -67421,11 +68169,23 @@
       <c r="F1285" t="s">
         <v>42</v>
       </c>
+      <c r="G1285" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1285" s="16">
+        <v>18.315999999999999</v>
+      </c>
+      <c r="I1285" s="16">
+        <v>19.442</v>
+      </c>
       <c r="J1285">
         <v>2</v>
       </c>
       <c r="K1285" s="1">
         <v>1</v>
+      </c>
+      <c r="L1285" s="1">
+        <v>32</v>
       </c>
       <c r="Q1285" s="7" t="s">
         <v>79</v>
@@ -67450,11 +68210,23 @@
       <c r="F1286" t="s">
         <v>50</v>
       </c>
+      <c r="G1286" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1286" s="16">
+        <v>18.103000000000002</v>
+      </c>
+      <c r="I1286" s="16">
+        <v>19.228999999999999</v>
+      </c>
       <c r="J1286">
         <v>2</v>
       </c>
       <c r="K1286" s="1">
         <v>1</v>
+      </c>
+      <c r="L1286" s="1">
+        <v>32</v>
       </c>
       <c r="Q1286" s="7" t="s">
         <v>80</v>
@@ -67479,11 +68251,23 @@
       <c r="F1287" t="s">
         <v>32</v>
       </c>
+      <c r="G1287" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1287" s="16">
+        <v>18.178999999999998</v>
+      </c>
+      <c r="I1287" s="16">
+        <v>19.408999999999999</v>
+      </c>
       <c r="J1287">
         <v>2</v>
       </c>
       <c r="K1287" s="1">
         <v>1</v>
+      </c>
+      <c r="L1287" s="1">
+        <v>32</v>
       </c>
       <c r="Q1287" s="7" t="s">
         <v>81</v>
@@ -67508,11 +68292,23 @@
       <c r="F1288" t="s">
         <v>48</v>
       </c>
+      <c r="G1288" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1288" s="16">
+        <v>18.042000000000002</v>
+      </c>
+      <c r="I1288" s="16">
+        <v>19.355</v>
+      </c>
       <c r="J1288">
         <v>2</v>
       </c>
       <c r="K1288" s="1">
         <v>1</v>
+      </c>
+      <c r="L1288" s="1">
+        <v>32</v>
       </c>
       <c r="Q1288" s="7" t="s">
         <v>86</v>
@@ -67537,11 +68333,23 @@
       <c r="F1289" t="s">
         <v>60</v>
       </c>
+      <c r="G1289" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1289" s="16">
+        <v>18.077000000000002</v>
+      </c>
+      <c r="I1289" s="16">
+        <v>19.439</v>
+      </c>
       <c r="J1289">
         <v>2</v>
       </c>
       <c r="K1289" s="1">
         <v>1</v>
+      </c>
+      <c r="L1289" s="1">
+        <v>32</v>
       </c>
       <c r="Q1289" s="7" t="s">
         <v>85</v>
@@ -67566,11 +68374,23 @@
       <c r="F1290" t="s">
         <v>64</v>
       </c>
+      <c r="G1290" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1290" s="16">
+        <v>17.972999999999999</v>
+      </c>
+      <c r="I1290" s="16">
+        <v>19.155999999999999</v>
+      </c>
       <c r="J1290">
         <v>2</v>
       </c>
       <c r="K1290" s="1">
         <v>1</v>
+      </c>
+      <c r="L1290" s="1">
+        <v>32</v>
       </c>
       <c r="Q1290" s="7" t="s">
         <v>82</v>
@@ -67595,11 +68415,23 @@
       <c r="F1291" t="s">
         <v>34</v>
       </c>
+      <c r="G1291" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1291" s="16">
+        <v>18.192</v>
+      </c>
+      <c r="I1291" s="16">
+        <v>19.327999999999999</v>
+      </c>
       <c r="J1291">
         <v>2</v>
       </c>
       <c r="K1291" s="1">
         <v>1</v>
+      </c>
+      <c r="L1291" s="1">
+        <v>32</v>
       </c>
       <c r="Q1291" s="7" t="s">
         <v>83</v>
@@ -67624,11 +68456,23 @@
       <c r="F1292" t="s">
         <v>38</v>
       </c>
+      <c r="G1292" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1292" s="16">
+        <v>18.134</v>
+      </c>
+      <c r="I1292" s="16">
+        <v>19.478000000000002</v>
+      </c>
       <c r="J1292">
         <v>2</v>
       </c>
       <c r="K1292" s="1">
         <v>1</v>
+      </c>
+      <c r="L1292" s="1">
+        <v>32</v>
       </c>
       <c r="Q1292" s="7" t="s">
         <v>84</v>
@@ -67653,11 +68497,23 @@
       <c r="F1293" t="s">
         <v>56</v>
       </c>
+      <c r="G1293" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1293" s="16">
+        <v>18.529</v>
+      </c>
+      <c r="I1293" s="16">
+        <v>19.53</v>
+      </c>
       <c r="J1293">
         <v>1</v>
       </c>
       <c r="K1293" s="1">
         <v>2</v>
+      </c>
+      <c r="L1293" s="1">
+        <v>26</v>
       </c>
       <c r="Q1293" s="7" t="s">
         <v>66</v>
@@ -67682,11 +68538,23 @@
       <c r="F1294" t="s">
         <v>58</v>
       </c>
+      <c r="G1294" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1294" s="16">
+        <v>17.837</v>
+      </c>
+      <c r="I1294" s="16">
+        <v>18.207999999999998</v>
+      </c>
       <c r="J1294">
         <v>1</v>
       </c>
       <c r="K1294" s="1">
         <v>2</v>
+      </c>
+      <c r="L1294" s="1">
+        <v>26</v>
       </c>
       <c r="Q1294" s="7" t="s">
         <v>67</v>
@@ -67711,11 +68579,23 @@
       <c r="F1295" t="s">
         <v>28</v>
       </c>
+      <c r="G1295" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1295" s="16">
+        <v>17.681999999999999</v>
+      </c>
+      <c r="I1295" s="16">
+        <v>18.844999999999999</v>
+      </c>
       <c r="J1295">
         <v>1</v>
       </c>
       <c r="K1295" s="1">
         <v>2</v>
+      </c>
+      <c r="L1295" s="1">
+        <v>26</v>
       </c>
       <c r="Q1295" s="7" t="s">
         <v>68</v>
@@ -67740,11 +68620,23 @@
       <c r="F1296" t="s">
         <v>30</v>
       </c>
+      <c r="G1296" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1296" s="16">
+        <v>17.847000000000001</v>
+      </c>
+      <c r="I1296" s="16">
+        <v>18.998999999999999</v>
+      </c>
       <c r="J1296">
         <v>1</v>
       </c>
       <c r="K1296" s="1">
         <v>2</v>
+      </c>
+      <c r="L1296" s="1">
+        <v>26</v>
       </c>
       <c r="Q1296" s="7" t="s">
         <v>69</v>
@@ -67769,11 +68661,23 @@
       <c r="F1297" t="s">
         <v>46</v>
       </c>
+      <c r="G1297" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1297" s="16">
+        <v>18.119</v>
+      </c>
+      <c r="I1297" s="16">
+        <v>19.367999999999999</v>
+      </c>
       <c r="J1297">
         <v>1</v>
       </c>
       <c r="K1297" s="1">
         <v>2</v>
+      </c>
+      <c r="L1297" s="1">
+        <v>26</v>
       </c>
       <c r="Q1297" s="7" t="s">
         <v>70</v>
@@ -67798,11 +68702,23 @@
       <c r="F1298" t="s">
         <v>54</v>
       </c>
+      <c r="G1298" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1298" s="16">
+        <v>18.164000000000001</v>
+      </c>
+      <c r="I1298" s="16">
+        <v>19.408000000000001</v>
+      </c>
       <c r="J1298">
         <v>1</v>
       </c>
       <c r="K1298" s="1">
         <v>2</v>
+      </c>
+      <c r="L1298" s="1">
+        <v>26</v>
       </c>
       <c r="Q1298" s="7" t="s">
         <v>71</v>
@@ -67827,11 +68743,23 @@
       <c r="F1299" t="s">
         <v>36</v>
       </c>
+      <c r="G1299" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1299" s="16">
+        <v>17.841000000000001</v>
+      </c>
+      <c r="I1299" s="16">
+        <v>19.058</v>
+      </c>
       <c r="J1299">
         <v>1</v>
       </c>
       <c r="K1299" s="1">
         <v>2</v>
+      </c>
+      <c r="L1299" s="1">
+        <v>26</v>
       </c>
       <c r="Q1299" s="7" t="s">
         <v>72</v>
@@ -67856,11 +68784,23 @@
       <c r="F1300" t="s">
         <v>52</v>
       </c>
+      <c r="G1300" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="H1300" s="16">
+        <v>18.123000000000001</v>
+      </c>
+      <c r="I1300" s="16">
+        <v>19.391999999999999</v>
+      </c>
       <c r="J1300">
         <v>1</v>
       </c>
       <c r="K1300" s="1">
         <v>2</v>
+      </c>
+      <c r="L1300" s="1">
+        <v>26</v>
       </c>
       <c r="Q1300" s="7" t="s">
         <v>73</v>
@@ -67885,11 +68825,23 @@
       <c r="F1301" t="s">
         <v>40</v>
       </c>
+      <c r="G1301" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1301" s="16">
+        <v>18.323</v>
+      </c>
+      <c r="I1301" s="16">
+        <v>19.7</v>
+      </c>
       <c r="J1301">
         <v>1</v>
       </c>
       <c r="K1301" s="1">
         <v>2</v>
+      </c>
+      <c r="L1301" s="1">
+        <v>26</v>
       </c>
       <c r="Q1301" s="7" t="s">
         <v>74</v>
@@ -67914,11 +68866,23 @@
       <c r="F1302" t="s">
         <v>26</v>
       </c>
+      <c r="G1302" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1302" s="16">
+        <v>18.102</v>
+      </c>
+      <c r="I1302" s="16">
+        <v>19.463000000000001</v>
+      </c>
       <c r="J1302">
         <v>1</v>
       </c>
       <c r="K1302" s="1">
         <v>2</v>
+      </c>
+      <c r="L1302" s="1">
+        <v>26</v>
       </c>
       <c r="Q1302" s="7" t="s">
         <v>75</v>
@@ -67943,11 +68907,23 @@
       <c r="F1303" t="s">
         <v>24</v>
       </c>
+      <c r="G1303" s="1">
+        <v>28</v>
+      </c>
+      <c r="H1303" s="16">
+        <v>17.713999999999999</v>
+      </c>
+      <c r="I1303" s="16">
+        <v>18.983000000000001</v>
+      </c>
       <c r="J1303">
         <v>2</v>
       </c>
       <c r="K1303" s="1">
         <v>2</v>
+      </c>
+      <c r="L1303" s="1">
+        <v>30</v>
       </c>
       <c r="Q1303" s="7" t="s">
         <v>76</v>
@@ -67972,11 +68948,23 @@
       <c r="F1304" t="s">
         <v>62</v>
       </c>
+      <c r="G1304" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1304" s="16">
+        <v>17.984000000000002</v>
+      </c>
+      <c r="I1304" s="16">
+        <v>19.100999999999999</v>
+      </c>
       <c r="J1304">
         <v>2</v>
       </c>
       <c r="K1304" s="1">
         <v>2</v>
+      </c>
+      <c r="L1304" s="1">
+        <v>30</v>
       </c>
       <c r="Q1304" s="7" t="s">
         <v>77</v>
@@ -68001,11 +68989,23 @@
       <c r="F1305" t="s">
         <v>44</v>
       </c>
+      <c r="G1305" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1305" s="16">
+        <v>18.201000000000001</v>
+      </c>
+      <c r="I1305" s="16">
+        <v>19.332999999999998</v>
+      </c>
       <c r="J1305">
         <v>2</v>
       </c>
       <c r="K1305" s="1">
         <v>2</v>
+      </c>
+      <c r="L1305" s="1">
+        <v>30</v>
       </c>
       <c r="Q1305" s="7" t="s">
         <v>78</v>
@@ -68030,11 +69030,23 @@
       <c r="F1306" t="s">
         <v>42</v>
       </c>
+      <c r="G1306" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1306" s="16">
+        <v>18.315999999999999</v>
+      </c>
+      <c r="I1306" s="16">
+        <v>19.442</v>
+      </c>
       <c r="J1306">
         <v>2</v>
       </c>
       <c r="K1306" s="1">
         <v>2</v>
+      </c>
+      <c r="L1306" s="1">
+        <v>30</v>
       </c>
       <c r="Q1306" s="7" t="s">
         <v>79</v>
@@ -68059,11 +69071,23 @@
       <c r="F1307" t="s">
         <v>50</v>
       </c>
+      <c r="G1307" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1307" s="16">
+        <v>18.103000000000002</v>
+      </c>
+      <c r="I1307" s="16">
+        <v>19.228999999999999</v>
+      </c>
       <c r="J1307">
         <v>2</v>
       </c>
       <c r="K1307" s="1">
         <v>2</v>
+      </c>
+      <c r="L1307" s="1">
+        <v>30</v>
       </c>
       <c r="Q1307" s="7" t="s">
         <v>80</v>
@@ -68088,11 +69112,23 @@
       <c r="F1308" t="s">
         <v>32</v>
       </c>
+      <c r="G1308" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1308" s="16">
+        <v>18.178999999999998</v>
+      </c>
+      <c r="I1308" s="16">
+        <v>19.408999999999999</v>
+      </c>
       <c r="J1308">
         <v>2</v>
       </c>
       <c r="K1308" s="1">
         <v>2</v>
+      </c>
+      <c r="L1308" s="1">
+        <v>30</v>
       </c>
       <c r="Q1308" s="7" t="s">
         <v>81</v>
@@ -68117,11 +69153,23 @@
       <c r="F1309" t="s">
         <v>48</v>
       </c>
+      <c r="G1309" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1309" s="16">
+        <v>18.042000000000002</v>
+      </c>
+      <c r="I1309" s="16">
+        <v>19.355</v>
+      </c>
       <c r="J1309">
         <v>2</v>
       </c>
       <c r="K1309" s="1">
         <v>2</v>
+      </c>
+      <c r="L1309" s="1">
+        <v>30</v>
       </c>
       <c r="Q1309" s="7" t="s">
         <v>86</v>
@@ -68146,11 +69194,23 @@
       <c r="F1310" t="s">
         <v>60</v>
       </c>
+      <c r="G1310" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1310" s="16">
+        <v>18.077000000000002</v>
+      </c>
+      <c r="I1310" s="16">
+        <v>19.439</v>
+      </c>
       <c r="J1310">
         <v>2</v>
       </c>
       <c r="K1310" s="1">
         <v>2</v>
+      </c>
+      <c r="L1310" s="1">
+        <v>30</v>
       </c>
       <c r="Q1310" s="7" t="s">
         <v>85</v>
@@ -68175,11 +69235,23 @@
       <c r="F1311" t="s">
         <v>64</v>
       </c>
+      <c r="G1311" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1311" s="16">
+        <v>17.972999999999999</v>
+      </c>
+      <c r="I1311" s="16">
+        <v>19.155999999999999</v>
+      </c>
       <c r="J1311">
         <v>2</v>
       </c>
       <c r="K1311" s="1">
         <v>2</v>
+      </c>
+      <c r="L1311" s="1">
+        <v>30</v>
       </c>
       <c r="Q1311" s="7" t="s">
         <v>82</v>
@@ -68204,11 +69276,23 @@
       <c r="F1312" t="s">
         <v>34</v>
       </c>
+      <c r="G1312" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1312" s="16">
+        <v>18.192</v>
+      </c>
+      <c r="I1312" s="16">
+        <v>19.327999999999999</v>
+      </c>
       <c r="J1312">
         <v>2</v>
       </c>
       <c r="K1312" s="1">
         <v>2</v>
+      </c>
+      <c r="L1312" s="1">
+        <v>30</v>
       </c>
       <c r="Q1312" s="7" t="s">
         <v>83</v>
@@ -68233,11 +69317,23 @@
       <c r="F1313" t="s">
         <v>38</v>
       </c>
+      <c r="G1313" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1313" s="16">
+        <v>18.134</v>
+      </c>
+      <c r="I1313" s="16">
+        <v>19.478000000000002</v>
+      </c>
       <c r="J1313">
         <v>2</v>
       </c>
       <c r="K1313" s="1">
         <v>2</v>
+      </c>
+      <c r="L1313" s="1">
+        <v>30</v>
       </c>
       <c r="Q1313" s="7" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
integrated 25.1.17 both temps
</commit_message>
<xml_diff>
--- a/data/ldeli_integrate.xlsx
+++ b/data/ldeli_integrate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="7680" windowWidth="25280" windowHeight="9540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5432" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5475" uniqueCount="174">
   <si>
     <t>date</t>
   </si>
@@ -534,6 +534,15 @@
   <si>
     <t>DoublePO2BL</t>
   </si>
+  <si>
+    <t>NegCO2BL</t>
+  </si>
+  <si>
+    <t>NegCO2BL, NoPCO2T2</t>
+  </si>
+  <si>
+    <t>MultiPCO2BL</t>
+  </si>
 </sst>
 </file>
 
@@ -629,11 +638,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="574">
+  <cellStyleXfs count="584">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1290,7 +1309,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="574">
+  <cellStyles count="584">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1579,6 +1598,11 @@
     <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -1864,6 +1888,11 @@
     <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2195,9 +2224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1302" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1314" sqref="G1314"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1308" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T1313" sqref="T1313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -67303,7 +67332,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="1265" spans="1:17" ht="16" customHeight="1">
+    <row r="1265" spans="1:28" ht="16" customHeight="1">
       <c r="A1265" s="3">
         <v>42753</v>
       </c>
@@ -67354,7 +67383,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="1266" spans="1:17" ht="16" customHeight="1">
+    <row r="1266" spans="1:28" ht="16" customHeight="1">
       <c r="A1266" s="3">
         <v>42753</v>
       </c>
@@ -67405,7 +67434,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="1267" spans="1:17" ht="16" customHeight="1">
+    <row r="1267" spans="1:28" ht="16" customHeight="1">
       <c r="A1267" s="3">
         <v>42753</v>
       </c>
@@ -67456,7 +67485,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="1268" spans="1:17" ht="16" customHeight="1">
+    <row r="1268" spans="1:28" ht="16" customHeight="1">
       <c r="A1268" s="3">
         <v>42753</v>
       </c>
@@ -67507,7 +67536,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="1269" spans="1:17" ht="16" customHeight="1">
+    <row r="1269" spans="1:28" ht="16" customHeight="1">
       <c r="A1269" s="3">
         <v>42753</v>
       </c>
@@ -67558,7 +67587,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="1270" spans="1:17" ht="16" customHeight="1">
+    <row r="1270" spans="1:28" ht="16" customHeight="1">
       <c r="A1270" s="3">
         <v>42753</v>
       </c>
@@ -67609,7 +67638,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="1271" spans="1:17" s="14" customFormat="1" ht="16" customHeight="1">
+    <row r="1271" spans="1:28" s="14" customFormat="1" ht="16" customHeight="1">
       <c r="H1271" s="17"/>
       <c r="I1271" s="17"/>
       <c r="M1271" s="19"/>
@@ -67617,7 +67646,7 @@
       <c r="O1271" s="15"/>
       <c r="P1271" s="15"/>
     </row>
-    <row r="1272" spans="1:17" ht="16" customHeight="1">
+    <row r="1272" spans="1:28" ht="16" customHeight="1">
       <c r="A1272" s="3">
         <v>42760</v>
       </c>
@@ -67657,8 +67686,17 @@
       <c r="Q1272" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="1273" spans="1:17" ht="16" customHeight="1">
+      <c r="R1272" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1272" s="28">
+        <v>1.0480000000000001E-3</v>
+      </c>
+      <c r="T1272" s="28">
+        <v>1.4909999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:28" ht="16" customHeight="1">
       <c r="A1273" s="3">
         <v>42760</v>
       </c>
@@ -67698,8 +67736,17 @@
       <c r="Q1273" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="1274" spans="1:17" ht="16" customHeight="1">
+      <c r="R1273" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1273" s="28">
+        <v>1.139E-3</v>
+      </c>
+      <c r="T1273" s="28">
+        <v>1.524E-3</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:28" ht="16" customHeight="1">
       <c r="A1274" s="3">
         <v>42760</v>
       </c>
@@ -67739,8 +67786,17 @@
       <c r="Q1274" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="1275" spans="1:17" ht="16" customHeight="1">
+      <c r="R1274" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1274" s="28">
+        <v>1.395E-3</v>
+      </c>
+      <c r="T1274" s="28">
+        <v>1.42E-3</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:28" ht="16" customHeight="1">
       <c r="A1275" s="3">
         <v>42760</v>
       </c>
@@ -67780,8 +67836,20 @@
       <c r="Q1275" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="1276" spans="1:17" ht="16" customHeight="1">
+      <c r="R1275" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1275" s="28">
+        <v>1.3079999999999999E-3</v>
+      </c>
+      <c r="T1275" s="28">
+        <v>2.042E-3</v>
+      </c>
+      <c r="AB1275" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:28" ht="16" customHeight="1">
       <c r="A1276" s="3">
         <v>42760</v>
       </c>
@@ -67821,8 +67889,20 @@
       <c r="Q1276" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="1277" spans="1:17" ht="16" customHeight="1">
+      <c r="R1276" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1276" s="28">
+        <v>1.6449999999999999E-4</v>
+      </c>
+      <c r="T1276" s="28">
+        <v>1.1709999999999999E-3</v>
+      </c>
+      <c r="AB1276" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:28" ht="16" customHeight="1">
       <c r="A1277" s="3">
         <v>42760</v>
       </c>
@@ -67862,8 +67942,20 @@
       <c r="Q1277" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="1278" spans="1:17" ht="16" customHeight="1">
+      <c r="R1277" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1277" s="28">
+        <v>1.4109999999999999E-3</v>
+      </c>
+      <c r="T1277" s="28">
+        <v>1.531E-3</v>
+      </c>
+      <c r="AB1277" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:28" ht="16" customHeight="1">
       <c r="A1278" s="3">
         <v>42760</v>
       </c>
@@ -67903,8 +67995,20 @@
       <c r="Q1278" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="1279" spans="1:17" ht="16" customHeight="1">
+      <c r="R1278" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1278" s="28">
+        <v>1.6019999999999999E-3</v>
+      </c>
+      <c r="T1278" s="28">
+        <v>1.4270000000000001E-3</v>
+      </c>
+      <c r="AB1278" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:28" ht="16" customHeight="1">
       <c r="A1279" s="3">
         <v>42760</v>
       </c>
@@ -67944,8 +68048,20 @@
       <c r="Q1279" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="1280" spans="1:17" ht="16" customHeight="1">
+      <c r="R1279" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1279" s="28">
+        <v>9.8079999999999999E-4</v>
+      </c>
+      <c r="T1279" s="28">
+        <v>1.2930000000000001E-3</v>
+      </c>
+      <c r="AB1279" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:28" ht="16" customHeight="1">
       <c r="A1280" s="3">
         <v>42760</v>
       </c>
@@ -67985,8 +68101,20 @@
       <c r="Q1280" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="1281" spans="1:17" ht="16" customHeight="1">
+      <c r="R1280" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1280" s="28">
+        <v>1.3090000000000001E-3</v>
+      </c>
+      <c r="T1280" s="28">
+        <v>7.2300000000000001E-4</v>
+      </c>
+      <c r="AB1280" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:28" ht="16" customHeight="1">
       <c r="A1281" s="3">
         <v>42760</v>
       </c>
@@ -68026,8 +68154,20 @@
       <c r="Q1281" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1282" spans="1:17" ht="16" customHeight="1">
+      <c r="R1281" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1281" s="28">
+        <v>1.101E-3</v>
+      </c>
+      <c r="T1281" s="28">
+        <v>2.836E-3</v>
+      </c>
+      <c r="AB1281" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:28" ht="16" customHeight="1">
       <c r="A1282" s="3">
         <v>42760</v>
       </c>
@@ -68067,8 +68207,17 @@
       <c r="Q1282" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="1283" spans="1:17" ht="16" customHeight="1">
+      <c r="R1282" s="28">
+        <v>2.6509999999999999E-4</v>
+      </c>
+      <c r="S1282" s="1">
+        <v>1.33218E-2</v>
+      </c>
+      <c r="T1282" s="28">
+        <v>2.4399999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:28" ht="16" customHeight="1">
       <c r="A1283" s="3">
         <v>42760</v>
       </c>
@@ -68108,8 +68257,17 @@
       <c r="Q1283" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="1284" spans="1:17" ht="16" customHeight="1">
+      <c r="R1283" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1283" s="28">
+        <v>6.2919999999999998E-3</v>
+      </c>
+      <c r="T1283" s="28">
+        <v>6.4260000000000003E-3</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:28" ht="16" customHeight="1">
       <c r="A1284" s="3">
         <v>42760</v>
       </c>
@@ -68149,8 +68307,17 @@
       <c r="Q1284" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="1285" spans="1:17" ht="16" customHeight="1">
+      <c r="R1284" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1284" s="28">
+        <v>2.9819999999999998E-3</v>
+      </c>
+      <c r="T1284" s="28">
+        <v>3.6180000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:28" ht="16" customHeight="1">
       <c r="A1285" s="3">
         <v>42760</v>
       </c>
@@ -68190,8 +68357,17 @@
       <c r="Q1285" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="1286" spans="1:17" ht="16" customHeight="1">
+      <c r="R1285" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1285" s="28">
+        <v>3.2299999999999998E-3</v>
+      </c>
+      <c r="T1285" s="28">
+        <v>5.3489999999999996E-3</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:28" ht="16" customHeight="1">
       <c r="A1286" s="3">
         <v>42760</v>
       </c>
@@ -68231,8 +68407,17 @@
       <c r="Q1286" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1287" spans="1:17" ht="16" customHeight="1">
+      <c r="R1286" s="28">
+        <v>6.7549999999999999E-4</v>
+      </c>
+      <c r="S1286" s="1">
+        <v>1.3783399999999999E-2</v>
+      </c>
+      <c r="T1286" s="1">
+        <v>1.2678699999999999E-2</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:28" ht="16" customHeight="1">
       <c r="A1287" s="3">
         <v>42760</v>
       </c>
@@ -68272,8 +68457,17 @@
       <c r="Q1287" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="1288" spans="1:17" ht="16" customHeight="1">
+      <c r="R1287" s="28">
+        <v>3.2539999999999999E-4</v>
+      </c>
+      <c r="S1287" s="28">
+        <v>4.3480000000000003E-3</v>
+      </c>
+      <c r="T1287" s="28">
+        <v>3.5300000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:28" ht="16" customHeight="1">
       <c r="A1288" s="3">
         <v>42760</v>
       </c>
@@ -68313,8 +68507,17 @@
       <c r="Q1288" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="1289" spans="1:17" ht="16" customHeight="1">
+      <c r="R1288" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1288" s="28">
+        <v>4.8219999999999999E-3</v>
+      </c>
+      <c r="T1288" s="28">
+        <v>3.2759999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:28" ht="16" customHeight="1">
       <c r="A1289" s="3">
         <v>42760</v>
       </c>
@@ -68354,8 +68557,17 @@
       <c r="Q1289" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="1290" spans="1:17" ht="16" customHeight="1">
+      <c r="R1289" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1289" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1289" s="28">
+        <v>4.9849999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:28" ht="16" customHeight="1">
       <c r="A1290" s="3">
         <v>42760</v>
       </c>
@@ -68395,8 +68607,17 @@
       <c r="Q1290" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="1291" spans="1:17" ht="16" customHeight="1">
+      <c r="R1290" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1290" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1290" s="28">
+        <v>6.3280000000000003E-3</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:28" ht="16" customHeight="1">
       <c r="A1291" s="3">
         <v>42760</v>
       </c>
@@ -68436,8 +68657,17 @@
       <c r="Q1291" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="1292" spans="1:17" ht="16" customHeight="1">
+      <c r="R1291" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1291" s="28">
+        <v>4.6410000000000002E-3</v>
+      </c>
+      <c r="T1291" s="28">
+        <v>4.9100000000000003E-3</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:28" ht="16" customHeight="1">
       <c r="A1292" s="3">
         <v>42760</v>
       </c>
@@ -68477,8 +68707,20 @@
       <c r="Q1292" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="1293" spans="1:17" ht="16" customHeight="1">
+      <c r="R1292" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1292" s="28">
+        <v>5.365E-3</v>
+      </c>
+      <c r="T1292" s="28">
+        <v>3.8289999999999999E-3</v>
+      </c>
+      <c r="AB1292" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:28" ht="16" customHeight="1">
       <c r="A1293" s="3">
         <v>42760</v>
       </c>
@@ -68518,8 +68760,17 @@
       <c r="Q1293" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="1294" spans="1:17" ht="16" customHeight="1">
+      <c r="R1293" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1293" s="28">
+        <v>1.3879999999999999E-3</v>
+      </c>
+      <c r="T1293" s="28">
+        <v>2.0730000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:28" ht="16" customHeight="1">
       <c r="A1294" s="3">
         <v>42760</v>
       </c>
@@ -68559,8 +68810,17 @@
       <c r="Q1294" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="1295" spans="1:17" ht="16" customHeight="1">
+      <c r="R1294" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1294" s="28">
+        <v>4.5629999999999998E-4</v>
+      </c>
+      <c r="T1294" s="28">
+        <v>1.2459999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:28" ht="16" customHeight="1">
       <c r="A1295" s="3">
         <v>42760</v>
       </c>
@@ -68600,8 +68860,17 @@
       <c r="Q1295" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="1296" spans="1:17" ht="16" customHeight="1">
+      <c r="R1295" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1295" s="28">
+        <v>2.055E-3</v>
+      </c>
+      <c r="T1295" s="28">
+        <v>1.9170000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:28" ht="16" customHeight="1">
       <c r="A1296" s="3">
         <v>42760</v>
       </c>
@@ -68641,8 +68910,17 @@
       <c r="Q1296" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="1297" spans="1:17" ht="16" customHeight="1">
+      <c r="R1296" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1296" s="28">
+        <v>2.1879999999999998E-3</v>
+      </c>
+      <c r="T1296" s="28">
+        <v>2.5430000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:28" ht="16" customHeight="1">
       <c r="A1297" s="3">
         <v>42760</v>
       </c>
@@ -68682,8 +68960,17 @@
       <c r="Q1297" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="1298" spans="1:17" ht="16" customHeight="1">
+      <c r="R1297" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1297" s="28">
+        <v>2.4949999999999998E-3</v>
+      </c>
+      <c r="T1297" s="28">
+        <v>9.2170000000000001E-4</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:28" ht="16" customHeight="1">
       <c r="A1298" s="3">
         <v>42760</v>
       </c>
@@ -68723,8 +69010,17 @@
       <c r="Q1298" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="1299" spans="1:17" ht="16" customHeight="1">
+      <c r="R1298" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1298" s="28">
+        <v>5.2339999999999999E-3</v>
+      </c>
+      <c r="T1298" s="28">
+        <v>5.2090000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:28" ht="16" customHeight="1">
       <c r="A1299" s="3">
         <v>42760</v>
       </c>
@@ -68764,8 +69060,17 @@
       <c r="Q1299" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="1300" spans="1:17" ht="16" customHeight="1">
+      <c r="R1299" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1299" s="28">
+        <v>2.184E-4</v>
+      </c>
+      <c r="T1299" s="28">
+        <v>1.931E-3</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:28" ht="16" customHeight="1">
       <c r="A1300" s="3">
         <v>42760</v>
       </c>
@@ -68805,8 +69110,17 @@
       <c r="Q1300" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="1301" spans="1:17" ht="16" customHeight="1">
+      <c r="R1300" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1300" s="28">
+        <v>2.055E-3</v>
+      </c>
+      <c r="T1300" s="28">
+        <v>2.4160000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:28" ht="16" customHeight="1">
       <c r="A1301" s="3">
         <v>42760</v>
       </c>
@@ -68846,8 +69160,17 @@
       <c r="Q1301" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="1302" spans="1:17" ht="16" customHeight="1">
+      <c r="R1301" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1301" s="28">
+        <v>3.0899999999999999E-3</v>
+      </c>
+      <c r="T1301" s="28">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:28" ht="16" customHeight="1">
       <c r="A1302" s="3">
         <v>42760</v>
       </c>
@@ -68887,8 +69210,17 @@
       <c r="Q1302" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1303" spans="1:17" ht="16" customHeight="1">
+      <c r="R1302" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1302" s="1">
+        <v>8.3671000000000006E-3</v>
+      </c>
+      <c r="T1302" s="28">
+        <v>7.4409999999999997E-3</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:28" ht="16" customHeight="1">
       <c r="A1303" s="3">
         <v>42760</v>
       </c>
@@ -68928,8 +69260,17 @@
       <c r="Q1303" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="1304" spans="1:17" ht="16" customHeight="1">
+      <c r="R1303" s="28">
+        <v>3.7839999999999998E-4</v>
+      </c>
+      <c r="S1303" s="28">
+        <v>7.7070000000000003E-3</v>
+      </c>
+      <c r="T1303" s="1">
+        <v>8.0794999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:28" ht="16" customHeight="1">
       <c r="A1304" s="3">
         <v>42760</v>
       </c>
@@ -68969,8 +69310,17 @@
       <c r="Q1304" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="1305" spans="1:17" ht="16" customHeight="1">
+      <c r="R1304" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1304" s="28">
+        <v>6.2620000000000002E-3</v>
+      </c>
+      <c r="T1304" s="28">
+        <v>6.2839999999999997E-3</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:28" ht="16" customHeight="1">
       <c r="A1305" s="3">
         <v>42760</v>
       </c>
@@ -69010,8 +69360,17 @@
       <c r="Q1305" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="1306" spans="1:17" ht="16" customHeight="1">
+      <c r="R1305" s="28">
+        <v>1.8220000000000001E-4</v>
+      </c>
+      <c r="S1305" s="28">
+        <v>4.2649999999999997E-3</v>
+      </c>
+      <c r="T1305" s="28">
+        <v>4.431E-3</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:28" ht="16" customHeight="1">
       <c r="A1306" s="3">
         <v>42760</v>
       </c>
@@ -69051,8 +69410,17 @@
       <c r="Q1306" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="1307" spans="1:17" ht="16" customHeight="1">
+      <c r="R1306" s="28">
+        <v>5.1170000000000002E-4</v>
+      </c>
+      <c r="S1306" s="28">
+        <v>5.6600000000000001E-3</v>
+      </c>
+      <c r="T1306" s="28">
+        <v>5.9659999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:28" ht="16" customHeight="1">
       <c r="A1307" s="3">
         <v>42760</v>
       </c>
@@ -69092,8 +69460,17 @@
       <c r="Q1307" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1308" spans="1:17" ht="16" customHeight="1">
+      <c r="R1307" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1307" s="1">
+        <v>1.39116E-2</v>
+      </c>
+      <c r="T1307" s="28">
+        <v>4.3350000000000003E-3</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:28" ht="16" customHeight="1">
       <c r="A1308" s="3">
         <v>42760</v>
       </c>
@@ -69133,8 +69510,20 @@
       <c r="Q1308" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="1309" spans="1:17" ht="16" customHeight="1">
+      <c r="R1308" s="28">
+        <v>1.1349999999999999E-3</v>
+      </c>
+      <c r="S1308" s="28">
+        <v>6.221E-4</v>
+      </c>
+      <c r="T1308" s="28">
+        <v>4.9820000000000003E-3</v>
+      </c>
+      <c r="AB1308" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:28" ht="16" customHeight="1">
       <c r="A1309" s="3">
         <v>42760</v>
       </c>
@@ -69174,8 +69563,17 @@
       <c r="Q1309" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="1310" spans="1:17" ht="16" customHeight="1">
+      <c r="R1309" s="28">
+        <v>2.397E-4</v>
+      </c>
+      <c r="S1309" s="1">
+        <v>8.0672000000000001E-3</v>
+      </c>
+      <c r="T1309" s="1">
+        <v>8.6555999999999994E-3</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:28" ht="16" customHeight="1">
       <c r="A1310" s="3">
         <v>42760</v>
       </c>
@@ -69215,8 +69613,17 @@
       <c r="Q1310" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="1311" spans="1:17" ht="16" customHeight="1">
+      <c r="R1310" s="28">
+        <v>6.0780000000000003E-4</v>
+      </c>
+      <c r="S1310" s="28">
+        <v>5.2230000000000002E-3</v>
+      </c>
+      <c r="T1310" s="28">
+        <v>5.7219999999999997E-3</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:28" ht="16" customHeight="1">
       <c r="A1311" s="3">
         <v>42760</v>
       </c>
@@ -69256,8 +69663,17 @@
       <c r="Q1311" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="1312" spans="1:17" ht="16" customHeight="1">
+      <c r="R1311" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1311" s="28">
+        <v>6.0419999999999996E-3</v>
+      </c>
+      <c r="T1311" s="28">
+        <v>4.731E-3</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:28" ht="16" customHeight="1">
       <c r="A1312" s="3">
         <v>42760</v>
       </c>
@@ -69297,8 +69713,17 @@
       <c r="Q1312" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="1313" spans="1:17" ht="16" customHeight="1">
+      <c r="R1312" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1312" s="28">
+        <v>4.47E-3</v>
+      </c>
+      <c r="T1312" s="28">
+        <v>4.9069999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:20" ht="16" customHeight="1">
       <c r="A1313" s="3">
         <v>42760</v>
       </c>
@@ -69338,8 +69763,17 @@
       <c r="Q1313" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="1314" spans="1:17" ht="16" customHeight="1">
+      <c r="R1313" s="28">
+        <v>3.3940000000000001E-4</v>
+      </c>
+      <c r="S1313" s="28">
+        <v>3.885E-3</v>
+      </c>
+      <c r="T1313" s="28">
+        <v>4.2110000000000003E-3</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:20" ht="16" customHeight="1">
       <c r="A1314" s="3">
         <v>42761</v>
       </c>
@@ -69368,7 +69802,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1315" spans="1:17" ht="16" customHeight="1">
+    <row r="1315" spans="1:20" ht="16" customHeight="1">
       <c r="A1315" s="3">
         <v>42761</v>
       </c>
@@ -69397,7 +69831,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1316" spans="1:17" ht="16" customHeight="1">
+    <row r="1316" spans="1:20" ht="16" customHeight="1">
       <c r="A1316" s="3">
         <v>42761</v>
       </c>
@@ -69426,7 +69860,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="1317" spans="1:17" ht="16" customHeight="1">
+    <row r="1317" spans="1:20" ht="16" customHeight="1">
       <c r="A1317" s="3">
         <v>42761</v>
       </c>
@@ -69455,7 +69889,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="1318" spans="1:17" ht="16" customHeight="1">
+    <row r="1318" spans="1:20" ht="16" customHeight="1">
       <c r="A1318" s="3">
         <v>42761</v>
       </c>
@@ -69484,7 +69918,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="1319" spans="1:17" ht="16" customHeight="1">
+    <row r="1319" spans="1:20" ht="16" customHeight="1">
       <c r="A1319" s="3">
         <v>42761</v>
       </c>
@@ -69513,7 +69947,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="1320" spans="1:17" ht="16" customHeight="1">
+    <row r="1320" spans="1:20" ht="16" customHeight="1">
       <c r="A1320" s="3">
         <v>42761</v>
       </c>
@@ -69542,7 +69976,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="1321" spans="1:17" ht="16" customHeight="1">
+    <row r="1321" spans="1:20" ht="16" customHeight="1">
       <c r="A1321" s="3">
         <v>42761</v>
       </c>
@@ -69571,7 +70005,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="1322" spans="1:17" ht="16" customHeight="1">
+    <row r="1322" spans="1:20" ht="16" customHeight="1">
       <c r="A1322" s="3">
         <v>42761</v>
       </c>
@@ -69600,7 +70034,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="1323" spans="1:17" ht="16" customHeight="1">
+    <row r="1323" spans="1:20" ht="16" customHeight="1">
       <c r="A1323" s="3">
         <v>42761</v>
       </c>
@@ -69629,7 +70063,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="1324" spans="1:17" ht="16" customHeight="1">
+    <row r="1324" spans="1:20" ht="16" customHeight="1">
       <c r="A1324" s="3">
         <v>42761</v>
       </c>
@@ -69658,7 +70092,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="1325" spans="1:17" ht="16" customHeight="1">
+    <row r="1325" spans="1:20" ht="16" customHeight="1">
       <c r="A1325" s="3">
         <v>42761</v>
       </c>
@@ -69687,7 +70121,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="1326" spans="1:17" ht="16" customHeight="1">
+    <row r="1326" spans="1:20" ht="16" customHeight="1">
       <c r="A1326" s="3">
         <v>42761</v>
       </c>
@@ -69716,7 +70150,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="1327" spans="1:17" ht="16" customHeight="1">
+    <row r="1327" spans="1:20" ht="16" customHeight="1">
       <c r="A1327" s="3">
         <v>42761</v>
       </c>
@@ -69745,7 +70179,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="1328" spans="1:17" ht="16" customHeight="1">
+    <row r="1328" spans="1:20" ht="16" customHeight="1">
       <c r="A1328" s="3">
         <v>42761</v>
       </c>

</xml_diff>

<commit_message>
Entered general data for 27/1/17
</commit_message>
<xml_diff>
--- a/data/ldeli_integrate.xlsx
+++ b/data/ldeli_integrate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="7680" windowWidth="25280" windowHeight="9540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -638,11 +638,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="584">
+  <cellStyleXfs count="606">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1309,7 +1331,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="584">
+  <cellStyles count="606">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1603,6 +1625,17 @@
     <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -1893,6 +1926,17 @@
     <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2224,9 +2268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1308" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1313" sqref="T1313"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1331" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1345" sqref="N1345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -64673,7 +64717,7 @@
         <v>0.49652777777777773</v>
       </c>
       <c r="O1212" s="2">
-        <f t="shared" ref="O1212:O1270" si="21">N1212*1440-M1212*1440</f>
+        <f t="shared" ref="O1212:O1272" si="21">N1212*1440-M1212*1440</f>
         <v>90</v>
       </c>
       <c r="Q1212" s="7" t="s">
@@ -67683,6 +67727,16 @@
       <c r="L1272" s="1">
         <v>24</v>
       </c>
+      <c r="M1272" s="18">
+        <v>0.31805555555555554</v>
+      </c>
+      <c r="N1272" s="18">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="O1272" s="2">
+        <f>N1272*1440-M1272*1440</f>
+        <v>90</v>
+      </c>
       <c r="Q1272" s="7" t="s">
         <v>66</v>
       </c>
@@ -67733,6 +67787,16 @@
       <c r="L1273" s="1">
         <v>24</v>
       </c>
+      <c r="M1273" s="18">
+        <v>0.31875000000000003</v>
+      </c>
+      <c r="N1273" s="18">
+        <v>0.38125000000000003</v>
+      </c>
+      <c r="O1273" s="2">
+        <f t="shared" ref="O1273:O1354" si="22">N1273*1440-M1273*1440</f>
+        <v>89.999999999999943</v>
+      </c>
       <c r="Q1273" s="7" t="s">
         <v>67</v>
       </c>
@@ -67783,6 +67847,16 @@
       <c r="L1274" s="1">
         <v>24</v>
       </c>
+      <c r="M1274" s="18">
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="N1274" s="18">
+        <v>0.38263888888888892</v>
+      </c>
+      <c r="O1274" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999943</v>
+      </c>
       <c r="Q1274" s="7" t="s">
         <v>68</v>
       </c>
@@ -67833,6 +67907,16 @@
       <c r="L1275" s="1">
         <v>24</v>
       </c>
+      <c r="M1275" s="18">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="N1275" s="18">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="O1275" s="2">
+        <f t="shared" si="22"/>
+        <v>30</v>
+      </c>
       <c r="Q1275" s="7" t="s">
         <v>69</v>
       </c>
@@ -67886,6 +67970,16 @@
       <c r="L1276" s="1">
         <v>24</v>
       </c>
+      <c r="M1276" s="18">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="N1276" s="18">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="O1276" s="2">
+        <f t="shared" si="22"/>
+        <v>30</v>
+      </c>
       <c r="Q1276" s="7" t="s">
         <v>70</v>
       </c>
@@ -67939,6 +68033,16 @@
       <c r="L1277" s="1">
         <v>24</v>
       </c>
+      <c r="M1277" s="18">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="N1277" s="18">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="O1277" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1277" s="7" t="s">
         <v>71</v>
       </c>
@@ -67992,6 +68096,16 @@
       <c r="L1278" s="1">
         <v>24</v>
       </c>
+      <c r="M1278" s="18">
+        <v>0.32430555555555557</v>
+      </c>
+      <c r="N1278" s="18">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="O1278" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1278" s="7" t="s">
         <v>72</v>
       </c>
@@ -68045,6 +68159,16 @@
       <c r="L1279" s="1">
         <v>24</v>
       </c>
+      <c r="M1279" s="18">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="N1279" s="18">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="O1279" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1279" s="7" t="s">
         <v>73</v>
       </c>
@@ -68098,6 +68222,16 @@
       <c r="L1280" s="1">
         <v>24</v>
       </c>
+      <c r="M1280" s="18">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="N1280" s="18">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="O1280" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1280" s="7" t="s">
         <v>74</v>
       </c>
@@ -68151,6 +68285,16 @@
       <c r="L1281" s="1">
         <v>24</v>
       </c>
+      <c r="M1281" s="18">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="N1281" s="18">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="O1281" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1281" s="7" t="s">
         <v>75</v>
       </c>
@@ -68204,6 +68348,16 @@
       <c r="L1282" s="1">
         <v>32</v>
       </c>
+      <c r="M1282" s="18">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="N1282" s="18">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="O1282" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1282" s="7" t="s">
         <v>76</v>
       </c>
@@ -68254,6 +68408,16 @@
       <c r="L1283" s="1">
         <v>32</v>
       </c>
+      <c r="M1283" s="18">
+        <v>0.36041666666666666</v>
+      </c>
+      <c r="N1283" s="18">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="O1283" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1283" s="7" t="s">
         <v>77</v>
       </c>
@@ -68304,6 +68468,16 @@
       <c r="L1284" s="1">
         <v>32</v>
       </c>
+      <c r="M1284" s="18">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="N1284" s="18">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="O1284" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1284" s="7" t="s">
         <v>78</v>
       </c>
@@ -68354,6 +68528,16 @@
       <c r="L1285" s="1">
         <v>32</v>
       </c>
+      <c r="M1285" s="18">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="N1285" s="18">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="O1285" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1285" s="7" t="s">
         <v>79</v>
       </c>
@@ -68404,6 +68588,16 @@
       <c r="L1286" s="1">
         <v>32</v>
       </c>
+      <c r="M1286" s="18">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="N1286" s="18">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="O1286" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1286" s="7" t="s">
         <v>80</v>
       </c>
@@ -68454,6 +68648,16 @@
       <c r="L1287" s="1">
         <v>32</v>
       </c>
+      <c r="M1287" s="18">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="N1287" s="18">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="O1287" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1287" s="7" t="s">
         <v>81</v>
       </c>
@@ -68504,6 +68708,16 @@
       <c r="L1288" s="1">
         <v>32</v>
       </c>
+      <c r="M1288" s="18">
+        <v>0.36527777777777781</v>
+      </c>
+      <c r="N1288" s="18">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="O1288" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1288" s="7" t="s">
         <v>86</v>
       </c>
@@ -68554,6 +68768,16 @@
       <c r="L1289" s="1">
         <v>32</v>
       </c>
+      <c r="M1289" s="18">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="N1289" s="18">
+        <v>0.4291666666666667</v>
+      </c>
+      <c r="O1289" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1289" s="7" t="s">
         <v>85</v>
       </c>
@@ -68604,6 +68828,16 @@
       <c r="L1290" s="1">
         <v>32</v>
       </c>
+      <c r="M1290" s="18">
+        <v>0.36736111111111108</v>
+      </c>
+      <c r="N1290" s="18">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="O1290" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1290" s="7" t="s">
         <v>82</v>
       </c>
@@ -68654,6 +68888,16 @@
       <c r="L1291" s="1">
         <v>32</v>
       </c>
+      <c r="M1291" s="18">
+        <v>0.36874999999999997</v>
+      </c>
+      <c r="N1291" s="18">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="O1291" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1291" s="7" t="s">
         <v>83</v>
       </c>
@@ -68704,6 +68948,16 @@
       <c r="L1292" s="1">
         <v>32</v>
       </c>
+      <c r="M1292" s="18">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="N1292" s="18">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="O1292" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1292" s="7" t="s">
         <v>84</v>
       </c>
@@ -68757,6 +69011,16 @@
       <c r="L1293" s="1">
         <v>26</v>
       </c>
+      <c r="M1293" s="18">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="N1293" s="18">
+        <v>0.49861111111111112</v>
+      </c>
+      <c r="O1293" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1293" s="7" t="s">
         <v>66</v>
       </c>
@@ -68807,6 +69071,16 @@
       <c r="L1294" s="1">
         <v>26</v>
       </c>
+      <c r="M1294" s="18">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="N1294" s="18">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="O1294" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1294" s="7" t="s">
         <v>67</v>
       </c>
@@ -68857,6 +69131,16 @@
       <c r="L1295" s="1">
         <v>26</v>
       </c>
+      <c r="M1295" s="18">
+        <v>0.4375</v>
+      </c>
+      <c r="N1295" s="18">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="O1295" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1295" s="7" t="s">
         <v>68</v>
       </c>
@@ -68907,6 +69191,16 @@
       <c r="L1296" s="1">
         <v>26</v>
       </c>
+      <c r="M1296" s="18">
+        <v>0.43888888888888888</v>
+      </c>
+      <c r="N1296" s="18">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="O1296" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1296" s="7" t="s">
         <v>69</v>
       </c>
@@ -68957,6 +69251,16 @@
       <c r="L1297" s="1">
         <v>26</v>
       </c>
+      <c r="M1297" s="18">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="N1297" s="18">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="O1297" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999886</v>
+      </c>
       <c r="Q1297" s="7" t="s">
         <v>70</v>
       </c>
@@ -69007,6 +69311,16 @@
       <c r="L1298" s="1">
         <v>26</v>
       </c>
+      <c r="M1298" s="18">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="N1298" s="18">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="O1298" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999886</v>
+      </c>
       <c r="Q1298" s="7" t="s">
         <v>71</v>
       </c>
@@ -69057,6 +69371,16 @@
       <c r="L1299" s="1">
         <v>26</v>
       </c>
+      <c r="M1299" s="18">
+        <v>0.44166666666666665</v>
+      </c>
+      <c r="N1299" s="18">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="O1299" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1299" s="7" t="s">
         <v>72</v>
       </c>
@@ -69107,6 +69431,16 @@
       <c r="L1300" s="1">
         <v>26</v>
       </c>
+      <c r="M1300" s="18">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="N1300" s="18">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="O1300" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1300" s="7" t="s">
         <v>73</v>
       </c>
@@ -69157,6 +69491,16 @@
       <c r="L1301" s="1">
         <v>26</v>
       </c>
+      <c r="M1301" s="18">
+        <v>0.44375000000000003</v>
+      </c>
+      <c r="N1301" s="18">
+        <v>0.50624999999999998</v>
+      </c>
+      <c r="O1301" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1301" s="7" t="s">
         <v>74</v>
       </c>
@@ -69207,6 +69551,16 @@
       <c r="L1302" s="1">
         <v>26</v>
       </c>
+      <c r="M1302" s="18">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N1302" s="18">
+        <v>0.50763888888888886</v>
+      </c>
+      <c r="O1302" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
       <c r="Q1302" s="7" t="s">
         <v>75</v>
       </c>
@@ -69257,6 +69611,16 @@
       <c r="L1303" s="1">
         <v>30</v>
       </c>
+      <c r="M1303" s="18">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="N1303" s="18">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="O1303" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
       <c r="Q1303" s="7" t="s">
         <v>76</v>
       </c>
@@ -69307,6 +69671,16 @@
       <c r="L1304" s="1">
         <v>30</v>
       </c>
+      <c r="M1304" s="18">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="N1304" s="18">
+        <v>0.54305555555555551</v>
+      </c>
+      <c r="O1304" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999886</v>
+      </c>
       <c r="Q1304" s="7" t="s">
         <v>77</v>
       </c>
@@ -69357,6 +69731,16 @@
       <c r="L1305" s="1">
         <v>30</v>
       </c>
+      <c r="M1305" s="18">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="N1305" s="18">
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="O1305" s="2">
+        <f t="shared" si="22"/>
+        <v>91.000000000000114</v>
+      </c>
       <c r="Q1305" s="7" t="s">
         <v>78</v>
       </c>
@@ -69407,6 +69791,16 @@
       <c r="L1306" s="1">
         <v>30</v>
       </c>
+      <c r="M1306" s="18">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="N1306" s="18">
+        <v>0.5444444444444444</v>
+      </c>
+      <c r="O1306" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999886</v>
+      </c>
       <c r="Q1306" s="7" t="s">
         <v>79</v>
       </c>
@@ -69457,6 +69851,16 @@
       <c r="L1307" s="1">
         <v>30</v>
       </c>
+      <c r="M1307" s="18">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="N1307" s="18">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="O1307" s="2">
+        <f t="shared" si="22"/>
+        <v>90.000000000000114</v>
+      </c>
       <c r="Q1307" s="7" t="s">
         <v>80</v>
       </c>
@@ -69507,6 +69911,16 @@
       <c r="L1308" s="1">
         <v>30</v>
       </c>
+      <c r="M1308" s="18">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="N1308" s="18">
+        <v>0.54652777777777783</v>
+      </c>
+      <c r="O1308" s="2">
+        <f t="shared" si="22"/>
+        <v>90.000000000000114</v>
+      </c>
       <c r="Q1308" s="7" t="s">
         <v>81</v>
       </c>
@@ -69560,6 +69974,16 @@
       <c r="L1309" s="1">
         <v>30</v>
       </c>
+      <c r="M1309" s="18">
+        <v>0.48472222222222222</v>
+      </c>
+      <c r="N1309" s="18">
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="O1309" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999886</v>
+      </c>
       <c r="Q1309" s="7" t="s">
         <v>86</v>
       </c>
@@ -69610,6 +70034,16 @@
       <c r="L1310" s="1">
         <v>30</v>
       </c>
+      <c r="M1310" s="18">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="N1310" s="18">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="O1310" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999886</v>
+      </c>
       <c r="Q1310" s="7" t="s">
         <v>85</v>
       </c>
@@ -69660,6 +70094,16 @@
       <c r="L1311" s="1">
         <v>30</v>
       </c>
+      <c r="M1311" s="18">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="N1311" s="18">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="O1311" s="2">
+        <f t="shared" si="22"/>
+        <v>90.000000000000114</v>
+      </c>
       <c r="Q1311" s="7" t="s">
         <v>82</v>
       </c>
@@ -69710,6 +70154,16 @@
       <c r="L1312" s="1">
         <v>30</v>
       </c>
+      <c r="M1312" s="18">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="N1312" s="18">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="O1312" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999886</v>
+      </c>
       <c r="Q1312" s="7" t="s">
         <v>83</v>
       </c>
@@ -69760,6 +70214,16 @@
       <c r="L1313" s="1">
         <v>30</v>
       </c>
+      <c r="M1313" s="18">
+        <v>0.48819444444444443</v>
+      </c>
+      <c r="N1313" s="18">
+        <v>0.55138888888888882</v>
+      </c>
+      <c r="O1313" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999886</v>
+      </c>
       <c r="Q1313" s="7" t="s">
         <v>84</v>
       </c>
@@ -69792,11 +70256,33 @@
       <c r="F1314" t="s">
         <v>56</v>
       </c>
+      <c r="G1314" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1314" s="16">
+        <v>18.536999999999999</v>
+      </c>
+      <c r="I1314" s="16">
+        <v>19.512</v>
+      </c>
       <c r="J1314">
         <v>1</v>
       </c>
       <c r="K1314" s="1">
         <v>1</v>
+      </c>
+      <c r="L1314" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1314" s="18">
+        <v>0.31319444444444444</v>
+      </c>
+      <c r="N1314" s="18">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="O1314" s="2">
+        <f t="shared" si="22"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1314" s="7" t="s">
         <v>66</v>
@@ -69821,11 +70307,33 @@
       <c r="F1315" t="s">
         <v>58</v>
       </c>
+      <c r="G1315" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1315" s="16">
+        <v>17.863</v>
+      </c>
+      <c r="I1315" s="16">
+        <v>19.22</v>
+      </c>
       <c r="J1315">
         <v>1</v>
       </c>
       <c r="K1315" s="1">
         <v>1</v>
+      </c>
+      <c r="L1315" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1315" s="18">
+        <v>0.31388888888888888</v>
+      </c>
+      <c r="N1315" s="18">
+        <v>0.37638888888888888</v>
+      </c>
+      <c r="O1315" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1315" s="7" t="s">
         <v>67</v>
@@ -69850,11 +70358,33 @@
       <c r="F1316" t="s">
         <v>28</v>
       </c>
+      <c r="G1316" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1316" s="16">
+        <v>17.734000000000002</v>
+      </c>
+      <c r="I1316" s="16">
+        <v>18.846</v>
+      </c>
       <c r="J1316">
         <v>1</v>
       </c>
       <c r="K1316" s="1">
         <v>1</v>
+      </c>
+      <c r="L1316" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1316" s="18">
+        <v>0.31527777777777777</v>
+      </c>
+      <c r="N1316" s="18">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="O1316" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1316" s="7" t="s">
         <v>68</v>
@@ -69879,11 +70409,33 @@
       <c r="F1317" t="s">
         <v>30</v>
       </c>
+      <c r="G1317" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1317" s="16">
+        <v>17.702999999999999</v>
+      </c>
+      <c r="I1317" s="16">
+        <v>18.997</v>
+      </c>
       <c r="J1317">
         <v>1</v>
       </c>
       <c r="K1317" s="1">
         <v>1</v>
+      </c>
+      <c r="L1317" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1317" s="18">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="N1317" s="18">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="O1317" s="2">
+        <f t="shared" si="22"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1317" s="7" t="s">
         <v>69</v>
@@ -69908,11 +70460,33 @@
       <c r="F1318" t="s">
         <v>46</v>
       </c>
+      <c r="G1318" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1318" s="16">
+        <v>18.146000000000001</v>
+      </c>
+      <c r="I1318" s="16">
+        <v>19.376000000000001</v>
+      </c>
       <c r="J1318">
         <v>1</v>
       </c>
       <c r="K1318" s="1">
         <v>1</v>
+      </c>
+      <c r="L1318" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1318" s="18">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="N1318" s="18">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="O1318" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1318" s="7" t="s">
         <v>70</v>
@@ -69937,11 +70511,33 @@
       <c r="F1319" t="s">
         <v>54</v>
       </c>
+      <c r="G1319" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1319" s="16">
+        <v>18.34</v>
+      </c>
+      <c r="I1319" s="16">
+        <v>19.562000000000001</v>
+      </c>
       <c r="J1319">
         <v>1</v>
       </c>
       <c r="K1319" s="1">
         <v>1</v>
+      </c>
+      <c r="L1319" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1319" s="18">
+        <v>0.31805555555555554</v>
+      </c>
+      <c r="N1319" s="18">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="O1319" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1319" s="7" t="s">
         <v>71</v>
@@ -69966,11 +70562,33 @@
       <c r="F1320" t="s">
         <v>36</v>
       </c>
+      <c r="G1320" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1320" s="16">
+        <v>17.957999999999998</v>
+      </c>
+      <c r="I1320" s="16">
+        <v>19.158999999999999</v>
+      </c>
       <c r="J1320">
         <v>1</v>
       </c>
       <c r="K1320" s="1">
         <v>1</v>
+      </c>
+      <c r="L1320" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1320" s="18">
+        <v>0.31875000000000003</v>
+      </c>
+      <c r="N1320" s="18">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="O1320" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1320" s="7" t="s">
         <v>72</v>
@@ -69995,11 +70613,33 @@
       <c r="F1321" t="s">
         <v>52</v>
       </c>
+      <c r="G1321" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="H1321" s="16">
+        <v>18.151</v>
+      </c>
+      <c r="I1321" s="16">
+        <v>19.38</v>
+      </c>
       <c r="J1321">
         <v>1</v>
       </c>
       <c r="K1321" s="1">
         <v>1</v>
+      </c>
+      <c r="L1321" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1321" s="18">
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="N1321" s="18">
+        <v>0.38263888888888892</v>
+      </c>
+      <c r="O1321" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1321" s="7" t="s">
         <v>73</v>
@@ -70024,11 +70664,33 @@
       <c r="F1322" t="s">
         <v>40</v>
       </c>
+      <c r="G1322" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1322" s="16">
+        <v>18.385000000000002</v>
+      </c>
+      <c r="I1322" s="16">
+        <v>19.734000000000002</v>
+      </c>
       <c r="J1322">
         <v>1</v>
       </c>
       <c r="K1322" s="1">
         <v>1</v>
+      </c>
+      <c r="L1322" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1322" s="18">
+        <v>0.32083333333333336</v>
+      </c>
+      <c r="N1322" s="18">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="O1322" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1322" s="7" t="s">
         <v>74</v>
@@ -70053,11 +70715,33 @@
       <c r="F1323" t="s">
         <v>26</v>
       </c>
+      <c r="G1323" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1323" s="16">
+        <v>18.157</v>
+      </c>
+      <c r="I1323" s="16">
+        <v>19.510000000000002</v>
+      </c>
       <c r="J1323">
         <v>1</v>
       </c>
       <c r="K1323" s="1">
         <v>1</v>
+      </c>
+      <c r="L1323" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1323" s="18">
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="N1323" s="18">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="O1323" s="2">
+        <f t="shared" si="22"/>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1323" s="7" t="s">
         <v>75</v>
@@ -70082,11 +70766,33 @@
       <c r="F1324" t="s">
         <v>24</v>
       </c>
+      <c r="G1324" s="1">
+        <v>27</v>
+      </c>
+      <c r="H1324" s="16">
+        <v>17.713000000000001</v>
+      </c>
+      <c r="I1324" s="16">
+        <v>18.977</v>
+      </c>
       <c r="J1324">
         <v>2</v>
       </c>
       <c r="K1324" s="1">
         <v>1</v>
+      </c>
+      <c r="L1324" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1324" s="18">
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="N1324" s="18">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="O1324" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1324" s="7" t="s">
         <v>76</v>
@@ -70111,11 +70817,33 @@
       <c r="F1325" t="s">
         <v>62</v>
       </c>
+      <c r="G1325" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1325" s="16">
+        <v>18.068000000000001</v>
+      </c>
+      <c r="I1325" s="16">
+        <v>19.151</v>
+      </c>
       <c r="J1325">
         <v>2</v>
       </c>
       <c r="K1325" s="1">
         <v>1</v>
+      </c>
+      <c r="L1325" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1325" s="18">
+        <v>0.35625000000000001</v>
+      </c>
+      <c r="N1325" s="18">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="O1325" s="2">
+        <f t="shared" si="22"/>
+        <v>89</v>
       </c>
       <c r="Q1325" s="7" t="s">
         <v>77</v>
@@ -70140,11 +70868,33 @@
       <c r="F1326" t="s">
         <v>44</v>
       </c>
+      <c r="G1326" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1326" s="16">
+        <v>18.225000000000001</v>
+      </c>
+      <c r="I1326" s="16">
+        <v>19.344000000000001</v>
+      </c>
       <c r="J1326">
         <v>2</v>
       </c>
       <c r="K1326" s="1">
         <v>1</v>
+      </c>
+      <c r="L1326" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1326" s="18">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="N1326" s="18">
+        <v>0.41944444444444445</v>
+      </c>
+      <c r="O1326" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1326" s="7" t="s">
         <v>78</v>
@@ -70169,11 +70919,33 @@
       <c r="F1327" t="s">
         <v>42</v>
       </c>
+      <c r="G1327" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1327" s="16">
+        <v>18.390999999999998</v>
+      </c>
+      <c r="I1327" s="16">
+        <v>19.497</v>
+      </c>
       <c r="J1327">
         <v>2</v>
       </c>
       <c r="K1327" s="1">
         <v>1</v>
+      </c>
+      <c r="L1327" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1327" s="18">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="N1327" s="18">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="O1327" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1327" s="7" t="s">
         <v>79</v>
@@ -70198,11 +70970,33 @@
       <c r="F1328" t="s">
         <v>50</v>
       </c>
+      <c r="G1328" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1328" s="16">
+        <v>18.102</v>
+      </c>
+      <c r="I1328" s="16">
+        <v>19.190999999999999</v>
+      </c>
       <c r="J1328">
         <v>2</v>
       </c>
       <c r="K1328" s="1">
         <v>1</v>
+      </c>
+      <c r="L1328" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1328" s="18">
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="N1328" s="18">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="O1328" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1328" s="7" t="s">
         <v>80</v>
@@ -70227,11 +71021,33 @@
       <c r="F1329" t="s">
         <v>32</v>
       </c>
+      <c r="G1329" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1329" s="16">
+        <v>18.167999999999999</v>
+      </c>
+      <c r="I1329" s="16">
+        <v>19.356999999999999</v>
+      </c>
       <c r="J1329">
         <v>2</v>
       </c>
       <c r="K1329" s="1">
         <v>1</v>
+      </c>
+      <c r="L1329" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1329" s="18">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="N1329" s="18">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="O1329" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1329" s="7" t="s">
         <v>81</v>
@@ -70256,11 +71072,33 @@
       <c r="F1330" t="s">
         <v>48</v>
       </c>
+      <c r="G1330" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1330" s="16">
+        <v>18.074000000000002</v>
+      </c>
+      <c r="I1330" s="16">
+        <v>19.346</v>
+      </c>
       <c r="J1330">
         <v>2</v>
       </c>
       <c r="K1330" s="1">
         <v>1</v>
+      </c>
+      <c r="L1330" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1330" s="18">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="N1330" s="18">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="O1330" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1330" s="7" t="s">
         <v>86</v>
@@ -70285,11 +71123,33 @@
       <c r="F1331" t="s">
         <v>60</v>
       </c>
+      <c r="G1331" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1331" s="16">
+        <v>18.126000000000001</v>
+      </c>
+      <c r="I1331" s="16">
+        <v>19.456</v>
+      </c>
       <c r="J1331">
         <v>2</v>
       </c>
       <c r="K1331" s="1">
         <v>1</v>
+      </c>
+      <c r="L1331" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1331" s="18">
+        <v>0.36180555555555555</v>
+      </c>
+      <c r="N1331" s="18">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="O1331" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1331" s="7" t="s">
         <v>85</v>
@@ -70314,11 +71174,33 @@
       <c r="F1332" t="s">
         <v>64</v>
       </c>
+      <c r="G1332" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1332" s="16">
+        <v>17.969000000000001</v>
+      </c>
+      <c r="I1332" s="16">
+        <v>19.148</v>
+      </c>
       <c r="J1332">
         <v>2</v>
       </c>
       <c r="K1332" s="1">
         <v>1</v>
+      </c>
+      <c r="L1332" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1332" s="18">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="N1332" s="18">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="O1332" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
       </c>
       <c r="Q1332" s="7" t="s">
         <v>82</v>
@@ -70343,11 +71225,33 @@
       <c r="F1333" t="s">
         <v>34</v>
       </c>
+      <c r="G1333" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1333" s="16">
+        <v>18.215</v>
+      </c>
+      <c r="I1333" s="16">
+        <v>19.332999999999998</v>
+      </c>
       <c r="J1333">
         <v>2</v>
       </c>
       <c r="K1333" s="1">
         <v>1</v>
+      </c>
+      <c r="L1333" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1333" s="18">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="N1333" s="18">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="O1333" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1333" s="7" t="s">
         <v>83</v>
@@ -70372,11 +71276,33 @@
       <c r="F1334" t="s">
         <v>38</v>
       </c>
+      <c r="G1334" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1334" s="16">
+        <v>18.245000000000001</v>
+      </c>
+      <c r="I1334" s="16">
+        <v>19.527000000000001</v>
+      </c>
       <c r="J1334">
         <v>2</v>
       </c>
       <c r="K1334" s="1">
         <v>1</v>
+      </c>
+      <c r="L1334" s="1">
+        <v>22</v>
+      </c>
+      <c r="M1334" s="18">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="N1334" s="18">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="O1334" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
       </c>
       <c r="Q1334" s="7" t="s">
         <v>84</v>
@@ -70401,11 +71327,33 @@
       <c r="F1335" t="s">
         <v>56</v>
       </c>
+      <c r="G1335" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1335" s="16">
+        <v>18.536999999999999</v>
+      </c>
+      <c r="I1335" s="16">
+        <v>19.512</v>
+      </c>
       <c r="J1335">
         <v>1</v>
       </c>
       <c r="K1335" s="1">
         <v>2</v>
+      </c>
+      <c r="L1335" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1335" s="18">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="N1335" s="18">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="O1335" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1335" s="7" t="s">
         <v>66</v>
@@ -70430,11 +71378,33 @@
       <c r="F1336" t="s">
         <v>58</v>
       </c>
+      <c r="G1336" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1336" s="16">
+        <v>17.863</v>
+      </c>
+      <c r="I1336" s="16">
+        <v>19.22</v>
+      </c>
       <c r="J1336">
         <v>1</v>
       </c>
       <c r="K1336" s="1">
         <v>2</v>
+      </c>
+      <c r="L1336" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1336" s="18">
+        <v>0.43194444444444446</v>
+      </c>
+      <c r="N1336" s="18">
+        <v>0.49444444444444446</v>
+      </c>
+      <c r="O1336" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1336" s="7" t="s">
         <v>67</v>
@@ -70459,11 +71429,33 @@
       <c r="F1337" t="s">
         <v>28</v>
       </c>
+      <c r="G1337" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1337" s="16">
+        <v>17.734000000000002</v>
+      </c>
+      <c r="I1337" s="16">
+        <v>18.846</v>
+      </c>
       <c r="J1337">
         <v>1</v>
       </c>
       <c r="K1337" s="1">
         <v>2</v>
+      </c>
+      <c r="L1337" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1337" s="18">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="N1337" s="18">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="O1337" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
       </c>
       <c r="Q1337" s="7" t="s">
         <v>68</v>
@@ -70488,11 +71480,33 @@
       <c r="F1338" t="s">
         <v>30</v>
       </c>
+      <c r="G1338" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1338" s="16">
+        <v>17.702999999999999</v>
+      </c>
+      <c r="I1338" s="16">
+        <v>18.997</v>
+      </c>
       <c r="J1338">
         <v>1</v>
       </c>
       <c r="K1338" s="1">
         <v>2</v>
+      </c>
+      <c r="L1338" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1338" s="18">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="N1338" s="18">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="O1338" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1338" s="7" t="s">
         <v>69</v>
@@ -70517,11 +71531,33 @@
       <c r="F1339" t="s">
         <v>46</v>
       </c>
+      <c r="G1339" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1339" s="16">
+        <v>18.146000000000001</v>
+      </c>
+      <c r="I1339" s="16">
+        <v>19.376000000000001</v>
+      </c>
       <c r="J1339">
         <v>1</v>
       </c>
       <c r="K1339" s="1">
         <v>2</v>
+      </c>
+      <c r="L1339" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1339" s="18">
+        <v>0.43472222222222223</v>
+      </c>
+      <c r="N1339" s="18">
+        <v>0.49791666666666662</v>
+      </c>
+      <c r="O1339" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1339" s="7" t="s">
         <v>70</v>
@@ -70546,11 +71582,33 @@
       <c r="F1340" t="s">
         <v>54</v>
       </c>
+      <c r="G1340" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1340" s="16">
+        <v>18.34</v>
+      </c>
+      <c r="I1340" s="16">
+        <v>19.562000000000001</v>
+      </c>
       <c r="J1340">
         <v>1</v>
       </c>
       <c r="K1340" s="1">
         <v>2</v>
+      </c>
+      <c r="L1340" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1340" s="18">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="N1340" s="18">
+        <v>0.49861111111111112</v>
+      </c>
+      <c r="O1340" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1340" s="7" t="s">
         <v>71</v>
@@ -70575,11 +71633,33 @@
       <c r="F1341" t="s">
         <v>36</v>
       </c>
+      <c r="G1341" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1341" s="16">
+        <v>17.957999999999998</v>
+      </c>
+      <c r="I1341" s="16">
+        <v>19.158999999999999</v>
+      </c>
       <c r="J1341">
         <v>1</v>
       </c>
       <c r="K1341" s="1">
         <v>2</v>
+      </c>
+      <c r="L1341" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1341" s="18">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="N1341" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="O1341" s="2">
+        <f t="shared" si="22"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1341" s="7" t="s">
         <v>72</v>
@@ -70604,11 +71684,33 @@
       <c r="F1342" t="s">
         <v>52</v>
       </c>
+      <c r="G1342" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="H1342" s="16">
+        <v>18.151</v>
+      </c>
+      <c r="I1342" s="16">
+        <v>19.38</v>
+      </c>
       <c r="J1342">
         <v>1</v>
       </c>
       <c r="K1342" s="1">
         <v>2</v>
+      </c>
+      <c r="L1342" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1342" s="18">
+        <v>0.4375</v>
+      </c>
+      <c r="N1342" s="18">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="O1342" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
       </c>
       <c r="Q1342" s="7" t="s">
         <v>73</v>
@@ -70633,11 +71735,33 @@
       <c r="F1343" t="s">
         <v>40</v>
       </c>
+      <c r="G1343" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1343" s="16">
+        <v>18.385000000000002</v>
+      </c>
+      <c r="I1343" s="16">
+        <v>19.734000000000002</v>
+      </c>
       <c r="J1343">
         <v>1</v>
       </c>
       <c r="K1343" s="1">
         <v>2</v>
+      </c>
+      <c r="L1343" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1343" s="18">
+        <v>0.43888888888888888</v>
+      </c>
+      <c r="N1343" s="18">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="O1343" s="2">
+        <f t="shared" si="22"/>
+        <v>91</v>
       </c>
       <c r="Q1343" s="7" t="s">
         <v>74</v>
@@ -70662,11 +71786,33 @@
       <c r="F1344" t="s">
         <v>26</v>
       </c>
+      <c r="G1344" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1344" s="16">
+        <v>18.157</v>
+      </c>
+      <c r="I1344" s="16">
+        <v>19.510000000000002</v>
+      </c>
       <c r="J1344">
         <v>1</v>
       </c>
       <c r="K1344" s="1">
         <v>2</v>
+      </c>
+      <c r="L1344" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1344" s="18">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="N1344" s="18">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="O1344" s="2">
+        <f t="shared" si="22"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1344" s="7" t="s">
         <v>75</v>
@@ -70691,11 +71837,33 @@
       <c r="F1345" t="s">
         <v>24</v>
       </c>
+      <c r="G1345" s="1">
+        <v>27</v>
+      </c>
+      <c r="H1345" s="16">
+        <v>17.713000000000001</v>
+      </c>
+      <c r="I1345" s="16">
+        <v>18.977</v>
+      </c>
       <c r="J1345">
         <v>2</v>
       </c>
       <c r="K1345" s="1">
         <v>2</v>
+      </c>
+      <c r="L1345" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1345" s="18">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="N1345" s="18">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="O1345" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1345" s="7" t="s">
         <v>76</v>
@@ -70720,11 +71888,33 @@
       <c r="F1346" t="s">
         <v>62</v>
       </c>
+      <c r="G1346" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1346" s="16">
+        <v>18.068000000000001</v>
+      </c>
+      <c r="I1346" s="16">
+        <v>19.151</v>
+      </c>
       <c r="J1346">
         <v>2</v>
       </c>
       <c r="K1346" s="1">
         <v>2</v>
+      </c>
+      <c r="L1346" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1346" s="18">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="N1346" s="18">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="O1346" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1346" s="7" t="s">
         <v>77</v>
@@ -70749,11 +71939,33 @@
       <c r="F1347" t="s">
         <v>44</v>
       </c>
+      <c r="G1347" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1347" s="16">
+        <v>18.225000000000001</v>
+      </c>
+      <c r="I1347" s="16">
+        <v>19.344000000000001</v>
+      </c>
       <c r="J1347">
         <v>2</v>
       </c>
       <c r="K1347" s="1">
         <v>2</v>
+      </c>
+      <c r="L1347" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1347" s="18">
+        <v>0.47638888888888892</v>
+      </c>
+      <c r="N1347" s="18">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="O1347" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1347" s="7" t="s">
         <v>78</v>
@@ -70778,11 +71990,33 @@
       <c r="F1348" t="s">
         <v>42</v>
       </c>
+      <c r="G1348" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1348" s="16">
+        <v>18.390999999999998</v>
+      </c>
+      <c r="I1348" s="16">
+        <v>19.497</v>
+      </c>
       <c r="J1348">
         <v>2</v>
       </c>
       <c r="K1348" s="1">
         <v>2</v>
+      </c>
+      <c r="L1348" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1348" s="18">
+        <v>0.4770833333333333</v>
+      </c>
+      <c r="N1348" s="18">
+        <v>0.5395833333333333</v>
+      </c>
+      <c r="O1348" s="2">
+        <f t="shared" si="22"/>
+        <v>90</v>
       </c>
       <c r="Q1348" s="7" t="s">
         <v>79</v>
@@ -70807,11 +72041,33 @@
       <c r="F1349" t="s">
         <v>50</v>
       </c>
+      <c r="G1349" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1349" s="16">
+        <v>18.102</v>
+      </c>
+      <c r="I1349" s="16">
+        <v>19.190999999999999</v>
+      </c>
       <c r="J1349">
         <v>2</v>
       </c>
       <c r="K1349" s="1">
         <v>2</v>
+      </c>
+      <c r="L1349" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1349" s="18">
+        <v>0.47847222222222219</v>
+      </c>
+      <c r="N1349" s="18">
+        <v>0.54097222222222219</v>
+      </c>
+      <c r="O1349" s="2">
+        <f>N1350*1440-M1349*1440</f>
+        <v>91</v>
       </c>
       <c r="Q1349" s="7" t="s">
         <v>80</v>
@@ -70836,11 +72092,33 @@
       <c r="F1350" t="s">
         <v>32</v>
       </c>
+      <c r="G1350" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1350" s="16">
+        <v>18.167999999999999</v>
+      </c>
+      <c r="I1350" s="16">
+        <v>19.356999999999999</v>
+      </c>
       <c r="J1350">
         <v>2</v>
       </c>
       <c r="K1350" s="1">
         <v>2</v>
+      </c>
+      <c r="L1350" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1350" s="18">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="N1350" s="18">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="O1350" s="2">
+        <f>N1351*1440-M1350*1440</f>
+        <v>91.999999999999886</v>
       </c>
       <c r="Q1350" s="7" t="s">
         <v>81</v>
@@ -70865,11 +72143,33 @@
       <c r="F1351" t="s">
         <v>48</v>
       </c>
+      <c r="G1351" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1351" s="16">
+        <v>18.074000000000002</v>
+      </c>
+      <c r="I1351" s="16">
+        <v>19.346</v>
+      </c>
       <c r="J1351">
         <v>2</v>
       </c>
       <c r="K1351" s="1">
         <v>2</v>
+      </c>
+      <c r="L1351" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1351" s="18">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="N1351" s="18">
+        <v>0.54305555555555551</v>
+      </c>
+      <c r="O1351" s="2">
+        <f>N1352*1440-M1351*1440</f>
+        <v>92.000000000000114</v>
       </c>
       <c r="Q1351" s="7" t="s">
         <v>86</v>
@@ -70894,11 +72194,33 @@
       <c r="F1352" t="s">
         <v>60</v>
       </c>
+      <c r="G1352" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1352" s="16">
+        <v>18.126000000000001</v>
+      </c>
+      <c r="I1352" s="16">
+        <v>19.456</v>
+      </c>
       <c r="J1352">
         <v>2</v>
       </c>
       <c r="K1352" s="1">
         <v>2</v>
+      </c>
+      <c r="L1352" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1352" s="18">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="N1352" s="18">
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="O1352" s="2">
+        <f>N1353*1440-M1352*1440</f>
+        <v>92.000000000000114</v>
       </c>
       <c r="Q1352" s="7" t="s">
         <v>85</v>
@@ -70923,11 +72245,33 @@
       <c r="F1353" t="s">
         <v>64</v>
       </c>
+      <c r="G1353" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1353" s="16">
+        <v>17.969000000000001</v>
+      </c>
+      <c r="I1353" s="16">
+        <v>19.148</v>
+      </c>
       <c r="J1353">
         <v>2</v>
       </c>
       <c r="K1353" s="1">
         <v>2</v>
+      </c>
+      <c r="L1353" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1353" s="18">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="N1353" s="18">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="O1353" s="2">
+        <f>N1354*1440-M1353*1440</f>
+        <v>91.999999999999886</v>
       </c>
       <c r="Q1353" s="7" t="s">
         <v>82</v>
@@ -70952,11 +72296,33 @@
       <c r="F1354" t="s">
         <v>34</v>
       </c>
+      <c r="G1354" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1354" s="16">
+        <v>18.215</v>
+      </c>
+      <c r="I1354" s="16">
+        <v>19.332999999999998</v>
+      </c>
       <c r="J1354">
         <v>2</v>
       </c>
       <c r="K1354" s="1">
         <v>2</v>
+      </c>
+      <c r="L1354" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1354" s="18">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="N1354" s="18">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="O1354" s="2">
+        <f>N1355*1440-M1354*1440</f>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1354" s="7" t="s">
         <v>83</v>
@@ -70981,11 +72347,33 @@
       <c r="F1355" t="s">
         <v>38</v>
       </c>
+      <c r="G1355" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1355" s="16">
+        <v>18.245000000000001</v>
+      </c>
+      <c r="I1355" s="16">
+        <v>19.527000000000001</v>
+      </c>
       <c r="J1355">
         <v>2</v>
       </c>
       <c r="K1355" s="1">
         <v>2</v>
+      </c>
+      <c r="L1355" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1355" s="18">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="N1355" s="18">
+        <v>0.54652777777777783</v>
+      </c>
+      <c r="O1355" s="2">
+        <f>N1355*1440-M1355*1440</f>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1355" s="7" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
General data entry complete up till 29.01.17
</commit_message>
<xml_diff>
--- a/data/ldeli_integrate.xlsx
+++ b/data/ldeli_integrate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5475" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5484" uniqueCount="175">
   <si>
     <t>date</t>
   </si>
@@ -543,6 +543,9 @@
   <si>
     <t>MultiPCO2BL</t>
   </si>
+  <si>
+    <t>BadBLCO2</t>
+  </si>
 </sst>
 </file>
 
@@ -638,11 +641,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="606">
+  <cellStyleXfs count="626">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1331,7 +1354,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="606">
+  <cellStyles count="626">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1636,6 +1659,16 @@
     <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -1937,6 +1970,16 @@
     <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2268,9 +2311,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1779"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1331" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1345" sqref="N1345"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1465" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1483" sqref="N1483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -64717,7 +64760,7 @@
         <v>0.49652777777777773</v>
       </c>
       <c r="O1212" s="2">
-        <f t="shared" ref="O1212:O1272" si="21">N1212*1440-M1212*1440</f>
+        <f t="shared" ref="O1212:O1270" si="21">N1212*1440-M1212*1440</f>
         <v>90</v>
       </c>
       <c r="Q1212" s="7" t="s">
@@ -67794,7 +67837,7 @@
         <v>0.38125000000000003</v>
       </c>
       <c r="O1273" s="2">
-        <f t="shared" ref="O1273:O1354" si="22">N1273*1440-M1273*1440</f>
+        <f t="shared" ref="O1273:O1348" si="22">N1273*1440-M1273*1440</f>
         <v>89.999999999999943</v>
       </c>
       <c r="Q1273" s="7" t="s">
@@ -70177,7 +70220,7 @@
         <v>4.9069999999999999E-3</v>
       </c>
     </row>
-    <row r="1313" spans="1:20" ht="16" customHeight="1">
+    <row r="1313" spans="1:28" ht="16" customHeight="1">
       <c r="A1313" s="3">
         <v>42760</v>
       </c>
@@ -70237,7 +70280,7 @@
         <v>4.2110000000000003E-3</v>
       </c>
     </row>
-    <row r="1314" spans="1:20" ht="16" customHeight="1">
+    <row r="1314" spans="1:28" ht="16" customHeight="1">
       <c r="A1314" s="3">
         <v>42761</v>
       </c>
@@ -70287,8 +70330,17 @@
       <c r="Q1314" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="1315" spans="1:20" ht="16" customHeight="1">
+      <c r="R1314" s="28">
+        <v>1.906E-4</v>
+      </c>
+      <c r="S1314" s="28">
+        <v>1.0369999999999999E-3</v>
+      </c>
+      <c r="T1314" s="28">
+        <v>1.758E-3</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:28" ht="16" customHeight="1">
       <c r="A1315" s="3">
         <v>42761</v>
       </c>
@@ -70338,8 +70390,17 @@
       <c r="Q1315" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="1316" spans="1:20" ht="16" customHeight="1">
+      <c r="R1315" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1315" s="28">
+        <v>1.413E-3</v>
+      </c>
+      <c r="T1315" s="28">
+        <v>1.3569999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:28" ht="16" customHeight="1">
       <c r="A1316" s="3">
         <v>42761</v>
       </c>
@@ -70389,8 +70450,17 @@
       <c r="Q1316" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="1317" spans="1:20" ht="16" customHeight="1">
+      <c r="R1316" s="28">
+        <v>3.0640000000000002E-4</v>
+      </c>
+      <c r="S1316" s="28">
+        <v>1.2639999999999999E-3</v>
+      </c>
+      <c r="T1316" s="28">
+        <v>8.7679999999999995E-4</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:28" ht="16" customHeight="1">
       <c r="A1317" s="3">
         <v>42761</v>
       </c>
@@ -70440,8 +70510,20 @@
       <c r="Q1317" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="1318" spans="1:20" ht="16" customHeight="1">
+      <c r="R1317" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1317" s="28">
+        <v>1.407E-3</v>
+      </c>
+      <c r="T1317" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB1317" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:28" ht="16" customHeight="1">
       <c r="A1318" s="3">
         <v>42761</v>
       </c>
@@ -70491,8 +70573,17 @@
       <c r="Q1318" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="1319" spans="1:20" ht="16" customHeight="1">
+      <c r="R1318" s="28">
+        <v>1.2970000000000001E-4</v>
+      </c>
+      <c r="S1318" s="28">
+        <v>1.81E-3</v>
+      </c>
+      <c r="T1318" s="28">
+        <v>1.382E-3</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:28" ht="16" customHeight="1">
       <c r="A1319" s="3">
         <v>42761</v>
       </c>
@@ -70542,8 +70633,17 @@
       <c r="Q1319" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="1320" spans="1:20" ht="16" customHeight="1">
+      <c r="R1319" s="28">
+        <v>3.7960000000000001E-4</v>
+      </c>
+      <c r="S1319" s="28">
+        <v>1.4610000000000001E-3</v>
+      </c>
+      <c r="T1319" s="28">
+        <v>1.6379999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:28" ht="16" customHeight="1">
       <c r="A1320" s="3">
         <v>42761</v>
       </c>
@@ -70593,8 +70693,17 @@
       <c r="Q1320" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="1321" spans="1:20" ht="16" customHeight="1">
+      <c r="R1320" s="28">
+        <v>5.62E-4</v>
+      </c>
+      <c r="S1320" s="28">
+        <v>1.5629999999999999E-3</v>
+      </c>
+      <c r="T1320" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:28" ht="16" customHeight="1">
       <c r="A1321" s="3">
         <v>42761</v>
       </c>
@@ -70644,8 +70753,17 @@
       <c r="Q1321" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="1322" spans="1:20" ht="16" customHeight="1">
+      <c r="R1321" s="28">
+        <v>2.2039999999999999E-4</v>
+      </c>
+      <c r="S1321" s="28">
+        <v>1.7799999999999999E-3</v>
+      </c>
+      <c r="T1321" s="28">
+        <v>1.372E-3</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:28" ht="16" customHeight="1">
       <c r="A1322" s="3">
         <v>42761</v>
       </c>
@@ -70695,8 +70813,17 @@
       <c r="Q1322" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="1323" spans="1:20" ht="16" customHeight="1">
+      <c r="R1322" s="28">
+        <v>5.6879999999999995E-4</v>
+      </c>
+      <c r="S1322" s="28">
+        <v>1.302E-3</v>
+      </c>
+      <c r="T1322" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:28" ht="16" customHeight="1">
       <c r="A1323" s="3">
         <v>42761</v>
       </c>
@@ -70746,8 +70873,17 @@
       <c r="Q1323" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1324" spans="1:20" ht="16" customHeight="1">
+      <c r="R1323" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1323" s="28">
+        <v>7.3200000000000001E-4</v>
+      </c>
+      <c r="T1323" s="28">
+        <v>1.14E-3</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:28" ht="16" customHeight="1">
       <c r="A1324" s="3">
         <v>42761</v>
       </c>
@@ -70797,8 +70933,17 @@
       <c r="Q1324" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="1325" spans="1:20" ht="16" customHeight="1">
+      <c r="R1324" s="28">
+        <v>3.7179999999999998E-4</v>
+      </c>
+      <c r="S1324" s="28">
+        <v>2.1589999999999999E-3</v>
+      </c>
+      <c r="T1324" s="28">
+        <v>2.5669999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:28" ht="16" customHeight="1">
       <c r="A1325" s="3">
         <v>42761</v>
       </c>
@@ -70848,8 +70993,17 @@
       <c r="Q1325" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="1326" spans="1:20" ht="16" customHeight="1">
+      <c r="R1325" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1325" s="28">
+        <v>1.5219999999999999E-3</v>
+      </c>
+      <c r="T1325" s="28">
+        <v>1.464E-3</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:28" ht="16" customHeight="1">
       <c r="A1326" s="3">
         <v>42761</v>
       </c>
@@ -70899,8 +71053,14 @@
       <c r="Q1326" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="1327" spans="1:20" ht="16" customHeight="1">
+      <c r="S1326" s="28">
+        <v>1.0319999999999999E-3</v>
+      </c>
+      <c r="T1326" s="28">
+        <v>1.4369999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:28" ht="16" customHeight="1">
       <c r="A1327" s="3">
         <v>42761</v>
       </c>
@@ -70950,8 +71110,17 @@
       <c r="Q1327" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="1328" spans="1:20" ht="16" customHeight="1">
+      <c r="R1327" s="28">
+        <v>5.4719999999999997E-4</v>
+      </c>
+      <c r="S1327" s="28">
+        <v>2.114E-3</v>
+      </c>
+      <c r="T1327" s="28">
+        <v>1.7240000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:28" ht="16" customHeight="1">
       <c r="A1328" s="3">
         <v>42761</v>
       </c>
@@ -71001,8 +71170,17 @@
       <c r="Q1328" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1329" spans="1:17" ht="16" customHeight="1">
+      <c r="R1328" s="28">
+        <v>2.7609999999999999E-4</v>
+      </c>
+      <c r="S1328" s="28">
+        <v>1.4E-3</v>
+      </c>
+      <c r="T1328" s="28">
+        <v>1.41E-3</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:20" ht="16" customHeight="1">
       <c r="A1329" s="3">
         <v>42761</v>
       </c>
@@ -71052,8 +71230,17 @@
       <c r="Q1329" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="1330" spans="1:17" ht="16" customHeight="1">
+      <c r="R1329" s="28">
+        <v>4.0789999999999999E-4</v>
+      </c>
+      <c r="S1329" s="28">
+        <v>1.707E-3</v>
+      </c>
+      <c r="T1329" s="28">
+        <v>1.9980000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:20" ht="16" customHeight="1">
       <c r="A1330" s="3">
         <v>42761</v>
       </c>
@@ -71103,8 +71290,17 @@
       <c r="Q1330" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="1331" spans="1:17" ht="16" customHeight="1">
+      <c r="R1330" s="28">
+        <v>1.0859999999999999E-3</v>
+      </c>
+      <c r="S1330" s="28">
+        <v>2.7680000000000001E-3</v>
+      </c>
+      <c r="T1330" s="28">
+        <v>1.078E-3</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:20" ht="16" customHeight="1">
       <c r="A1331" s="3">
         <v>42761</v>
       </c>
@@ -71154,8 +71350,17 @@
       <c r="Q1331" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="1332" spans="1:17" ht="16" customHeight="1">
+      <c r="R1331" s="28">
+        <v>1.232E-3</v>
+      </c>
+      <c r="S1331" s="28">
+        <v>1.6590000000000001E-3</v>
+      </c>
+      <c r="T1331" s="28">
+        <v>1.7329999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:20" ht="16" customHeight="1">
       <c r="A1332" s="3">
         <v>42761</v>
       </c>
@@ -71205,8 +71410,17 @@
       <c r="Q1332" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="1333" spans="1:17" ht="16" customHeight="1">
+      <c r="R1332" s="28">
+        <v>2.7500000000000002E-4</v>
+      </c>
+      <c r="S1332" s="28">
+        <v>2.5720000000000001E-3</v>
+      </c>
+      <c r="T1332" s="28">
+        <v>1.678E-3</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:20" ht="16" customHeight="1">
       <c r="A1333" s="3">
         <v>42761</v>
       </c>
@@ -71256,8 +71470,17 @@
       <c r="Q1333" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="1334" spans="1:17" ht="16" customHeight="1">
+      <c r="R1333" s="28">
+        <v>3.8919999999999997E-4</v>
+      </c>
+      <c r="S1333" s="28">
+        <v>1.591E-3</v>
+      </c>
+      <c r="T1333" s="28">
+        <v>2.4090000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:20" ht="16" customHeight="1">
       <c r="A1334" s="3">
         <v>42761</v>
       </c>
@@ -71307,8 +71530,17 @@
       <c r="Q1334" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="1335" spans="1:17" ht="16" customHeight="1">
+      <c r="R1334" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1334" s="28">
+        <v>2.1059999999999998E-3</v>
+      </c>
+      <c r="T1334" s="28">
+        <v>1.805E-3</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:20" ht="16" customHeight="1">
       <c r="A1335" s="3">
         <v>42761</v>
       </c>
@@ -71359,7 +71591,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1336" spans="1:17" ht="16" customHeight="1">
+    <row r="1336" spans="1:20" ht="16" customHeight="1">
       <c r="A1336" s="3">
         <v>42761</v>
       </c>
@@ -71410,7 +71642,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1337" spans="1:17" ht="16" customHeight="1">
+    <row r="1337" spans="1:20" ht="16" customHeight="1">
       <c r="A1337" s="3">
         <v>42761</v>
       </c>
@@ -71461,7 +71693,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="1338" spans="1:17" ht="16" customHeight="1">
+    <row r="1338" spans="1:20" ht="16" customHeight="1">
       <c r="A1338" s="3">
         <v>42761</v>
       </c>
@@ -71512,7 +71744,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="1339" spans="1:17" ht="16" customHeight="1">
+    <row r="1339" spans="1:20" ht="16" customHeight="1">
       <c r="A1339" s="3">
         <v>42761</v>
       </c>
@@ -71563,7 +71795,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="1340" spans="1:17" ht="16" customHeight="1">
+    <row r="1340" spans="1:20" ht="16" customHeight="1">
       <c r="A1340" s="3">
         <v>42761</v>
       </c>
@@ -71614,7 +71846,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="1341" spans="1:17" ht="16" customHeight="1">
+    <row r="1341" spans="1:20" ht="16" customHeight="1">
       <c r="A1341" s="3">
         <v>42761</v>
       </c>
@@ -71665,7 +71897,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="1342" spans="1:17" ht="16" customHeight="1">
+    <row r="1342" spans="1:20" ht="16" customHeight="1">
       <c r="A1342" s="3">
         <v>42761</v>
       </c>
@@ -71716,7 +71948,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="1343" spans="1:17" ht="16" customHeight="1">
+    <row r="1343" spans="1:20" ht="16" customHeight="1">
       <c r="A1343" s="3">
         <v>42761</v>
       </c>
@@ -71767,7 +71999,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="1344" spans="1:17" ht="16" customHeight="1">
+    <row r="1344" spans="1:20" ht="16" customHeight="1">
       <c r="A1344" s="3">
         <v>42761</v>
       </c>
@@ -72066,7 +72298,7 @@
         <v>0.54097222222222219</v>
       </c>
       <c r="O1349" s="2">
-        <f>N1350*1440-M1349*1440</f>
+        <f t="shared" ref="O1349:O1354" si="23">N1350*1440-M1349*1440</f>
         <v>91</v>
       </c>
       <c r="Q1349" s="7" t="s">
@@ -72117,7 +72349,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="O1350" s="2">
-        <f>N1351*1440-M1350*1440</f>
+        <f t="shared" si="23"/>
         <v>91.999999999999886</v>
       </c>
       <c r="Q1350" s="7" t="s">
@@ -72168,7 +72400,7 @@
         <v>0.54305555555555551</v>
       </c>
       <c r="O1351" s="2">
-        <f>N1352*1440-M1351*1440</f>
+        <f t="shared" si="23"/>
         <v>92.000000000000114</v>
       </c>
       <c r="Q1351" s="7" t="s">
@@ -72219,7 +72451,7 @@
         <v>0.54375000000000007</v>
       </c>
       <c r="O1352" s="2">
-        <f>N1353*1440-M1352*1440</f>
+        <f t="shared" si="23"/>
         <v>92.000000000000114</v>
       </c>
       <c r="Q1352" s="7" t="s">
@@ -72270,7 +72502,7 @@
         <v>0.54513888888888895</v>
       </c>
       <c r="O1353" s="2">
-        <f>N1354*1440-M1353*1440</f>
+        <f t="shared" si="23"/>
         <v>91.999999999999886</v>
       </c>
       <c r="Q1353" s="7" t="s">
@@ -72321,7 +72553,7 @@
         <v>0.54583333333333328</v>
       </c>
       <c r="O1354" s="2">
-        <f>N1355*1440-M1354*1440</f>
+        <f t="shared" si="23"/>
         <v>91.000000000000114</v>
       </c>
       <c r="Q1354" s="7" t="s">
@@ -72398,11 +72630,33 @@
       <c r="F1356" t="s">
         <v>56</v>
       </c>
+      <c r="G1356" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1356" s="16">
+        <v>18.524000000000001</v>
+      </c>
+      <c r="I1356" s="16">
+        <v>19.507999999999999</v>
+      </c>
       <c r="J1356">
         <v>1</v>
       </c>
       <c r="K1356" s="1">
         <v>1</v>
+      </c>
+      <c r="L1356" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1356" s="18">
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="N1356" s="18">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="O1356" s="2">
+        <f>N1356*1440-M1356*1440</f>
+        <v>90</v>
       </c>
       <c r="Q1356" s="7" t="s">
         <v>66</v>
@@ -72427,11 +72681,33 @@
       <c r="F1357" t="s">
         <v>58</v>
       </c>
+      <c r="G1357" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1357" s="16">
+        <v>17.863</v>
+      </c>
+      <c r="I1357" s="16">
+        <v>19.21</v>
+      </c>
       <c r="J1357">
         <v>1</v>
       </c>
       <c r="K1357" s="1">
         <v>1</v>
+      </c>
+      <c r="L1357" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1357" s="18">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="N1357" s="18">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="O1357" s="2">
+        <f>N1357*1440-M1357*1440</f>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1357" s="7" t="s">
         <v>67</v>
@@ -72456,11 +72732,33 @@
       <c r="F1358" t="s">
         <v>28</v>
       </c>
+      <c r="G1358" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1358" s="16">
+        <v>17.704999999999998</v>
+      </c>
+      <c r="I1358" s="16">
+        <v>18.837</v>
+      </c>
       <c r="J1358">
         <v>1</v>
       </c>
       <c r="K1358" s="1">
         <v>1</v>
+      </c>
+      <c r="L1358" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1358" s="18">
+        <v>0.31875000000000003</v>
+      </c>
+      <c r="N1358" s="18">
+        <v>0.38125000000000003</v>
+      </c>
+      <c r="O1358" s="2">
+        <f t="shared" ref="O1358:O1421" si="24">N1358*1440-M1358*1440</f>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1358" s="7" t="s">
         <v>68</v>
@@ -72485,11 +72783,33 @@
       <c r="F1359" t="s">
         <v>30</v>
       </c>
+      <c r="G1359" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1359" s="16">
+        <v>17.841999999999999</v>
+      </c>
+      <c r="I1359" s="16">
+        <v>18.954000000000001</v>
+      </c>
       <c r="J1359">
         <v>1</v>
       </c>
       <c r="K1359" s="1">
         <v>1</v>
+      </c>
+      <c r="L1359" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1359" s="18">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="N1359" s="18">
+        <v>0.38263888888888892</v>
+      </c>
+      <c r="O1359" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1359" s="7" t="s">
         <v>69</v>
@@ -72514,11 +72834,33 @@
       <c r="F1360" t="s">
         <v>46</v>
       </c>
+      <c r="G1360" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1360" s="16">
+        <v>18.134</v>
+      </c>
+      <c r="I1360" s="16">
+        <v>19.350999999999999</v>
+      </c>
       <c r="J1360">
         <v>1</v>
       </c>
       <c r="K1360" s="1">
         <v>1</v>
+      </c>
+      <c r="L1360" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1360" s="18">
+        <v>0.32083333333333336</v>
+      </c>
+      <c r="N1360" s="18">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="O1360" s="2">
+        <f t="shared" si="24"/>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1360" s="7" t="s">
         <v>70</v>
@@ -72543,11 +72885,33 @@
       <c r="F1361" t="s">
         <v>54</v>
       </c>
+      <c r="G1361" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1361" s="16">
+        <v>18.315000000000001</v>
+      </c>
+      <c r="I1361" s="16">
+        <v>19.53</v>
+      </c>
       <c r="J1361">
         <v>1</v>
       </c>
       <c r="K1361" s="1">
         <v>1</v>
+      </c>
+      <c r="L1361" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1361" s="18">
+        <v>0.3215277777777778</v>
+      </c>
+      <c r="N1361" s="18">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="O1361" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1361" s="7" t="s">
         <v>71</v>
@@ -72572,11 +72936,33 @@
       <c r="F1362" t="s">
         <v>36</v>
       </c>
+      <c r="G1362" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1362" s="16">
+        <v>17.965</v>
+      </c>
+      <c r="I1362" s="16">
+        <v>19.145</v>
+      </c>
       <c r="J1362">
         <v>1</v>
       </c>
       <c r="K1362" s="1">
         <v>1</v>
+      </c>
+      <c r="L1362" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1362" s="18">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="N1362" s="18">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="O1362" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1362" s="7" t="s">
         <v>72</v>
@@ -72601,11 +72987,33 @@
       <c r="F1363" t="s">
         <v>52</v>
       </c>
+      <c r="G1363" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1363" s="16">
+        <v>18.132999999999999</v>
+      </c>
+      <c r="I1363" s="16">
+        <v>19.37</v>
+      </c>
       <c r="J1363">
         <v>1</v>
       </c>
       <c r="K1363" s="1">
         <v>1</v>
+      </c>
+      <c r="L1363" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1363" s="18">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="N1363" s="18">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="O1363" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1363" s="7" t="s">
         <v>73</v>
@@ -72630,11 +73038,33 @@
       <c r="F1364" t="s">
         <v>40</v>
       </c>
+      <c r="G1364" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="H1364" s="16">
+        <v>18.361000000000001</v>
+      </c>
+      <c r="I1364" s="16">
+        <v>19.707000000000001</v>
+      </c>
       <c r="J1364">
         <v>1</v>
       </c>
       <c r="K1364" s="1">
         <v>1</v>
+      </c>
+      <c r="L1364" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1364" s="18">
+        <v>0.32430555555555557</v>
+      </c>
+      <c r="N1364" s="18">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="O1364" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1364" s="7" t="s">
         <v>74</v>
@@ -72659,11 +73089,33 @@
       <c r="F1365" t="s">
         <v>26</v>
       </c>
+      <c r="G1365" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1365" s="16">
+        <v>18.16</v>
+      </c>
+      <c r="I1365" s="16">
+        <v>19.488</v>
+      </c>
       <c r="J1365">
         <v>1</v>
       </c>
       <c r="K1365" s="1">
         <v>1</v>
+      </c>
+      <c r="L1365" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1365" s="18">
+        <v>0.32569444444444445</v>
+      </c>
+      <c r="N1365" s="18">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="O1365" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1365" s="7" t="s">
         <v>75</v>
@@ -72688,11 +73140,33 @@
       <c r="F1366" t="s">
         <v>24</v>
       </c>
+      <c r="G1366" s="1">
+        <v>26</v>
+      </c>
+      <c r="H1366" s="16">
+        <v>17.712</v>
+      </c>
+      <c r="I1366" s="16">
+        <v>18.951000000000001</v>
+      </c>
       <c r="J1366">
         <v>2</v>
       </c>
       <c r="K1366" s="1">
         <v>1</v>
+      </c>
+      <c r="L1366" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1366" s="18">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="N1366" s="18">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="O1366" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1366" s="7" t="s">
         <v>76</v>
@@ -72717,11 +73191,33 @@
       <c r="F1367" t="s">
         <v>62</v>
       </c>
+      <c r="G1367" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1367" s="16">
+        <v>18.039000000000001</v>
+      </c>
+      <c r="I1367" s="16">
+        <v>19.145</v>
+      </c>
       <c r="J1367">
         <v>2</v>
       </c>
       <c r="K1367" s="1">
         <v>1</v>
+      </c>
+      <c r="L1367" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1367" s="18">
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="N1367" s="18">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="O1367" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1367" s="7" t="s">
         <v>77</v>
@@ -72746,11 +73242,33 @@
       <c r="F1368" t="s">
         <v>44</v>
       </c>
+      <c r="G1368" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1368" s="16">
+        <v>18.234000000000002</v>
+      </c>
+      <c r="I1368" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1368">
         <v>2</v>
       </c>
       <c r="K1368" s="1">
         <v>1</v>
+      </c>
+      <c r="L1368" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1368" s="18">
+        <v>0.36041666666666666</v>
+      </c>
+      <c r="N1368" s="18">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="O1368" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1368" s="7" t="s">
         <v>78</v>
@@ -72775,11 +73293,33 @@
       <c r="F1369" t="s">
         <v>42</v>
       </c>
+      <c r="G1369" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1369" s="16">
+        <v>18.39</v>
+      </c>
+      <c r="I1369" s="16">
+        <v>19.492000000000001</v>
+      </c>
       <c r="J1369">
         <v>2</v>
       </c>
       <c r="K1369" s="1">
         <v>1</v>
+      </c>
+      <c r="L1369" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1369" s="18">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="N1369" s="18">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="O1369" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1369" s="7" t="s">
         <v>79</v>
@@ -72804,11 +73344,33 @@
       <c r="F1370" t="s">
         <v>50</v>
       </c>
+      <c r="G1370" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1370" s="16">
+        <v>18.132000000000001</v>
+      </c>
+      <c r="I1370" s="16">
+        <v>19.213999999999999</v>
+      </c>
       <c r="J1370">
         <v>2</v>
       </c>
       <c r="K1370" s="1">
         <v>1</v>
+      </c>
+      <c r="L1370" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1370" s="18">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="N1370" s="18">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="O1370" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1370" s="7" t="s">
         <v>80</v>
@@ -72833,11 +73395,33 @@
       <c r="F1371" t="s">
         <v>32</v>
       </c>
+      <c r="G1371" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1371" s="16">
+        <v>18.186</v>
+      </c>
+      <c r="I1371" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1371">
         <v>2</v>
       </c>
       <c r="K1371" s="1">
         <v>1</v>
+      </c>
+      <c r="L1371" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1371" s="18">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="N1371" s="18">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="O1371" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1371" s="7" t="s">
         <v>81</v>
@@ -72862,11 +73446,33 @@
       <c r="F1372" t="s">
         <v>48</v>
       </c>
+      <c r="G1372" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1372" s="16">
+        <v>18.084</v>
+      </c>
+      <c r="I1372" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1372">
         <v>2</v>
       </c>
       <c r="K1372" s="1">
         <v>1</v>
+      </c>
+      <c r="L1372" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1372" s="18">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="N1372" s="18">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="O1372" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1372" s="7" t="s">
         <v>86</v>
@@ -72891,11 +73497,33 @@
       <c r="F1373" t="s">
         <v>60</v>
       </c>
+      <c r="G1373" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1373" s="16">
+        <v>18.132999999999999</v>
+      </c>
+      <c r="I1373" s="16">
+        <v>19.454999999999998</v>
+      </c>
       <c r="J1373">
         <v>2</v>
       </c>
       <c r="K1373" s="1">
         <v>1</v>
+      </c>
+      <c r="L1373" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1373" s="18">
+        <v>0.36527777777777781</v>
+      </c>
+      <c r="N1373" s="18">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="O1373" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1373" s="7" t="s">
         <v>85</v>
@@ -72920,11 +73548,33 @@
       <c r="F1374" t="s">
         <v>64</v>
       </c>
+      <c r="G1374" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1374" s="16">
+        <v>18</v>
+      </c>
+      <c r="I1374" s="16">
+        <v>19.158000000000001</v>
+      </c>
       <c r="J1374">
         <v>2</v>
       </c>
       <c r="K1374" s="1">
         <v>1</v>
+      </c>
+      <c r="L1374" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1374" s="18">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="N1374" s="18">
+        <v>0.4291666666666667</v>
+      </c>
+      <c r="O1374" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1374" s="7" t="s">
         <v>82</v>
@@ -72949,11 +73599,33 @@
       <c r="F1375" t="s">
         <v>34</v>
       </c>
+      <c r="G1375" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1375" s="16">
+        <v>48.195</v>
+      </c>
+      <c r="I1375" s="16">
+        <v>19.306000000000001</v>
+      </c>
       <c r="J1375">
         <v>2</v>
       </c>
       <c r="K1375" s="1">
         <v>1</v>
+      </c>
+      <c r="L1375" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1375" s="18">
+        <v>0.36736111111111108</v>
+      </c>
+      <c r="N1375" s="18">
+        <v>0.42986111111111108</v>
+      </c>
+      <c r="O1375" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1375" s="7" t="s">
         <v>83</v>
@@ -72978,11 +73650,33 @@
       <c r="F1376" t="s">
         <v>38</v>
       </c>
+      <c r="G1376" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1376" s="16">
+        <v>18.215</v>
+      </c>
+      <c r="I1376" s="16">
+        <v>19.52</v>
+      </c>
       <c r="J1376">
         <v>2</v>
       </c>
       <c r="K1376" s="1">
         <v>1</v>
+      </c>
+      <c r="L1376" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1376" s="18">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="N1376" s="18">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="O1376" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1376" s="7" t="s">
         <v>84</v>
@@ -73007,11 +73701,33 @@
       <c r="F1377" t="s">
         <v>56</v>
       </c>
+      <c r="G1377" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1377" s="16">
+        <v>18.524000000000001</v>
+      </c>
+      <c r="I1377" s="16">
+        <v>19.507999999999999</v>
+      </c>
       <c r="J1377">
         <v>1</v>
       </c>
       <c r="K1377" s="1">
         <v>2</v>
+      </c>
+      <c r="L1377" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1377" s="18">
+        <v>0.43472222222222223</v>
+      </c>
+      <c r="N1377" s="18">
+        <v>0.49722222222222223</v>
+      </c>
+      <c r="O1377" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1377" s="7" t="s">
         <v>66</v>
@@ -73036,11 +73752,33 @@
       <c r="F1378" t="s">
         <v>58</v>
       </c>
+      <c r="G1378" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1378" s="16">
+        <v>17.863</v>
+      </c>
+      <c r="I1378" s="16">
+        <v>19.21</v>
+      </c>
       <c r="J1378">
         <v>1</v>
       </c>
       <c r="K1378" s="1">
         <v>2</v>
+      </c>
+      <c r="L1378" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1378" s="18">
+        <v>0.43541666666666662</v>
+      </c>
+      <c r="N1378" s="18">
+        <v>0.49791666666666662</v>
+      </c>
+      <c r="O1378" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1378" s="7" t="s">
         <v>67</v>
@@ -73065,11 +73803,33 @@
       <c r="F1379" t="s">
         <v>28</v>
       </c>
+      <c r="G1379" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1379" s="16">
+        <v>17.704999999999998</v>
+      </c>
+      <c r="I1379" s="16">
+        <v>18.837</v>
+      </c>
       <c r="J1379">
         <v>1</v>
       </c>
       <c r="K1379" s="1">
         <v>2</v>
+      </c>
+      <c r="L1379" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1379" s="18">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="N1379" s="18">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="O1379" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1379" s="7" t="s">
         <v>68</v>
@@ -73094,11 +73854,33 @@
       <c r="F1380" t="s">
         <v>30</v>
       </c>
+      <c r="G1380" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1380" s="16">
+        <v>17.841999999999999</v>
+      </c>
+      <c r="I1380" s="16">
+        <v>18.954000000000001</v>
+      </c>
       <c r="J1380">
         <v>1</v>
       </c>
       <c r="K1380" s="1">
         <v>2</v>
+      </c>
+      <c r="L1380" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1380" s="18">
+        <v>0.4375</v>
+      </c>
+      <c r="N1380" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="O1380" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1380" s="7" t="s">
         <v>69</v>
@@ -73123,11 +73905,33 @@
       <c r="F1381" t="s">
         <v>46</v>
       </c>
+      <c r="G1381" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1381" s="16">
+        <v>18.134</v>
+      </c>
+      <c r="I1381" s="16">
+        <v>19.350999999999999</v>
+      </c>
       <c r="J1381">
         <v>1</v>
       </c>
       <c r="K1381" s="1">
         <v>2</v>
+      </c>
+      <c r="L1381" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1381" s="18">
+        <v>0.4381944444444445</v>
+      </c>
+      <c r="N1381" s="18">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="O1381" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1381" s="7" t="s">
         <v>70</v>
@@ -73152,11 +73956,33 @@
       <c r="F1382" t="s">
         <v>54</v>
       </c>
+      <c r="G1382" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1382" s="16">
+        <v>18.315000000000001</v>
+      </c>
+      <c r="I1382" s="16">
+        <v>19.53</v>
+      </c>
       <c r="J1382">
         <v>1</v>
       </c>
       <c r="K1382" s="1">
         <v>2</v>
+      </c>
+      <c r="L1382" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1382" s="18">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="N1382" s="18">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="O1382" s="2">
+        <f t="shared" si="24"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1382" s="7" t="s">
         <v>71</v>
@@ -73181,11 +74007,33 @@
       <c r="F1383" t="s">
         <v>36</v>
       </c>
+      <c r="G1383" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1383" s="16">
+        <v>17.965</v>
+      </c>
+      <c r="I1383" s="16">
+        <v>19.145</v>
+      </c>
       <c r="J1383">
         <v>1</v>
       </c>
       <c r="K1383" s="1">
         <v>2</v>
+      </c>
+      <c r="L1383" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1383" s="18">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="N1383" s="18">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="O1383" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1383" s="7" t="s">
         <v>72</v>
@@ -73210,11 +74058,33 @@
       <c r="F1384" t="s">
         <v>52</v>
       </c>
+      <c r="G1384" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1384" s="16">
+        <v>18.132999999999999</v>
+      </c>
+      <c r="I1384" s="16">
+        <v>19.37</v>
+      </c>
       <c r="J1384">
         <v>1</v>
       </c>
       <c r="K1384" s="1">
         <v>2</v>
+      </c>
+      <c r="L1384" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1384" s="18">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="N1384" s="18">
+        <v>0.50416666666666665</v>
+      </c>
+      <c r="O1384" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1384" s="7" t="s">
         <v>73</v>
@@ -73239,11 +74109,33 @@
       <c r="F1385" t="s">
         <v>40</v>
       </c>
+      <c r="G1385" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="H1385" s="16">
+        <v>18.361000000000001</v>
+      </c>
+      <c r="I1385" s="16">
+        <v>19.707000000000001</v>
+      </c>
       <c r="J1385">
         <v>1</v>
       </c>
       <c r="K1385" s="1">
         <v>2</v>
+      </c>
+      <c r="L1385" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1385" s="18">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="N1385" s="18">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="O1385" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1385" s="7" t="s">
         <v>74</v>
@@ -73268,11 +74160,33 @@
       <c r="F1386" t="s">
         <v>26</v>
       </c>
+      <c r="G1386" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1386" s="16">
+        <v>18.16</v>
+      </c>
+      <c r="I1386" s="16">
+        <v>19.488</v>
+      </c>
       <c r="J1386">
         <v>1</v>
       </c>
       <c r="K1386" s="1">
         <v>2</v>
+      </c>
+      <c r="L1386" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1386" s="18">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="N1386" s="18">
+        <v>0.50624999999999998</v>
+      </c>
+      <c r="O1386" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1386" s="7" t="s">
         <v>75</v>
@@ -73297,11 +74211,33 @@
       <c r="F1387" t="s">
         <v>24</v>
       </c>
+      <c r="G1387" s="1">
+        <v>26</v>
+      </c>
+      <c r="H1387" s="16">
+        <v>17.712</v>
+      </c>
+      <c r="I1387" s="16">
+        <v>18.951000000000001</v>
+      </c>
       <c r="J1387">
         <v>2</v>
       </c>
       <c r="K1387" s="1">
         <v>2</v>
+      </c>
+      <c r="L1387" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1387" s="18">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="N1387" s="18">
+        <v>0.54027777777777775</v>
+      </c>
+      <c r="O1387" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1387" s="7" t="s">
         <v>76</v>
@@ -73326,11 +74262,33 @@
       <c r="F1388" t="s">
         <v>62</v>
       </c>
+      <c r="G1388" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1388" s="16">
+        <v>18.039000000000001</v>
+      </c>
+      <c r="I1388" s="16">
+        <v>19.145</v>
+      </c>
       <c r="J1388">
         <v>2</v>
       </c>
       <c r="K1388" s="1">
         <v>2</v>
+      </c>
+      <c r="L1388" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1388" s="18">
+        <v>0.47847222222222219</v>
+      </c>
+      <c r="N1388" s="18">
+        <v>0.54097222222222219</v>
+      </c>
+      <c r="O1388" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1388" s="7" t="s">
         <v>77</v>
@@ -73355,11 +74313,33 @@
       <c r="F1389" t="s">
         <v>44</v>
       </c>
+      <c r="G1389" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1389" s="16">
+        <v>18.234000000000002</v>
+      </c>
+      <c r="I1389" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1389">
         <v>2</v>
       </c>
       <c r="K1389" s="1">
         <v>2</v>
+      </c>
+      <c r="L1389" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1389" s="18">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="N1389" s="18">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="O1389" s="2">
+        <f t="shared" si="24"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1389" s="7" t="s">
         <v>78</v>
@@ -73384,11 +74364,33 @@
       <c r="F1390" t="s">
         <v>42</v>
       </c>
+      <c r="G1390" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1390" s="16">
+        <v>18.39</v>
+      </c>
+      <c r="I1390" s="16">
+        <v>19.492000000000001</v>
+      </c>
       <c r="J1390">
         <v>2</v>
       </c>
       <c r="K1390" s="1">
         <v>2</v>
+      </c>
+      <c r="L1390" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1390" s="18">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="N1390" s="18">
+        <v>0.54305555555555551</v>
+      </c>
+      <c r="O1390" s="2">
+        <f t="shared" si="24"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1390" s="7" t="s">
         <v>79</v>
@@ -73413,11 +74415,33 @@
       <c r="F1391" t="s">
         <v>50</v>
       </c>
+      <c r="G1391" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1391" s="16">
+        <v>18.132000000000001</v>
+      </c>
+      <c r="I1391" s="16">
+        <v>19.213999999999999</v>
+      </c>
       <c r="J1391">
         <v>2</v>
       </c>
       <c r="K1391" s="1">
         <v>2</v>
+      </c>
+      <c r="L1391" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1391" s="18">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="N1391" s="18">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="O1391" s="2">
+        <f t="shared" si="24"/>
+        <v>92.999999999999886</v>
       </c>
       <c r="Q1391" s="7" t="s">
         <v>80</v>
@@ -73442,11 +74466,33 @@
       <c r="F1392" t="s">
         <v>32</v>
       </c>
+      <c r="G1392" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1392" s="16">
+        <v>18.186</v>
+      </c>
+      <c r="I1392" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1392">
         <v>2</v>
       </c>
       <c r="K1392" s="1">
         <v>2</v>
+      </c>
+      <c r="L1392" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1392" s="18">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="N1392" s="18">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="O1392" s="2">
+        <f t="shared" si="24"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1392" s="7" t="s">
         <v>81</v>
@@ -73471,11 +74517,33 @@
       <c r="F1393" t="s">
         <v>48</v>
       </c>
+      <c r="G1393" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1393" s="16">
+        <v>18.084</v>
+      </c>
+      <c r="I1393" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1393">
         <v>2</v>
       </c>
       <c r="K1393" s="1">
         <v>2</v>
+      </c>
+      <c r="L1393" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1393" s="18">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="N1393" s="18">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="O1393" s="2">
+        <f t="shared" si="24"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1393" s="7" t="s">
         <v>86</v>
@@ -73500,11 +74568,33 @@
       <c r="F1394" t="s">
         <v>60</v>
       </c>
+      <c r="G1394" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1394" s="16">
+        <v>18.132999999999999</v>
+      </c>
+      <c r="I1394" s="16">
+        <v>19.454999999999998</v>
+      </c>
       <c r="J1394">
         <v>2</v>
       </c>
       <c r="K1394" s="1">
         <v>2</v>
+      </c>
+      <c r="L1394" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1394" s="18">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="N1394" s="18">
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="O1394" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1394" s="7" t="s">
         <v>85</v>
@@ -73529,11 +74619,33 @@
       <c r="F1395" t="s">
         <v>64</v>
       </c>
+      <c r="G1395" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1395" s="16">
+        <v>18</v>
+      </c>
+      <c r="I1395" s="16">
+        <v>19.158000000000001</v>
+      </c>
       <c r="J1395">
         <v>2</v>
       </c>
       <c r="K1395" s="1">
         <v>2</v>
+      </c>
+      <c r="L1395" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1395" s="18">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="N1395" s="18">
+        <v>0.54791666666666672</v>
+      </c>
+      <c r="O1395" s="2">
+        <f t="shared" si="24"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1395" s="7" t="s">
         <v>82</v>
@@ -73558,11 +74670,33 @@
       <c r="F1396" t="s">
         <v>34</v>
       </c>
+      <c r="G1396" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1396" s="16">
+        <v>48.195</v>
+      </c>
+      <c r="I1396" s="16">
+        <v>19.306000000000001</v>
+      </c>
       <c r="J1396">
         <v>2</v>
       </c>
       <c r="K1396" s="1">
         <v>2</v>
+      </c>
+      <c r="L1396" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1396" s="18">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="N1396" s="18">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="O1396" s="2">
+        <f t="shared" si="24"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1396" s="7" t="s">
         <v>83</v>
@@ -73587,11 +74721,33 @@
       <c r="F1397" t="s">
         <v>38</v>
       </c>
+      <c r="G1397" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1397" s="16">
+        <v>18.215</v>
+      </c>
+      <c r="I1397" s="16">
+        <v>19.52</v>
+      </c>
       <c r="J1397">
         <v>2</v>
       </c>
       <c r="K1397" s="1">
         <v>2</v>
+      </c>
+      <c r="L1397" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1397" s="18">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="N1397" s="18">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="O1397" s="2">
+        <f t="shared" si="24"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1397" s="7" t="s">
         <v>84</v>
@@ -73624,11 +74780,33 @@
       <c r="F1399" t="s">
         <v>122</v>
       </c>
+      <c r="G1399" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1399" s="16">
+        <v>18.536999999999999</v>
+      </c>
+      <c r="I1399" s="16">
+        <v>19.613</v>
+      </c>
       <c r="J1399">
         <v>1</v>
       </c>
       <c r="K1399" s="1">
         <v>1</v>
+      </c>
+      <c r="L1399" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1399" s="18">
+        <v>0.31527777777777777</v>
+      </c>
+      <c r="N1399" s="18">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="O1399" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1399" s="7" t="s">
         <v>66</v>
@@ -73653,11 +74831,33 @@
       <c r="F1400" t="s">
         <v>108</v>
       </c>
+      <c r="G1400" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1400" s="16">
+        <v>17.863</v>
+      </c>
+      <c r="I1400" s="16">
+        <v>19.087</v>
+      </c>
       <c r="J1400">
         <v>1</v>
       </c>
       <c r="K1400" s="1">
         <v>1</v>
+      </c>
+      <c r="L1400" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1400" s="18">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="N1400" s="18">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="O1400" s="2">
+        <f t="shared" si="24"/>
+        <v>30.000000000000057</v>
       </c>
       <c r="Q1400" s="7" t="s">
         <v>67</v>
@@ -73682,11 +74882,33 @@
       <c r="F1401" t="s">
         <v>100</v>
       </c>
+      <c r="G1401" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1401" s="16">
+        <v>17.731999999999999</v>
+      </c>
+      <c r="I1401" s="16">
+        <v>18.858000000000001</v>
+      </c>
       <c r="J1401">
         <v>1</v>
       </c>
       <c r="K1401" s="1">
         <v>1</v>
+      </c>
+      <c r="L1401" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1401" s="18">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="N1401" s="18">
+        <v>3.754861111111111</v>
+      </c>
+      <c r="O1401" s="2">
+        <f t="shared" si="24"/>
+        <v>4950</v>
       </c>
       <c r="Q1401" s="7" t="s">
         <v>68</v>
@@ -73711,11 +74933,33 @@
       <c r="F1402" t="s">
         <v>112</v>
       </c>
+      <c r="G1402" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1402" s="16">
+        <v>17.920999999999999</v>
+      </c>
+      <c r="I1402" s="16">
+        <v>19.177</v>
+      </c>
       <c r="J1402">
         <v>1</v>
       </c>
       <c r="K1402" s="1">
         <v>1</v>
+      </c>
+      <c r="L1402" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1402" s="18">
+        <v>0.31805555555555554</v>
+      </c>
+      <c r="N1402" s="18">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="O1402" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1402" s="7" t="s">
         <v>69</v>
@@ -73740,11 +74984,33 @@
       <c r="F1403" t="s">
         <v>126</v>
       </c>
+      <c r="G1403" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1403" s="16">
+        <v>18.170999999999999</v>
+      </c>
+      <c r="I1403" s="16">
+        <v>19.535</v>
+      </c>
       <c r="J1403">
         <v>1</v>
       </c>
       <c r="K1403" s="1">
         <v>1</v>
+      </c>
+      <c r="L1403" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1403" s="18">
+        <v>0.31875000000000003</v>
+      </c>
+      <c r="N1403" s="18">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="O1403" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1403" s="7" t="s">
         <v>70</v>
@@ -73769,11 +75035,33 @@
       <c r="F1404" t="s">
         <v>116</v>
       </c>
+      <c r="G1404" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1404" s="16">
+        <v>18.356999999999999</v>
+      </c>
+      <c r="I1404" s="16">
+        <v>19.709</v>
+      </c>
       <c r="J1404">
         <v>1</v>
       </c>
       <c r="K1404" s="1">
         <v>1</v>
+      </c>
+      <c r="L1404" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1404" s="18">
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="N1404" s="18">
+        <v>0.38263888888888892</v>
+      </c>
+      <c r="O1404" s="2">
+        <f t="shared" si="24"/>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1404" s="7" t="s">
         <v>71</v>
@@ -73798,11 +75086,33 @@
       <c r="F1405" t="s">
         <v>98</v>
       </c>
+      <c r="G1405" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1405" s="16">
+        <v>18.047999999999998</v>
+      </c>
+      <c r="I1405" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1405">
         <v>1</v>
       </c>
       <c r="K1405" s="1">
         <v>1</v>
+      </c>
+      <c r="L1405" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1405" s="18">
+        <v>0.32083333333333336</v>
+      </c>
+      <c r="N1405" s="18">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="O1405" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1405" s="7" t="s">
         <v>72</v>
@@ -73827,11 +75137,33 @@
       <c r="F1406" t="s">
         <v>106</v>
       </c>
+      <c r="G1406" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1406" s="16">
+        <v>18.138999999999999</v>
+      </c>
+      <c r="I1406" s="16">
+        <v>19.245000000000001</v>
+      </c>
       <c r="J1406">
         <v>1</v>
       </c>
       <c r="K1406" s="1">
         <v>1</v>
+      </c>
+      <c r="L1406" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1406" s="18">
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="N1406" s="18">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="O1406" s="2">
+        <f t="shared" si="24"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1406" s="7" t="s">
         <v>73</v>
@@ -73856,11 +75188,33 @@
       <c r="F1407" t="s">
         <v>102</v>
       </c>
+      <c r="G1407" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1407" s="16">
+        <v>18.388000000000002</v>
+      </c>
+      <c r="I1407" s="16">
+        <v>19.712</v>
+      </c>
       <c r="J1407">
         <v>1</v>
       </c>
       <c r="K1407" s="1">
         <v>1</v>
+      </c>
+      <c r="L1407" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1407" s="18">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="N1407" s="18">
+        <v>0.38611111111111113</v>
+      </c>
+      <c r="O1407" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1407" s="7" t="s">
         <v>74</v>
@@ -73885,11 +75239,33 @@
       <c r="F1408" t="s">
         <v>118</v>
       </c>
+      <c r="G1408" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1408" s="16">
+        <v>18.167999999999999</v>
+      </c>
+      <c r="I1408" s="16">
+        <v>19.231999999999999</v>
+      </c>
       <c r="J1408">
         <v>1</v>
       </c>
       <c r="K1408" s="1">
         <v>1</v>
+      </c>
+      <c r="L1408" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1408" s="18">
+        <v>0.32430555555555557</v>
+      </c>
+      <c r="N1408" s="18">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="O1408" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1408" s="7" t="s">
         <v>75</v>
@@ -73914,11 +75290,33 @@
       <c r="F1409" t="s">
         <v>96</v>
       </c>
+      <c r="G1409" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1409" s="16">
+        <v>17.742000000000001</v>
+      </c>
+      <c r="I1409" s="16">
+        <v>19.103000000000002</v>
+      </c>
       <c r="J1409">
         <v>2</v>
       </c>
       <c r="K1409" s="1">
         <v>1</v>
+      </c>
+      <c r="L1409" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1409" s="18">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="N1409" s="18">
+        <v>0.41944444444444445</v>
+      </c>
+      <c r="O1409" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1409" s="7" t="s">
         <v>76</v>
@@ -73943,11 +75341,33 @@
       <c r="F1410" t="s">
         <v>136</v>
       </c>
+      <c r="G1410" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1410" s="16">
+        <v>18.053000000000001</v>
+      </c>
+      <c r="I1410" s="16">
+        <v>19.335000000000001</v>
+      </c>
       <c r="J1410">
         <v>2</v>
       </c>
       <c r="K1410" s="1">
         <v>1</v>
+      </c>
+      <c r="L1410" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1410" s="18">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="N1410" s="18">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="O1410" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1410" s="7" t="s">
         <v>77</v>
@@ -73972,11 +75392,33 @@
       <c r="F1411" t="s">
         <v>132</v>
       </c>
+      <c r="G1411" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1411" s="16">
+        <v>18.241</v>
+      </c>
+      <c r="I1411" s="16">
+        <v>19.207000000000001</v>
+      </c>
       <c r="J1411">
         <v>2</v>
       </c>
       <c r="K1411" s="1">
         <v>1</v>
+      </c>
+      <c r="L1411" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1411" s="18">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="N1411" s="18">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="O1411" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1411" s="7" t="s">
         <v>78</v>
@@ -74001,11 +75443,33 @@
       <c r="F1412" t="s">
         <v>104</v>
       </c>
+      <c r="G1412" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1412" s="16">
+        <v>18.39</v>
+      </c>
+      <c r="I1412" s="16">
+        <v>19.513000000000002</v>
+      </c>
       <c r="J1412">
         <v>2</v>
       </c>
       <c r="K1412" s="1">
         <v>1</v>
+      </c>
+      <c r="L1412" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1412" s="18">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="N1412" s="18">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="O1412" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1412" s="7" t="s">
         <v>79</v>
@@ -74030,11 +75494,33 @@
       <c r="F1413" t="s">
         <v>124</v>
       </c>
+      <c r="G1413" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1413" s="16">
+        <v>18.131</v>
+      </c>
+      <c r="I1413" s="16">
+        <v>19.38</v>
+      </c>
       <c r="J1413">
         <v>2</v>
       </c>
       <c r="K1413" s="1">
         <v>1</v>
+      </c>
+      <c r="L1413" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1413" s="18">
+        <v>0.36041666666666666</v>
+      </c>
+      <c r="N1413" s="18">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="O1413" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1413" s="7" t="s">
         <v>80</v>
@@ -74059,11 +75545,33 @@
       <c r="F1414" t="s">
         <v>130</v>
       </c>
+      <c r="G1414" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1414" s="16">
+        <v>18.193999999999999</v>
+      </c>
+      <c r="I1414" s="16">
+        <v>19.361999999999998</v>
+      </c>
       <c r="J1414">
         <v>2</v>
       </c>
       <c r="K1414" s="1">
         <v>1</v>
+      </c>
+      <c r="L1414" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1414" s="18">
+        <v>0.36180555555555555</v>
+      </c>
+      <c r="N1414" s="18">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="O1414" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1414" s="7" t="s">
         <v>81</v>
@@ -74088,11 +75596,33 @@
       <c r="F1415" t="s">
         <v>128</v>
       </c>
+      <c r="G1415" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1415" s="16">
+        <v>18.076000000000001</v>
+      </c>
+      <c r="I1415" s="16">
+        <v>19.423999999999999</v>
+      </c>
       <c r="J1415">
         <v>2</v>
       </c>
       <c r="K1415" s="1">
         <v>1</v>
+      </c>
+      <c r="L1415" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1415" s="18">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="N1415" s="18">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="O1415" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1415" s="7" t="s">
         <v>86</v>
@@ -74117,11 +75647,33 @@
       <c r="F1416" t="s">
         <v>120</v>
       </c>
+      <c r="G1416" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1416" s="16">
+        <v>18.145</v>
+      </c>
+      <c r="I1416" s="16">
+        <v>19.213000000000001</v>
+      </c>
       <c r="J1416">
         <v>2</v>
       </c>
       <c r="K1416" s="1">
         <v>1</v>
+      </c>
+      <c r="L1416" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1416" s="18">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="N1416" s="18">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="O1416" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1416" s="7" t="s">
         <v>85</v>
@@ -74146,11 +75698,33 @@
       <c r="F1417" t="s">
         <v>134</v>
       </c>
+      <c r="G1417" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1417" s="16">
+        <v>17.995000000000001</v>
+      </c>
+      <c r="I1417" s="16">
+        <v>19.241</v>
+      </c>
       <c r="J1417">
         <v>2</v>
       </c>
       <c r="K1417" s="1">
         <v>1</v>
+      </c>
+      <c r="L1417" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1417" s="18">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="N1417" s="18">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="O1417" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1417" s="7" t="s">
         <v>82</v>
@@ -74175,11 +75749,33 @@
       <c r="F1418" t="s">
         <v>110</v>
       </c>
+      <c r="G1418" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1418" s="16">
+        <v>18.234000000000002</v>
+      </c>
+      <c r="I1418" s="16">
+        <v>19.338999999999999</v>
+      </c>
       <c r="J1418">
         <v>2</v>
       </c>
       <c r="K1418" s="1">
         <v>1</v>
+      </c>
+      <c r="L1418" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1418" s="18">
+        <v>0.36527777777777781</v>
+      </c>
+      <c r="N1418" s="18">
+        <v>0.4291666666666667</v>
+      </c>
+      <c r="O1418" s="2">
+        <f t="shared" si="24"/>
+        <v>92</v>
       </c>
       <c r="Q1418" s="7" t="s">
         <v>83</v>
@@ -74204,11 +75800,33 @@
       <c r="F1419" t="s">
         <v>114</v>
       </c>
+      <c r="G1419" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1419" s="16">
+        <v>18.210999999999999</v>
+      </c>
+      <c r="I1419" s="16">
+        <v>19.544</v>
+      </c>
       <c r="J1419">
         <v>2</v>
       </c>
       <c r="K1419" s="1">
         <v>1</v>
+      </c>
+      <c r="L1419" s="1">
+        <v>28</v>
+      </c>
+      <c r="M1419" s="18">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="N1419" s="18">
+        <v>0.42986111111111108</v>
+      </c>
+      <c r="O1419" s="2">
+        <f t="shared" si="24"/>
+        <v>91</v>
       </c>
       <c r="Q1419" s="7" t="s">
         <v>84</v>
@@ -74233,11 +75851,33 @@
       <c r="F1420" t="s">
         <v>122</v>
       </c>
+      <c r="G1420" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1420" s="16">
+        <v>18.536999999999999</v>
+      </c>
+      <c r="I1420" s="16">
+        <v>19.613</v>
+      </c>
       <c r="J1420">
         <v>1</v>
       </c>
       <c r="K1420" s="1">
         <v>2</v>
+      </c>
+      <c r="L1420" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1420" s="18">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="N1420" s="18">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="O1420" s="2">
+        <f t="shared" si="24"/>
+        <v>90</v>
       </c>
       <c r="Q1420" s="7" t="s">
         <v>66</v>
@@ -74262,11 +75902,33 @@
       <c r="F1421" t="s">
         <v>108</v>
       </c>
+      <c r="G1421" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1421" s="16">
+        <v>17.863</v>
+      </c>
+      <c r="I1421" s="16">
+        <v>19.087</v>
+      </c>
       <c r="J1421">
         <v>1</v>
       </c>
       <c r="K1421" s="1">
         <v>2</v>
+      </c>
+      <c r="L1421" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1421" s="18">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="N1421" s="18">
+        <v>0.49722222222222223</v>
+      </c>
+      <c r="O1421" s="2">
+        <f t="shared" si="24"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1421" s="7" t="s">
         <v>67</v>
@@ -74291,11 +75953,33 @@
       <c r="F1422" t="s">
         <v>100</v>
       </c>
+      <c r="G1422" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1422" s="16">
+        <v>17.731999999999999</v>
+      </c>
+      <c r="I1422" s="16">
+        <v>18.858000000000001</v>
+      </c>
       <c r="J1422">
         <v>1</v>
       </c>
       <c r="K1422" s="1">
         <v>2</v>
+      </c>
+      <c r="L1422" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1422" s="18">
+        <v>0.43541666666666662</v>
+      </c>
+      <c r="N1422" s="18">
+        <v>0.49791666666666662</v>
+      </c>
+      <c r="O1422" s="2">
+        <f t="shared" ref="O1422:O1482" si="25">N1422*1440-M1422*1440</f>
+        <v>90</v>
       </c>
       <c r="Q1422" s="7" t="s">
         <v>68</v>
@@ -74320,11 +76004,33 @@
       <c r="F1423" t="s">
         <v>112</v>
       </c>
+      <c r="G1423" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1423" s="16">
+        <v>17.920999999999999</v>
+      </c>
+      <c r="I1423" s="16">
+        <v>19.177</v>
+      </c>
       <c r="J1423">
         <v>1</v>
       </c>
       <c r="K1423" s="1">
         <v>2</v>
+      </c>
+      <c r="L1423" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1423" s="18">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="N1423" s="18">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="O1423" s="2">
+        <f t="shared" si="25"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1423" s="7" t="s">
         <v>69</v>
@@ -74349,11 +76055,33 @@
       <c r="F1424" t="s">
         <v>126</v>
       </c>
+      <c r="G1424" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1424" s="16">
+        <v>18.170999999999999</v>
+      </c>
+      <c r="I1424" s="16">
+        <v>19.535</v>
+      </c>
       <c r="J1424">
         <v>1</v>
       </c>
       <c r="K1424" s="1">
         <v>2</v>
+      </c>
+      <c r="L1424" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1424" s="18">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="N1424" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="O1424" s="2">
+        <f t="shared" si="25"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1424" s="7" t="s">
         <v>70</v>
@@ -74378,11 +76106,33 @@
       <c r="F1425" t="s">
         <v>116</v>
       </c>
+      <c r="G1425" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1425" s="16">
+        <v>18.356999999999999</v>
+      </c>
+      <c r="I1425" s="16">
+        <v>19.709</v>
+      </c>
       <c r="J1425">
         <v>1</v>
       </c>
       <c r="K1425" s="1">
         <v>2</v>
+      </c>
+      <c r="L1425" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1425" s="18">
+        <v>0.4381944444444445</v>
+      </c>
+      <c r="N1425" s="18">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="O1425" s="2">
+        <f t="shared" si="25"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1425" s="7" t="s">
         <v>71</v>
@@ -74407,11 +76157,33 @@
       <c r="F1426" t="s">
         <v>98</v>
       </c>
+      <c r="G1426" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1426" s="16">
+        <v>18.047999999999998</v>
+      </c>
+      <c r="I1426" s="16">
+        <v>19.369</v>
+      </c>
       <c r="J1426">
         <v>1</v>
       </c>
       <c r="K1426" s="1">
         <v>2</v>
+      </c>
+      <c r="L1426" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1426" s="18">
+        <v>0.43888888888888888</v>
+      </c>
+      <c r="N1426" s="18">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="O1426" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1426" s="7" t="s">
         <v>72</v>
@@ -74436,11 +76208,33 @@
       <c r="F1427" t="s">
         <v>106</v>
       </c>
+      <c r="G1427" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1427" s="16">
+        <v>18.138999999999999</v>
+      </c>
+      <c r="I1427" s="16">
+        <v>19.245000000000001</v>
+      </c>
       <c r="J1427">
         <v>1</v>
       </c>
       <c r="K1427" s="1">
         <v>2</v>
+      </c>
+      <c r="L1427" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1427" s="18">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="N1427" s="18">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="O1427" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1427" s="7" t="s">
         <v>73</v>
@@ -74465,11 +76259,33 @@
       <c r="F1428" t="s">
         <v>102</v>
       </c>
+      <c r="G1428" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1428" s="16">
+        <v>18.388000000000002</v>
+      </c>
+      <c r="I1428" s="16">
+        <v>19.712</v>
+      </c>
       <c r="J1428">
         <v>1</v>
       </c>
       <c r="K1428" s="1">
         <v>2</v>
+      </c>
+      <c r="L1428" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1428" s="18">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="N1428" s="18">
+        <v>0.50416666666666665</v>
+      </c>
+      <c r="O1428" s="2">
+        <f t="shared" si="25"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1428" s="7" t="s">
         <v>74</v>
@@ -74494,11 +76310,33 @@
       <c r="F1429" t="s">
         <v>118</v>
       </c>
+      <c r="G1429" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1429" s="16">
+        <v>18.167999999999999</v>
+      </c>
+      <c r="I1429" s="16">
+        <v>19.231999999999999</v>
+      </c>
       <c r="J1429">
         <v>1</v>
       </c>
       <c r="K1429" s="1">
         <v>2</v>
+      </c>
+      <c r="L1429" s="1">
+        <v>30</v>
+      </c>
+      <c r="M1429" s="18">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="N1429" s="18">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="O1429" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1429" s="7" t="s">
         <v>75</v>
@@ -74523,11 +76361,33 @@
       <c r="F1430" t="s">
         <v>96</v>
       </c>
+      <c r="G1430" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1430" s="16">
+        <v>17.742000000000001</v>
+      </c>
+      <c r="I1430" s="16">
+        <v>19.103000000000002</v>
+      </c>
       <c r="J1430">
         <v>2</v>
       </c>
       <c r="K1430" s="1">
         <v>2</v>
+      </c>
+      <c r="L1430" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1430" s="18">
+        <v>0.47638888888888892</v>
+      </c>
+      <c r="N1430" s="18">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="O1430" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1430" s="7" t="s">
         <v>76</v>
@@ -74552,11 +76412,33 @@
       <c r="F1431" t="s">
         <v>136</v>
       </c>
+      <c r="G1431" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1431" s="16">
+        <v>18.053000000000001</v>
+      </c>
+      <c r="I1431" s="16">
+        <v>19.335000000000001</v>
+      </c>
       <c r="J1431">
         <v>2</v>
       </c>
       <c r="K1431" s="1">
         <v>2</v>
+      </c>
+      <c r="L1431" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1431" s="18">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="N1431" s="18">
+        <v>0.5395833333333333</v>
+      </c>
+      <c r="O1431" s="2">
+        <f t="shared" si="25"/>
+        <v>89</v>
       </c>
       <c r="Q1431" s="7" t="s">
         <v>77</v>
@@ -74581,11 +76463,33 @@
       <c r="F1432" t="s">
         <v>132</v>
       </c>
+      <c r="G1432" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1432" s="16">
+        <v>18.241</v>
+      </c>
+      <c r="I1432" s="16">
+        <v>19.207000000000001</v>
+      </c>
       <c r="J1432">
         <v>2</v>
       </c>
       <c r="K1432" s="1">
         <v>2</v>
+      </c>
+      <c r="L1432" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1432" s="18">
+        <v>0.47847222222222219</v>
+      </c>
+      <c r="N1432" s="18">
+        <v>0.54097222222222219</v>
+      </c>
+      <c r="O1432" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1432" s="7" t="s">
         <v>78</v>
@@ -74610,11 +76514,33 @@
       <c r="F1433" t="s">
         <v>104</v>
       </c>
+      <c r="G1433" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1433" s="16">
+        <v>18.39</v>
+      </c>
+      <c r="I1433" s="16">
+        <v>19.513000000000002</v>
+      </c>
       <c r="J1433">
         <v>2</v>
       </c>
       <c r="K1433" s="1">
         <v>2</v>
+      </c>
+      <c r="L1433" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1433" s="18">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="N1433" s="18">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="O1433" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1433" s="7" t="s">
         <v>79</v>
@@ -74639,11 +76565,33 @@
       <c r="F1434" t="s">
         <v>124</v>
       </c>
+      <c r="G1434" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1434" s="16">
+        <v>18.131</v>
+      </c>
+      <c r="I1434" s="16">
+        <v>19.38</v>
+      </c>
       <c r="J1434">
         <v>2</v>
       </c>
       <c r="K1434" s="1">
         <v>2</v>
+      </c>
+      <c r="L1434" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1434" s="18">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="N1434" s="18">
+        <v>0.54305555555555551</v>
+      </c>
+      <c r="O1434" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1434" s="7" t="s">
         <v>80</v>
@@ -74668,11 +76616,33 @@
       <c r="F1435" t="s">
         <v>130</v>
       </c>
+      <c r="G1435" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1435" s="16">
+        <v>18.193999999999999</v>
+      </c>
+      <c r="I1435" s="16">
+        <v>19.361999999999998</v>
+      </c>
       <c r="J1435">
         <v>2</v>
       </c>
       <c r="K1435" s="1">
         <v>2</v>
+      </c>
+      <c r="L1435" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1435" s="18">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="N1435" s="18">
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="O1435" s="2">
+        <f t="shared" si="25"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1435" s="7" t="s">
         <v>81</v>
@@ -74697,11 +76667,33 @@
       <c r="F1436" t="s">
         <v>128</v>
       </c>
+      <c r="G1436" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1436" s="16">
+        <v>18.076000000000001</v>
+      </c>
+      <c r="I1436" s="16">
+        <v>19.423999999999999</v>
+      </c>
       <c r="J1436">
         <v>2</v>
       </c>
       <c r="K1436" s="1">
         <v>2</v>
+      </c>
+      <c r="L1436" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1436" s="18">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="N1436" s="18">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="O1436" s="2">
+        <f t="shared" si="25"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1436" s="7" t="s">
         <v>86</v>
@@ -74726,11 +76718,33 @@
       <c r="F1437" t="s">
         <v>120</v>
       </c>
+      <c r="G1437" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1437" s="16">
+        <v>18.145</v>
+      </c>
+      <c r="I1437" s="16">
+        <v>19.213000000000001</v>
+      </c>
       <c r="J1437">
         <v>2</v>
       </c>
       <c r="K1437" s="1">
         <v>2</v>
+      </c>
+      <c r="L1437" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1437" s="18">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="N1437" s="18">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="O1437" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1437" s="7" t="s">
         <v>85</v>
@@ -74755,11 +76769,33 @@
       <c r="F1438" t="s">
         <v>134</v>
       </c>
+      <c r="G1438" s="1">
+        <v>23</v>
+      </c>
+      <c r="H1438" s="16">
+        <v>17.995000000000001</v>
+      </c>
+      <c r="I1438" s="16">
+        <v>19.241</v>
+      </c>
       <c r="J1438">
         <v>2</v>
       </c>
       <c r="K1438" s="1">
         <v>2</v>
+      </c>
+      <c r="L1438" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1438" s="18">
+        <v>0.48472222222222222</v>
+      </c>
+      <c r="N1438" s="18">
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="O1438" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1438" s="7" t="s">
         <v>82</v>
@@ -74784,11 +76820,33 @@
       <c r="F1439" t="s">
         <v>110</v>
       </c>
+      <c r="G1439" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1439" s="16">
+        <v>18.234000000000002</v>
+      </c>
+      <c r="I1439" s="16">
+        <v>19.338999999999999</v>
+      </c>
       <c r="J1439">
         <v>2</v>
       </c>
       <c r="K1439" s="1">
         <v>2</v>
+      </c>
+      <c r="L1439" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1439" s="18">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="N1439" s="18">
+        <v>0.54791666666666672</v>
+      </c>
+      <c r="O1439" s="2">
+        <f t="shared" si="25"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1439" s="7" t="s">
         <v>83</v>
@@ -74813,11 +76871,33 @@
       <c r="F1440" t="s">
         <v>114</v>
       </c>
+      <c r="G1440" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1440" s="16">
+        <v>18.210999999999999</v>
+      </c>
+      <c r="I1440" s="16">
+        <v>19.544</v>
+      </c>
       <c r="J1440">
         <v>2</v>
       </c>
       <c r="K1440" s="1">
         <v>2</v>
+      </c>
+      <c r="L1440" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1440" s="18">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="N1440" s="18">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="O1440" s="2">
+        <f t="shared" si="25"/>
+        <v>90.000000000000114</v>
       </c>
       <c r="Q1440" s="7" t="s">
         <v>84</v>
@@ -74842,11 +76922,33 @@
       <c r="F1441" t="s">
         <v>122</v>
       </c>
+      <c r="G1441" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1441" s="16">
+        <v>18.587</v>
+      </c>
+      <c r="I1441" s="16">
+        <v>19.638000000000002</v>
+      </c>
       <c r="J1441">
         <v>1</v>
       </c>
       <c r="K1441" s="1">
         <v>1</v>
+      </c>
+      <c r="L1441" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1441" s="18">
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="N1441" s="18">
+        <v>0.37083333333333335</v>
+      </c>
+      <c r="O1441" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1441" s="7" t="s">
         <v>66</v>
@@ -74871,11 +76973,33 @@
       <c r="F1442" t="s">
         <v>108</v>
       </c>
+      <c r="G1442" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1442" s="16">
+        <v>17.878</v>
+      </c>
+      <c r="I1442" s="16">
+        <v>19.052</v>
+      </c>
       <c r="J1442">
         <v>1</v>
       </c>
       <c r="K1442" s="1">
         <v>1</v>
+      </c>
+      <c r="L1442" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1442" s="18">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="N1442" s="18">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="O1442" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1442" s="7" t="s">
         <v>67</v>
@@ -74900,11 +77024,33 @@
       <c r="F1443" t="s">
         <v>100</v>
       </c>
+      <c r="G1443" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1443" s="16">
+        <v>17.739000000000001</v>
+      </c>
+      <c r="I1443" s="16">
+        <v>18.838000000000001</v>
+      </c>
       <c r="J1443">
         <v>1</v>
       </c>
       <c r="K1443" s="1">
         <v>1</v>
+      </c>
+      <c r="L1443" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1443" s="18">
+        <v>0.30972222222222223</v>
+      </c>
+      <c r="N1443" s="18">
+        <v>0.37291666666666662</v>
+      </c>
+      <c r="O1443" s="2">
+        <f t="shared" si="25"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1443" s="7" t="s">
         <v>68</v>
@@ -74929,11 +77075,33 @@
       <c r="F1444" t="s">
         <v>112</v>
       </c>
+      <c r="G1444" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1444" s="16">
+        <v>17.943000000000001</v>
+      </c>
+      <c r="I1444" s="16">
+        <v>19.164000000000001</v>
+      </c>
       <c r="J1444">
         <v>1</v>
       </c>
       <c r="K1444" s="1">
         <v>1</v>
+      </c>
+      <c r="L1444" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1444" s="18">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="N1444" s="18">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="O1444" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1444" s="7" t="s">
         <v>69</v>
@@ -74958,11 +77126,33 @@
       <c r="F1445" t="s">
         <v>126</v>
       </c>
+      <c r="G1445" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1445" s="16">
+        <v>18.187999999999999</v>
+      </c>
+      <c r="I1445" s="16">
+        <v>19.544</v>
+      </c>
       <c r="J1445">
         <v>1</v>
       </c>
       <c r="K1445" s="1">
         <v>1</v>
+      </c>
+      <c r="L1445" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1445" s="18">
+        <v>0.31180555555555556</v>
+      </c>
+      <c r="N1445" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="O1445" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1445" s="7" t="s">
         <v>70</v>
@@ -74987,11 +77177,33 @@
       <c r="F1446" t="s">
         <v>116</v>
       </c>
+      <c r="G1446" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1446" s="16">
+        <v>18.399000000000001</v>
+      </c>
+      <c r="I1446" s="16">
+        <v>19.741</v>
+      </c>
       <c r="J1446">
         <v>1</v>
       </c>
       <c r="K1446" s="1">
         <v>1</v>
+      </c>
+      <c r="L1446" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1446" s="18">
+        <v>0.3125</v>
+      </c>
+      <c r="N1446" s="18">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="O1446" s="2">
+        <f t="shared" si="25"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1446" s="7" t="s">
         <v>71</v>
@@ -75016,11 +77228,33 @@
       <c r="F1447" t="s">
         <v>98</v>
       </c>
+      <c r="G1447" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1447" s="16">
+        <v>18.009</v>
+      </c>
+      <c r="I1447" s="16">
+        <v>19.329999999999998</v>
+      </c>
       <c r="J1447">
         <v>1</v>
       </c>
       <c r="K1447" s="1">
         <v>1</v>
+      </c>
+      <c r="L1447" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1447" s="18">
+        <v>0.31388888888888888</v>
+      </c>
+      <c r="N1447" s="18">
+        <v>0.37708333333333338</v>
+      </c>
+      <c r="O1447" s="2">
+        <f t="shared" si="25"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1447" s="7" t="s">
         <v>72</v>
@@ -75045,11 +77279,33 @@
       <c r="F1448" t="s">
         <v>106</v>
       </c>
+      <c r="G1448" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1448" s="16">
+        <v>18.132000000000001</v>
+      </c>
+      <c r="I1448" s="16">
+        <v>19.202000000000002</v>
+      </c>
       <c r="J1448">
         <v>1</v>
       </c>
       <c r="K1448" s="1">
         <v>1</v>
+      </c>
+      <c r="L1448" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1448" s="18">
+        <v>0.31458333333333333</v>
+      </c>
+      <c r="N1448" s="18">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="O1448" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1448" s="7" t="s">
         <v>73</v>
@@ -75074,11 +77330,33 @@
       <c r="F1449" t="s">
         <v>102</v>
       </c>
+      <c r="G1449" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1449" s="16">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="I1449" s="16">
+        <v>19.684000000000001</v>
+      </c>
       <c r="J1449">
         <v>1</v>
       </c>
       <c r="K1449" s="1">
         <v>1</v>
+      </c>
+      <c r="L1449" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1449" s="18">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="N1449" s="18">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="O1449" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1449" s="7" t="s">
         <v>74</v>
@@ -75103,11 +77381,33 @@
       <c r="F1450" t="s">
         <v>118</v>
       </c>
+      <c r="G1450" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1450" s="16">
+        <v>18.184000000000001</v>
+      </c>
+      <c r="I1450" s="16">
+        <v>19.204999999999998</v>
+      </c>
       <c r="J1450">
         <v>1</v>
       </c>
       <c r="K1450" s="1">
         <v>1</v>
+      </c>
+      <c r="L1450" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1450" s="18">
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="N1450" s="18">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="O1450" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1450" s="7" t="s">
         <v>75</v>
@@ -75132,11 +77432,33 @@
       <c r="F1451" t="s">
         <v>96</v>
       </c>
+      <c r="G1451" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1451" s="16">
+        <v>17.718</v>
+      </c>
+      <c r="I1451" s="16">
+        <v>19.056999999999999</v>
+      </c>
       <c r="J1451">
         <v>2</v>
       </c>
       <c r="K1451" s="1">
         <v>1</v>
+      </c>
+      <c r="L1451" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1451" s="18">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="N1451" s="18">
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="O1451" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1451" s="7" t="s">
         <v>76</v>
@@ -75161,11 +77483,33 @@
       <c r="F1452" t="s">
         <v>136</v>
       </c>
+      <c r="G1452" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1452" s="16">
+        <v>18.035</v>
+      </c>
+      <c r="I1452" s="16">
+        <v>19.298999999999999</v>
+      </c>
       <c r="J1452">
         <v>2</v>
       </c>
       <c r="K1452" s="1">
         <v>1</v>
+      </c>
+      <c r="L1452" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1452" s="18">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="N1452" s="18">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="O1452" s="2">
+        <f t="shared" si="25"/>
+        <v>90.000000000000057</v>
       </c>
       <c r="Q1452" s="7" t="s">
         <v>77</v>
@@ -75190,11 +77534,33 @@
       <c r="F1453" t="s">
         <v>132</v>
       </c>
+      <c r="G1453" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1453" s="16">
+        <v>18.228000000000002</v>
+      </c>
+      <c r="I1453" s="16">
+        <v>19.190000000000001</v>
+      </c>
       <c r="J1453">
         <v>2</v>
       </c>
       <c r="K1453" s="1">
         <v>1</v>
+      </c>
+      <c r="L1453" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1453" s="18">
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="N1453" s="18">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="O1453" s="2">
+        <f t="shared" si="25"/>
+        <v>90.999999999999943</v>
       </c>
       <c r="Q1453" s="7" t="s">
         <v>78</v>
@@ -75219,11 +77585,33 @@
       <c r="F1454" t="s">
         <v>104</v>
       </c>
+      <c r="G1454" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1454" s="16">
+        <v>18.391999999999999</v>
+      </c>
+      <c r="I1454" s="16">
+        <v>19.510999999999999</v>
+      </c>
       <c r="J1454">
         <v>2</v>
       </c>
       <c r="K1454" s="1">
         <v>1</v>
+      </c>
+      <c r="L1454" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1454" s="18">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="N1454" s="18">
+        <v>0.4152777777777778</v>
+      </c>
+      <c r="O1454" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999943</v>
       </c>
       <c r="Q1454" s="7" t="s">
         <v>79</v>
@@ -75248,11 +77636,33 @@
       <c r="F1455" t="s">
         <v>124</v>
       </c>
+      <c r="G1455" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1455" s="16">
+        <v>18.094999999999999</v>
+      </c>
+      <c r="I1455" s="16">
+        <v>19.338000000000001</v>
+      </c>
       <c r="J1455">
         <v>2</v>
       </c>
       <c r="K1455" s="1">
         <v>1</v>
+      </c>
+      <c r="L1455" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1455" s="18">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="N1455" s="18">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="O1455" s="2">
+        <f t="shared" si="25"/>
+        <v>91.000000000000057</v>
       </c>
       <c r="Q1455" s="7" t="s">
         <v>80</v>
@@ -75277,11 +77687,33 @@
       <c r="F1456" t="s">
         <v>130</v>
       </c>
+      <c r="G1456" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1456" s="16">
+        <v>18.207000000000001</v>
+      </c>
+      <c r="I1456" s="16">
+        <v>19.334</v>
+      </c>
       <c r="J1456">
         <v>2</v>
       </c>
       <c r="K1456" s="1">
         <v>1</v>
+      </c>
+      <c r="L1456" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1456" s="18">
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="N1456" s="18">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="O1456" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1456" s="7" t="s">
         <v>81</v>
@@ -75306,11 +77738,33 @@
       <c r="F1457" t="s">
         <v>128</v>
       </c>
+      <c r="G1457" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1457" s="16">
+        <v>18.068999999999999</v>
+      </c>
+      <c r="I1457" s="16">
+        <v>19.390999999999998</v>
+      </c>
       <c r="J1457">
         <v>2</v>
       </c>
       <c r="K1457" s="1">
         <v>1</v>
+      </c>
+      <c r="L1457" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1457" s="18">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="N1457" s="18">
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="O1457" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1457" s="7" t="s">
         <v>86</v>
@@ -75335,11 +77789,33 @@
       <c r="F1458" t="s">
         <v>120</v>
       </c>
+      <c r="G1458" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1458" s="16">
+        <v>18.103999999999999</v>
+      </c>
+      <c r="I1458" s="16">
+        <v>19.166</v>
+      </c>
       <c r="J1458">
         <v>2</v>
       </c>
       <c r="K1458" s="1">
         <v>1</v>
+      </c>
+      <c r="L1458" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1458" s="18">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="N1458" s="18">
+        <v>0.41944444444444445</v>
+      </c>
+      <c r="O1458" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1458" s="7" t="s">
         <v>85</v>
@@ -75364,11 +77840,33 @@
       <c r="F1459" t="s">
         <v>134</v>
       </c>
+      <c r="G1459" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1459" s="16">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="I1459" s="16">
+        <v>19.315000000000001</v>
+      </c>
       <c r="J1459">
         <v>2</v>
       </c>
       <c r="K1459" s="1">
         <v>1</v>
+      </c>
+      <c r="L1459" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1459" s="18">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="N1459" s="18">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="O1459" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1459" s="7" t="s">
         <v>82</v>
@@ -75393,11 +77891,33 @@
       <c r="F1460" t="s">
         <v>110</v>
       </c>
+      <c r="G1460" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1460" s="16">
+        <v>18.132999999999999</v>
+      </c>
+      <c r="I1460" s="16">
+        <v>19.222000000000001</v>
+      </c>
       <c r="J1460">
         <v>2</v>
       </c>
       <c r="K1460" s="1">
         <v>1</v>
+      </c>
+      <c r="L1460" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1460" s="18">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="N1460" s="18">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="O1460" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1460" s="7" t="s">
         <v>83</v>
@@ -75422,11 +77942,33 @@
       <c r="F1461" t="s">
         <v>114</v>
       </c>
+      <c r="G1461" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1461" s="16">
+        <v>18.212</v>
+      </c>
+      <c r="I1461" s="16">
+        <v>19.521999999999998</v>
+      </c>
       <c r="J1461">
         <v>2</v>
       </c>
       <c r="K1461" s="1">
         <v>1</v>
+      </c>
+      <c r="L1461" s="1">
+        <v>24</v>
+      </c>
+      <c r="M1461" s="18">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="N1461" s="18">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="O1461" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1461" s="7" t="s">
         <v>84</v>
@@ -75451,11 +77993,33 @@
       <c r="F1462" t="s">
         <v>122</v>
       </c>
+      <c r="G1462" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1462" s="16">
+        <v>18.587</v>
+      </c>
+      <c r="I1462" s="16">
+        <v>19.638000000000002</v>
+      </c>
       <c r="J1462">
         <v>1</v>
       </c>
       <c r="K1462" s="1">
         <v>2</v>
+      </c>
+      <c r="L1462" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1462" s="18">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="N1462" s="18">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="O1462" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1462" s="7" t="s">
         <v>66</v>
@@ -75480,11 +78044,33 @@
       <c r="F1463" t="s">
         <v>108</v>
       </c>
+      <c r="G1463" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1463" s="16">
+        <v>17.878</v>
+      </c>
+      <c r="I1463" s="16">
+        <v>19.052</v>
+      </c>
       <c r="J1463">
         <v>1</v>
       </c>
       <c r="K1463" s="1">
         <v>2</v>
+      </c>
+      <c r="L1463" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1463" s="18">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="N1463" s="18">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="O1463" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1463" s="7" t="s">
         <v>67</v>
@@ -75509,11 +78095,33 @@
       <c r="F1464" t="s">
         <v>100</v>
       </c>
+      <c r="G1464" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1464" s="16">
+        <v>17.739000000000001</v>
+      </c>
+      <c r="I1464" s="16">
+        <v>18.838000000000001</v>
+      </c>
       <c r="J1464">
         <v>1</v>
       </c>
       <c r="K1464" s="1">
         <v>2</v>
+      </c>
+      <c r="L1464" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1464" s="18">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="N1464" s="18">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="O1464" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1464" s="7" t="s">
         <v>68</v>
@@ -75538,11 +78146,33 @@
       <c r="F1465" t="s">
         <v>112</v>
       </c>
+      <c r="G1465" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1465" s="16">
+        <v>17.943000000000001</v>
+      </c>
+      <c r="I1465" s="16">
+        <v>19.164000000000001</v>
+      </c>
       <c r="J1465">
         <v>1</v>
       </c>
       <c r="K1465" s="1">
         <v>2</v>
+      </c>
+      <c r="L1465" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1465" s="18">
+        <v>0.4291666666666667</v>
+      </c>
+      <c r="N1465" s="18">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="O1465" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1465" s="7" t="s">
         <v>69</v>
@@ -75567,11 +78197,33 @@
       <c r="F1466" t="s">
         <v>126</v>
       </c>
+      <c r="G1466" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1466" s="16">
+        <v>18.187999999999999</v>
+      </c>
+      <c r="I1466" s="16">
+        <v>19.544</v>
+      </c>
       <c r="J1466">
         <v>1</v>
       </c>
       <c r="K1466" s="1">
         <v>2</v>
+      </c>
+      <c r="L1466" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1466" s="18">
+        <v>0.42986111111111108</v>
+      </c>
+      <c r="N1466" s="18">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="O1466" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1466" s="7" t="s">
         <v>70</v>
@@ -75596,11 +78248,33 @@
       <c r="F1467" t="s">
         <v>116</v>
       </c>
+      <c r="G1467" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1467" s="16">
+        <v>18.399000000000001</v>
+      </c>
+      <c r="I1467" s="16">
+        <v>19.741</v>
+      </c>
       <c r="J1467">
         <v>1</v>
       </c>
       <c r="K1467" s="1">
         <v>2</v>
+      </c>
+      <c r="L1467" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1467" s="18">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="N1467" s="18">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="O1467" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1467" s="7" t="s">
         <v>71</v>
@@ -75625,11 +78299,33 @@
       <c r="F1468" t="s">
         <v>98</v>
       </c>
+      <c r="G1468" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1468" s="16">
+        <v>18.009</v>
+      </c>
+      <c r="I1468" s="16">
+        <v>19.329999999999998</v>
+      </c>
       <c r="J1468">
         <v>1</v>
       </c>
       <c r="K1468" s="1">
         <v>2</v>
+      </c>
+      <c r="L1468" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1468" s="18">
+        <v>0.43194444444444446</v>
+      </c>
+      <c r="N1468" s="18">
+        <v>0.49513888888888885</v>
+      </c>
+      <c r="O1468" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1468" s="7" t="s">
         <v>72</v>
@@ -75654,11 +78350,33 @@
       <c r="F1469" t="s">
         <v>106</v>
       </c>
+      <c r="G1469" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1469" s="16">
+        <v>18.132000000000001</v>
+      </c>
+      <c r="I1469" s="16">
+        <v>19.202000000000002</v>
+      </c>
       <c r="J1469">
         <v>1</v>
       </c>
       <c r="K1469" s="1">
         <v>2</v>
+      </c>
+      <c r="L1469" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1469" s="18">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="N1469" s="18">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="O1469" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1469" s="7" t="s">
         <v>73</v>
@@ -75683,11 +78401,33 @@
       <c r="F1470" t="s">
         <v>102</v>
       </c>
+      <c r="G1470" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1470" s="16">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="I1470" s="16">
+        <v>19.684000000000001</v>
+      </c>
       <c r="J1470">
         <v>1</v>
       </c>
       <c r="K1470" s="1">
         <v>2</v>
+      </c>
+      <c r="L1470" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1470" s="18">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="N1470" s="18">
+        <v>0.49722222222222223</v>
+      </c>
+      <c r="O1470" s="2">
+        <f t="shared" si="25"/>
+        <v>91.000000000000114</v>
       </c>
       <c r="Q1470" s="7" t="s">
         <v>74</v>
@@ -75712,11 +78452,33 @@
       <c r="F1471" t="s">
         <v>118</v>
       </c>
+      <c r="G1471" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1471" s="16">
+        <v>18.184000000000001</v>
+      </c>
+      <c r="I1471" s="16">
+        <v>19.204999999999998</v>
+      </c>
       <c r="J1471">
         <v>1</v>
       </c>
       <c r="K1471" s="1">
         <v>2</v>
+      </c>
+      <c r="L1471" s="1">
+        <v>26</v>
+      </c>
+      <c r="M1471" s="18">
+        <v>0.43472222222222223</v>
+      </c>
+      <c r="N1471" s="18">
+        <v>0.49791666666666662</v>
+      </c>
+      <c r="O1471" s="2">
+        <f t="shared" si="25"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1471" s="7" t="s">
         <v>75</v>
@@ -75741,11 +78503,33 @@
       <c r="F1472" t="s">
         <v>96</v>
       </c>
+      <c r="G1472" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="H1472" s="16">
+        <v>17.718</v>
+      </c>
+      <c r="I1472" s="16">
+        <v>19.056999999999999</v>
+      </c>
       <c r="J1472">
         <v>2</v>
       </c>
       <c r="K1472" s="1">
         <v>2</v>
+      </c>
+      <c r="L1472" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1472" s="18">
+        <v>0.4694444444444445</v>
+      </c>
+      <c r="N1472" s="18">
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="O1472" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1472" s="7" t="s">
         <v>76</v>
@@ -75770,11 +78554,33 @@
       <c r="F1473" t="s">
         <v>136</v>
       </c>
+      <c r="G1473" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1473" s="16">
+        <v>18.035</v>
+      </c>
+      <c r="I1473" s="16">
+        <v>19.298999999999999</v>
+      </c>
       <c r="J1473">
         <v>2</v>
       </c>
       <c r="K1473" s="1">
         <v>2</v>
+      </c>
+      <c r="L1473" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1473" s="18">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="N1473" s="18">
+        <v>0.53263888888888888</v>
+      </c>
+      <c r="O1473" s="2">
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="Q1473" s="7" t="s">
         <v>77</v>
@@ -75799,11 +78605,33 @@
       <c r="F1474" t="s">
         <v>132</v>
       </c>
+      <c r="G1474" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1474" s="16">
+        <v>18.228000000000002</v>
+      </c>
+      <c r="I1474" s="16">
+        <v>19.190000000000001</v>
+      </c>
       <c r="J1474">
         <v>2</v>
       </c>
       <c r="K1474" s="1">
         <v>2</v>
+      </c>
+      <c r="L1474" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1474" s="18">
+        <v>0.47083333333333338</v>
+      </c>
+      <c r="N1474" s="18">
+        <v>0.53402777777777777</v>
+      </c>
+      <c r="O1474" s="2">
+        <f t="shared" si="25"/>
+        <v>90.999999999999886</v>
       </c>
       <c r="Q1474" s="7" t="s">
         <v>78</v>
@@ -75828,11 +78656,33 @@
       <c r="F1475" t="s">
         <v>104</v>
       </c>
+      <c r="G1475" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1475" s="16">
+        <v>18.391999999999999</v>
+      </c>
+      <c r="I1475" s="16">
+        <v>19.510999999999999</v>
+      </c>
       <c r="J1475">
         <v>2</v>
       </c>
       <c r="K1475" s="1">
         <v>2</v>
+      </c>
+      <c r="L1475" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1475" s="18">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="N1475" s="18">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="O1475" s="2">
+        <f t="shared" si="25"/>
+        <v>89.999999999999886</v>
       </c>
       <c r="Q1475" s="7" t="s">
         <v>79</v>
@@ -75857,11 +78707,33 @@
       <c r="F1476" t="s">
         <v>124</v>
       </c>
+      <c r="G1476" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1476" s="16">
+        <v>18.094999999999999</v>
+      </c>
+      <c r="I1476" s="16">
+        <v>19.338000000000001</v>
+      </c>
       <c r="J1476">
         <v>2</v>
       </c>
       <c r="K1476" s="1">
         <v>2</v>
+      </c>
+      <c r="L1476" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1476" s="18">
+        <v>0.47291666666666665</v>
+      </c>
+      <c r="N1476" s="18">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="O1476" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1476" s="7" t="s">
         <v>80</v>
@@ -75886,11 +78758,33 @@
       <c r="F1477" t="s">
         <v>130</v>
       </c>
+      <c r="G1477" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1477" s="16">
+        <v>18.207000000000001</v>
+      </c>
+      <c r="I1477" s="16">
+        <v>19.334</v>
+      </c>
       <c r="J1477">
         <v>2</v>
       </c>
       <c r="K1477" s="1">
         <v>2</v>
+      </c>
+      <c r="L1477" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1477" s="18">
+        <v>0.47361111111111115</v>
+      </c>
+      <c r="N1477" s="18">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="O1477" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1477" s="7" t="s">
         <v>81</v>
@@ -75915,11 +78809,33 @@
       <c r="F1478" t="s">
         <v>128</v>
       </c>
+      <c r="G1478" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H1478" s="16">
+        <v>18.068999999999999</v>
+      </c>
+      <c r="I1478" s="16">
+        <v>19.390999999999998</v>
+      </c>
       <c r="J1478">
         <v>2</v>
       </c>
       <c r="K1478" s="1">
         <v>2</v>
+      </c>
+      <c r="L1478" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1478" s="18">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="N1478" s="18">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="O1478" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1478" s="7" t="s">
         <v>86</v>
@@ -75944,11 +78860,33 @@
       <c r="F1479" t="s">
         <v>120</v>
       </c>
+      <c r="G1479" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1479" s="16">
+        <v>18.103999999999999</v>
+      </c>
+      <c r="I1479" s="16">
+        <v>19.166</v>
+      </c>
       <c r="J1479">
         <v>2</v>
       </c>
       <c r="K1479" s="1">
         <v>2</v>
+      </c>
+      <c r="L1479" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1479" s="18">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="N1479" s="18">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="O1479" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1479" s="7" t="s">
         <v>85</v>
@@ -75973,11 +78911,33 @@
       <c r="F1480" t="s">
         <v>134</v>
       </c>
+      <c r="G1480" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H1480" s="16">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="I1480" s="16">
+        <v>19.315000000000001</v>
+      </c>
       <c r="J1480">
         <v>2</v>
       </c>
       <c r="K1480" s="1">
         <v>2</v>
+      </c>
+      <c r="L1480" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1480" s="18">
+        <v>0.4770833333333333</v>
+      </c>
+      <c r="N1480" s="18">
+        <v>0.54027777777777775</v>
+      </c>
+      <c r="O1480" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1480" s="7" t="s">
         <v>82</v>
@@ -76002,11 +78962,33 @@
       <c r="F1481" t="s">
         <v>110</v>
       </c>
+      <c r="G1481" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1481" s="16">
+        <v>18.132999999999999</v>
+      </c>
+      <c r="I1481" s="16">
+        <v>19.222000000000001</v>
+      </c>
       <c r="J1481">
         <v>2</v>
       </c>
       <c r="K1481" s="1">
         <v>2</v>
+      </c>
+      <c r="L1481" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1481" s="18">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="N1481" s="18">
+        <v>0.54097222222222219</v>
+      </c>
+      <c r="O1481" s="2">
+        <f t="shared" si="25"/>
+        <v>91</v>
       </c>
       <c r="Q1481" s="7" t="s">
         <v>83</v>
@@ -76031,11 +79013,33 @@
       <c r="F1482" t="s">
         <v>114</v>
       </c>
+      <c r="G1482" s="1">
+        <v>24</v>
+      </c>
+      <c r="H1482" s="16">
+        <v>18.212</v>
+      </c>
+      <c r="I1482" s="16">
+        <v>19.521999999999998</v>
+      </c>
       <c r="J1482">
         <v>2</v>
       </c>
       <c r="K1482" s="1">
         <v>2</v>
+      </c>
+      <c r="L1482" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1482" s="18">
+        <v>0.47847222222222219</v>
+      </c>
+      <c r="N1482" s="18">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="O1482" s="2">
+        <f t="shared" si="25"/>
+        <v>92.000000000000114</v>
       </c>
       <c r="Q1482" s="7" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Integration done for 26.1.17
</commit_message>
<xml_diff>
--- a/data/ldeli_integrate.xlsx
+++ b/data/ldeli_integrate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="3120" yWindow="8160" windowWidth="22420" windowHeight="6580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5484" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5495" uniqueCount="177">
   <si>
     <t>date</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t>BadBLCO2</t>
+  </si>
+  <si>
+    <t>BadCO2BLP</t>
+  </si>
+  <si>
+    <t>LateCO2BLP</t>
   </si>
 </sst>
 </file>
@@ -2311,9 +2317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1465" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1483" sqref="N1483"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1354" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1356" sqref="R1356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -71180,7 +71186,7 @@
         <v>1.41E-3</v>
       </c>
     </row>
-    <row r="1329" spans="1:20" ht="16" customHeight="1">
+    <row r="1329" spans="1:29" ht="16" customHeight="1">
       <c r="A1329" s="3">
         <v>42761</v>
       </c>
@@ -71240,7 +71246,7 @@
         <v>1.9980000000000002E-3</v>
       </c>
     </row>
-    <row r="1330" spans="1:20" ht="16" customHeight="1">
+    <row r="1330" spans="1:29" ht="16" customHeight="1">
       <c r="A1330" s="3">
         <v>42761</v>
       </c>
@@ -71300,7 +71306,7 @@
         <v>1.078E-3</v>
       </c>
     </row>
-    <row r="1331" spans="1:20" ht="16" customHeight="1">
+    <row r="1331" spans="1:29" ht="16" customHeight="1">
       <c r="A1331" s="3">
         <v>42761</v>
       </c>
@@ -71360,7 +71366,7 @@
         <v>1.7329999999999999E-3</v>
       </c>
     </row>
-    <row r="1332" spans="1:20" ht="16" customHeight="1">
+    <row r="1332" spans="1:29" ht="16" customHeight="1">
       <c r="A1332" s="3">
         <v>42761</v>
       </c>
@@ -71420,7 +71426,7 @@
         <v>1.678E-3</v>
       </c>
     </row>
-    <row r="1333" spans="1:20" ht="16" customHeight="1">
+    <row r="1333" spans="1:29" ht="16" customHeight="1">
       <c r="A1333" s="3">
         <v>42761</v>
       </c>
@@ -71480,7 +71486,7 @@
         <v>2.4090000000000001E-3</v>
       </c>
     </row>
-    <row r="1334" spans="1:20" ht="16" customHeight="1">
+    <row r="1334" spans="1:29" ht="16" customHeight="1">
       <c r="A1334" s="3">
         <v>42761</v>
       </c>
@@ -71540,7 +71546,7 @@
         <v>1.805E-3</v>
       </c>
     </row>
-    <row r="1335" spans="1:20" ht="16" customHeight="1">
+    <row r="1335" spans="1:29" ht="16" customHeight="1">
       <c r="A1335" s="3">
         <v>42761</v>
       </c>
@@ -71590,8 +71596,17 @@
       <c r="Q1335" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="1336" spans="1:20" ht="16" customHeight="1">
+      <c r="R1335" s="28">
+        <v>3.4509999999999999E-4</v>
+      </c>
+      <c r="S1335" s="28">
+        <v>3.0040000000000002E-3</v>
+      </c>
+      <c r="T1335" s="28">
+        <v>3.2399999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:29" ht="16" customHeight="1">
       <c r="A1336" s="3">
         <v>42761</v>
       </c>
@@ -71641,8 +71656,17 @@
       <c r="Q1336" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="1337" spans="1:20" ht="16" customHeight="1">
+      <c r="R1336" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1336" s="28">
+        <v>5.3749999999999996E-3</v>
+      </c>
+      <c r="T1336" s="28">
+        <v>3.8930000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:29" ht="16" customHeight="1">
       <c r="A1337" s="3">
         <v>42761</v>
       </c>
@@ -71692,8 +71716,17 @@
       <c r="Q1337" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="1338" spans="1:20" ht="16" customHeight="1">
+      <c r="R1337" s="28">
+        <v>5.5460000000000004E-4</v>
+      </c>
+      <c r="S1337" s="28">
+        <v>3.98E-3</v>
+      </c>
+      <c r="T1337" s="28">
+        <v>3.7060000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:29" ht="16" customHeight="1">
       <c r="A1338" s="3">
         <v>42761</v>
       </c>
@@ -71743,8 +71776,17 @@
       <c r="Q1338" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="1339" spans="1:20" ht="16" customHeight="1">
+      <c r="R1338" s="28">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="S1338" s="28">
+        <v>3.9039999999999999E-3</v>
+      </c>
+      <c r="T1338" s="28">
+        <v>3.5560000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:29" ht="16" customHeight="1">
       <c r="A1339" s="3">
         <v>42761</v>
       </c>
@@ -71794,8 +71836,17 @@
       <c r="Q1339" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="1340" spans="1:20" ht="16" customHeight="1">
+      <c r="R1339" s="28">
+        <v>1.2459999999999999E-3</v>
+      </c>
+      <c r="S1339" s="1">
+        <v>1.03807E-2</v>
+      </c>
+      <c r="T1339" s="28">
+        <v>6.4660000000000004E-3</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:29" ht="16" customHeight="1">
       <c r="A1340" s="3">
         <v>42761</v>
       </c>
@@ -71845,8 +71896,17 @@
       <c r="Q1340" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="1341" spans="1:20" ht="16" customHeight="1">
+      <c r="R1340" s="28">
+        <v>3.5300000000000002E-4</v>
+      </c>
+      <c r="S1340" s="28">
+        <v>4.5729999999999998E-3</v>
+      </c>
+      <c r="T1340" s="28">
+        <v>3.859E-3</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:29" ht="16" customHeight="1">
       <c r="A1341" s="3">
         <v>42761</v>
       </c>
@@ -71896,8 +71956,17 @@
       <c r="Q1341" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="1342" spans="1:20" ht="16" customHeight="1">
+      <c r="R1341" s="28">
+        <v>2.106E-4</v>
+      </c>
+      <c r="S1341" s="28">
+        <v>3.9509999999999997E-3</v>
+      </c>
+      <c r="T1341" s="28">
+        <v>3.8790000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:29" ht="16" customHeight="1">
       <c r="A1342" s="3">
         <v>42761</v>
       </c>
@@ -71947,8 +72016,17 @@
       <c r="Q1342" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="1343" spans="1:20" ht="16" customHeight="1">
+      <c r="R1342" s="28">
+        <v>2.3039999999999999E-4</v>
+      </c>
+      <c r="S1342" s="28">
+        <v>5.3140000000000001E-3</v>
+      </c>
+      <c r="T1342" s="28">
+        <v>5.8979999999999996E-3</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:29" ht="16" customHeight="1">
       <c r="A1343" s="3">
         <v>42761</v>
       </c>
@@ -71998,8 +72076,20 @@
       <c r="Q1343" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="1344" spans="1:20" ht="16" customHeight="1">
+      <c r="R1343" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1343" s="28">
+        <v>5.4310000000000001E-3</v>
+      </c>
+      <c r="T1343" s="28">
+        <v>5.0410000000000003E-3</v>
+      </c>
+      <c r="AC1343" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:29" ht="16" customHeight="1">
       <c r="A1344" s="3">
         <v>42761</v>
       </c>
@@ -72049,8 +72139,17 @@
       <c r="Q1344" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1345" spans="1:17" ht="16" customHeight="1">
+      <c r="R1344" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1344" s="28">
+        <v>7.2589999999999998E-3</v>
+      </c>
+      <c r="T1344" s="28">
+        <v>7.5119999999999996E-3</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:29" ht="16" customHeight="1">
       <c r="A1345" s="3">
         <v>42761</v>
       </c>
@@ -72100,8 +72199,17 @@
       <c r="Q1345" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="1346" spans="1:17" ht="16" customHeight="1">
+      <c r="R1345" s="28">
+        <v>2.7129999999999998E-4</v>
+      </c>
+      <c r="S1345" s="28">
+        <v>2.5100000000000001E-3</v>
+      </c>
+      <c r="T1345" s="28">
+        <v>2.7920000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:29" ht="16" customHeight="1">
       <c r="A1346" s="3">
         <v>42761</v>
       </c>
@@ -72151,8 +72259,17 @@
       <c r="Q1346" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="1347" spans="1:17" ht="16" customHeight="1">
+      <c r="R1346" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1346" s="28">
+        <v>3.2989999999999998E-3</v>
+      </c>
+      <c r="T1346" s="28">
+        <v>2.5869999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:29" ht="16" customHeight="1">
       <c r="A1347" s="3">
         <v>42761</v>
       </c>
@@ -72202,8 +72319,17 @@
       <c r="Q1347" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="1348" spans="1:17" ht="16" customHeight="1">
+      <c r="R1347" s="28">
+        <v>4.8349999999999999E-4</v>
+      </c>
+      <c r="S1347" s="28">
+        <v>1.2819999999999999E-3</v>
+      </c>
+      <c r="T1347" s="28">
+        <v>3.6900000000000002E-4</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:29" ht="16" customHeight="1">
       <c r="A1348" s="3">
         <v>42761</v>
       </c>
@@ -72253,8 +72379,20 @@
       <c r="Q1348" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="1349" spans="1:17" ht="16" customHeight="1">
+      <c r="R1348" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1348" s="28">
+        <v>2.3080000000000002E-3</v>
+      </c>
+      <c r="T1348" s="28">
+        <v>1.97E-3</v>
+      </c>
+      <c r="AC1348" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:29" ht="16" customHeight="1">
       <c r="A1349" s="3">
         <v>42761</v>
       </c>
@@ -72304,8 +72442,17 @@
       <c r="Q1349" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1350" spans="1:17" ht="16" customHeight="1">
+      <c r="R1349" s="28">
+        <v>8.8020000000000004E-4</v>
+      </c>
+      <c r="S1349" s="28">
+        <v>4.6340000000000001E-3</v>
+      </c>
+      <c r="T1349" s="28">
+        <v>5.6839999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:29" ht="16" customHeight="1">
       <c r="A1350" s="3">
         <v>42761</v>
       </c>
@@ -72355,8 +72502,17 @@
       <c r="Q1350" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="1351" spans="1:17" ht="16" customHeight="1">
+      <c r="R1350" s="28">
+        <v>5.0370000000000005E-4</v>
+      </c>
+      <c r="S1350" s="28">
+        <v>2.6210000000000001E-3</v>
+      </c>
+      <c r="T1350" s="28">
+        <v>3.1410000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:29" ht="16" customHeight="1">
       <c r="A1351" s="3">
         <v>42761</v>
       </c>
@@ -72406,8 +72562,17 @@
       <c r="Q1351" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="1352" spans="1:17" ht="16" customHeight="1">
+      <c r="R1351" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1351" s="28">
+        <v>2.0040000000000001E-3</v>
+      </c>
+      <c r="T1351" s="28">
+        <v>7.7130000000000005E-4</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:29" ht="16" customHeight="1">
       <c r="A1352" s="3">
         <v>42761</v>
       </c>
@@ -72457,8 +72622,17 @@
       <c r="Q1352" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="1353" spans="1:17" ht="16" customHeight="1">
+      <c r="R1352" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1352" s="28">
+        <v>2.702E-3</v>
+      </c>
+      <c r="T1352" s="28">
+        <v>2.4849999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:29" ht="16" customHeight="1">
       <c r="A1353" s="3">
         <v>42761</v>
       </c>
@@ -72508,8 +72682,17 @@
       <c r="Q1353" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="1354" spans="1:17" ht="16" customHeight="1">
+      <c r="R1353" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1353" s="28">
+        <v>2.5560000000000001E-3</v>
+      </c>
+      <c r="T1353" s="28">
+        <v>3.222E-3</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:29" ht="16" customHeight="1">
       <c r="A1354" s="3">
         <v>42761</v>
       </c>
@@ -72559,8 +72742,17 @@
       <c r="Q1354" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="1355" spans="1:17" ht="16" customHeight="1">
+      <c r="R1354" s="28">
+        <v>3.2939999999999998E-4</v>
+      </c>
+      <c r="S1354" s="28">
+        <v>2.166E-3</v>
+      </c>
+      <c r="T1354" s="28">
+        <v>2.7490000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:29" ht="16" customHeight="1">
       <c r="A1355" s="3">
         <v>42761</v>
       </c>
@@ -72610,8 +72802,17 @@
       <c r="Q1355" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="1356" spans="1:17" ht="16" customHeight="1">
+      <c r="R1355" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1355" s="28">
+        <v>2.2039999999999998E-3</v>
+      </c>
+      <c r="T1355" s="28">
+        <v>3.7230000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:29" ht="16" customHeight="1">
       <c r="A1356" s="3">
         <v>42762</v>
       </c>
@@ -72662,7 +72863,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1357" spans="1:17" ht="16" customHeight="1">
+    <row r="1357" spans="1:29" ht="16" customHeight="1">
       <c r="A1357" s="3">
         <v>42762</v>
       </c>
@@ -72713,7 +72914,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1358" spans="1:17" ht="16" customHeight="1">
+    <row r="1358" spans="1:29" ht="16" customHeight="1">
       <c r="A1358" s="3">
         <v>42762</v>
       </c>
@@ -72764,7 +72965,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="1359" spans="1:17" ht="16" customHeight="1">
+    <row r="1359" spans="1:29" ht="16" customHeight="1">
       <c r="A1359" s="3">
         <v>42762</v>
       </c>
@@ -72815,7 +73016,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="1360" spans="1:17" ht="16" customHeight="1">
+    <row r="1360" spans="1:29" ht="16" customHeight="1">
       <c r="A1360" s="3">
         <v>42762</v>
       </c>

</xml_diff>

<commit_message>
T1 27/1/17 integrate done
</commit_message>
<xml_diff>
--- a/data/ldeli_integrate.xlsx
+++ b/data/ldeli_integrate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="8160" windowWidth="22420" windowHeight="6580" tabRatio="500"/>
+    <workbookView xWindow="3020" yWindow="7840" windowWidth="22420" windowHeight="6580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5495" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5503" uniqueCount="180">
   <si>
     <t>date</t>
   </si>
@@ -551,6 +551,15 @@
   </si>
   <si>
     <t>LateCO2BLP</t>
+  </si>
+  <si>
+    <t>BadCO2S1</t>
+  </si>
+  <si>
+    <t>DoublePCO2BL</t>
+  </si>
+  <si>
+    <t>NegCO2S1</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1284,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1358,6 +1367,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="626">
@@ -2318,8 +2330,8 @@
   <dimension ref="A1:AG1779"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1354" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1356" sqref="R1356"/>
+      <pane ySplit="1" topLeftCell="A1376" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1377" sqref="R1377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -72862,6 +72874,18 @@
       <c r="Q1356" s="7" t="s">
         <v>66</v>
       </c>
+      <c r="R1356" s="29">
+        <v>3.703E-4</v>
+      </c>
+      <c r="S1356" s="28">
+        <v>4.0400000000000001E-4</v>
+      </c>
+      <c r="T1356" s="28">
+        <v>2.581E-3</v>
+      </c>
+      <c r="AC1356" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="1357" spans="1:29" ht="16" customHeight="1">
       <c r="A1357" s="3">
@@ -72913,6 +72937,15 @@
       <c r="Q1357" s="7" t="s">
         <v>67</v>
       </c>
+      <c r="R1357" s="28">
+        <v>3.1869999999999999E-4</v>
+      </c>
+      <c r="S1357" s="28">
+        <v>9.4019999999999998E-4</v>
+      </c>
+      <c r="T1357" s="28">
+        <v>2.8999999999999998E-3</v>
+      </c>
     </row>
     <row r="1358" spans="1:29" ht="16" customHeight="1">
       <c r="A1358" s="3">
@@ -72964,6 +72997,15 @@
       <c r="Q1358" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="R1358" s="28">
+        <v>3.3119999999999997E-4</v>
+      </c>
+      <c r="S1358" s="28">
+        <v>2.4689999999999998E-3</v>
+      </c>
+      <c r="T1358" s="28">
+        <v>2.7299999999999998E-3</v>
+      </c>
     </row>
     <row r="1359" spans="1:29" ht="16" customHeight="1">
       <c r="A1359" s="3">
@@ -73015,6 +73057,15 @@
       <c r="Q1359" s="7" t="s">
         <v>69</v>
       </c>
+      <c r="R1359" s="28">
+        <v>5.2550000000000003E-4</v>
+      </c>
+      <c r="S1359" s="28">
+        <v>2.7880000000000001E-3</v>
+      </c>
+      <c r="T1359" s="28">
+        <v>2.8170000000000001E-3</v>
+      </c>
     </row>
     <row r="1360" spans="1:29" ht="16" customHeight="1">
       <c r="A1360" s="3">
@@ -73066,8 +73117,20 @@
       <c r="Q1360" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="1361" spans="1:17" ht="16" customHeight="1">
+      <c r="R1360" s="28">
+        <v>7.2320000000000001E-4</v>
+      </c>
+      <c r="S1360" s="28">
+        <v>3.0590000000000001E-3</v>
+      </c>
+      <c r="T1360" s="28">
+        <v>3.1710000000000002E-3</v>
+      </c>
+      <c r="AC1360" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:29" ht="16" customHeight="1">
       <c r="A1361" s="3">
         <v>42762</v>
       </c>
@@ -73117,8 +73180,17 @@
       <c r="Q1361" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="1362" spans="1:17" ht="16" customHeight="1">
+      <c r="R1361" s="28">
+        <v>7.5219999999999996E-4</v>
+      </c>
+      <c r="S1361" s="28">
+        <v>2.6280000000000001E-3</v>
+      </c>
+      <c r="T1361" s="28">
+        <v>2.66E-3</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:29" ht="16" customHeight="1">
       <c r="A1362" s="3">
         <v>42762</v>
       </c>
@@ -73168,8 +73240,17 @@
       <c r="Q1362" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="1363" spans="1:17" ht="16" customHeight="1">
+      <c r="R1362" s="28">
+        <v>4.4559999999999999E-4</v>
+      </c>
+      <c r="S1362" s="28">
+        <v>3.1189999999999998E-3</v>
+      </c>
+      <c r="T1362" s="28">
+        <v>3.4459999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:29" ht="16" customHeight="1">
       <c r="A1363" s="3">
         <v>42762</v>
       </c>
@@ -73219,8 +73300,17 @@
       <c r="Q1363" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="1364" spans="1:17" ht="16" customHeight="1">
+      <c r="R1363" s="28">
+        <v>7.9719999999999997E-4</v>
+      </c>
+      <c r="S1363" s="28">
+        <v>3.447E-3</v>
+      </c>
+      <c r="T1363" s="28">
+        <v>3.908E-3</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:29" ht="16" customHeight="1">
       <c r="A1364" s="3">
         <v>42762</v>
       </c>
@@ -73270,8 +73360,17 @@
       <c r="Q1364" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="1365" spans="1:17" ht="16" customHeight="1">
+      <c r="R1364" s="28">
+        <v>1.121E-4</v>
+      </c>
+      <c r="S1364" s="28">
+        <v>3.6020000000000002E-3</v>
+      </c>
+      <c r="T1364" s="28">
+        <v>3.248E-3</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:29" ht="16" customHeight="1">
       <c r="A1365" s="3">
         <v>42762</v>
       </c>
@@ -73321,8 +73420,17 @@
       <c r="Q1365" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1366" spans="1:17" ht="16" customHeight="1">
+      <c r="R1365" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1365" s="28">
+        <v>2.5119999999999999E-3</v>
+      </c>
+      <c r="T1365" s="28">
+        <v>3.0699999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:29" ht="16" customHeight="1">
       <c r="A1366" s="3">
         <v>42762</v>
       </c>
@@ -73372,8 +73480,17 @@
       <c r="Q1366" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="1367" spans="1:17" ht="16" customHeight="1">
+      <c r="R1366" s="28">
+        <v>7.8229999999999999E-4</v>
+      </c>
+      <c r="S1366" s="28">
+        <v>3.9610000000000001E-3</v>
+      </c>
+      <c r="T1366" s="28">
+        <v>4.5599999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:29" ht="16" customHeight="1">
       <c r="A1367" s="3">
         <v>42762</v>
       </c>
@@ -73423,8 +73540,17 @@
       <c r="Q1367" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="1368" spans="1:17" ht="16" customHeight="1">
+      <c r="R1367" s="28">
+        <v>3.7080000000000001E-4</v>
+      </c>
+      <c r="S1367" s="28">
+        <v>2.9740000000000001E-3</v>
+      </c>
+      <c r="T1367" s="28">
+        <v>3.3639999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:29" ht="16" customHeight="1">
       <c r="A1368" s="3">
         <v>42762</v>
       </c>
@@ -73474,8 +73600,17 @@
       <c r="Q1368" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="1369" spans="1:17" ht="16" customHeight="1">
+      <c r="R1368" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1368" s="28">
+        <v>2.4239999999999999E-3</v>
+      </c>
+      <c r="T1368" s="28">
+        <v>2.6310000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:29" ht="16" customHeight="1">
       <c r="A1369" s="3">
         <v>42762</v>
       </c>
@@ -73525,8 +73660,17 @@
       <c r="Q1369" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="1370" spans="1:17" ht="16" customHeight="1">
+      <c r="R1369" s="28">
+        <v>9.8639999999999991E-4</v>
+      </c>
+      <c r="S1369" s="28">
+        <v>2.8670000000000002E-3</v>
+      </c>
+      <c r="T1369" s="28">
+        <v>2.5709999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:29" ht="16" customHeight="1">
       <c r="A1370" s="3">
         <v>42762</v>
       </c>
@@ -73576,8 +73720,17 @@
       <c r="Q1370" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1371" spans="1:17" ht="16" customHeight="1">
+      <c r="R1370" s="28">
+        <v>1.2440000000000001E-3</v>
+      </c>
+      <c r="S1370" s="28">
+        <v>6.9629999999999996E-3</v>
+      </c>
+      <c r="T1370" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:29" ht="16" customHeight="1">
       <c r="A1371" s="3">
         <v>42762</v>
       </c>
@@ -73627,8 +73780,20 @@
       <c r="Q1371" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="1372" spans="1:17" ht="16" customHeight="1">
+      <c r="R1371" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1371" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1371" s="28">
+        <v>3.0270000000000002E-3</v>
+      </c>
+      <c r="AC1371" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:29" ht="16" customHeight="1">
       <c r="A1372" s="3">
         <v>42762</v>
       </c>
@@ -73678,8 +73843,17 @@
       <c r="Q1372" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="1373" spans="1:17" ht="16" customHeight="1">
+      <c r="R1372" s="28">
+        <v>5.1380000000000002E-4</v>
+      </c>
+      <c r="S1372" s="28">
+        <v>3.359E-3</v>
+      </c>
+      <c r="T1372" s="28">
+        <v>3.0379999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:29" ht="16" customHeight="1">
       <c r="A1373" s="3">
         <v>42762</v>
       </c>
@@ -73729,8 +73903,17 @@
       <c r="Q1373" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="1374" spans="1:17" ht="16" customHeight="1">
+      <c r="R1373" s="28">
+        <v>6.6580000000000003E-4</v>
+      </c>
+      <c r="S1373" s="28">
+        <v>3.444E-3</v>
+      </c>
+      <c r="T1373" s="28">
+        <v>1.245E-3</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:29" ht="16" customHeight="1">
       <c r="A1374" s="3">
         <v>42762</v>
       </c>
@@ -73780,8 +73963,17 @@
       <c r="Q1374" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="1375" spans="1:17" ht="16" customHeight="1">
+      <c r="R1374" s="28">
+        <v>1.5579999999999999E-4</v>
+      </c>
+      <c r="S1374" s="28">
+        <v>3.8960000000000002E-3</v>
+      </c>
+      <c r="T1374" s="28">
+        <v>3.0560000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:29" ht="16" customHeight="1">
       <c r="A1375" s="3">
         <v>42762</v>
       </c>
@@ -73831,8 +74023,17 @@
       <c r="Q1375" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="1376" spans="1:17" ht="16" customHeight="1">
+      <c r="R1375" s="28">
+        <v>4.2509999999999998E-4</v>
+      </c>
+      <c r="S1375" s="28">
+        <v>3.4970000000000001E-3</v>
+      </c>
+      <c r="T1375" s="28">
+        <v>3.5899999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:29" ht="16" customHeight="1">
       <c r="A1376" s="3">
         <v>42762</v>
       </c>
@@ -73881,6 +74082,15 @@
       </c>
       <c r="Q1376" s="7" t="s">
         <v>84</v>
+      </c>
+      <c r="R1376" s="28">
+        <v>1.712E-3</v>
+      </c>
+      <c r="S1376" s="28">
+        <v>3.6289999999999998E-3</v>
+      </c>
+      <c r="T1376" s="28">
+        <v>3.3630000000000001E-3</v>
       </c>
     </row>
     <row r="1377" spans="1:17" ht="16" customHeight="1">

</xml_diff>